<commit_message>
added dante connections as cables
</commit_message>
<xml_diff>
--- a/data/uac_cables.xlsx
+++ b/data/uac_cables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/donert/Documents/UACTech/SystemDocumentation/github/uactechdoc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DAF9AE2-987C-DE41-BF12-8221B0F08B87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1742A5C-55AB-F049-A3EE-1C23D065ED44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6060" yWindow="760" windowWidth="24180" windowHeight="18880" activeTab="1" xr2:uid="{288904EE-D384-EA4C-9B98-052B972FB267}"/>
+    <workbookView xWindow="-76040" yWindow="-31540" windowWidth="43180" windowHeight="40800" activeTab="1" xr2:uid="{288904EE-D384-EA4C-9B98-052B972FB267}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1614" uniqueCount="638">
   <si>
     <t>Tag</t>
   </si>
@@ -1351,6 +1351,609 @@
   </si>
   <si>
     <t>Need to update  ndi  ports with names</t>
+  </si>
+  <si>
+    <t>2309-1001</t>
+  </si>
+  <si>
+    <t>ZAMU-A001</t>
+  </si>
+  <si>
+    <t>ZAIU-B001</t>
+  </si>
+  <si>
+    <t>dante</t>
+  </si>
+  <si>
+    <t>ch3</t>
+  </si>
+  <si>
+    <t>ch4</t>
+  </si>
+  <si>
+    <t>ZAMU-B001</t>
+  </si>
+  <si>
+    <t>ZAMU-B002</t>
+  </si>
+  <si>
+    <t>ZAMU-B003</t>
+  </si>
+  <si>
+    <t>ZAIU-B002</t>
+  </si>
+  <si>
+    <t>HH03 - Ch35</t>
+  </si>
+  <si>
+    <t>HH04 - Ch36</t>
+  </si>
+  <si>
+    <t>HH01 - Ch33</t>
+  </si>
+  <si>
+    <t>HH02 - Ch34</t>
+  </si>
+  <si>
+    <t>HH05 - Ch37</t>
+  </si>
+  <si>
+    <t>HH06 - Ch38</t>
+  </si>
+  <si>
+    <t>HH07 - Ch39</t>
+  </si>
+  <si>
+    <t>HH08 - Ch40</t>
+  </si>
+  <si>
+    <t>HH09 - Ch41</t>
+  </si>
+  <si>
+    <t>HH10 - Ch42</t>
+  </si>
+  <si>
+    <t>HH11 - Ch43</t>
+  </si>
+  <si>
+    <t>HH12 - Ch44</t>
+  </si>
+  <si>
+    <t>BP06 - Ch45</t>
+  </si>
+  <si>
+    <t>BP01 - Ch01</t>
+  </si>
+  <si>
+    <t>BP02 - Ch02</t>
+  </si>
+  <si>
+    <t>BP03 - Ch03</t>
+  </si>
+  <si>
+    <t>BP04 - Ch04</t>
+  </si>
+  <si>
+    <t>BP05 - Ch05</t>
+  </si>
+  <si>
+    <t>BP06 - Ch06</t>
+  </si>
+  <si>
+    <t>s2___</t>
+  </si>
+  <si>
+    <t>CDMA-A001</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>_1_</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>_2_</t>
+  </si>
+  <si>
+    <t>_3_</t>
+  </si>
+  <si>
+    <t>_4</t>
+  </si>
+  <si>
+    <t>_5_</t>
+  </si>
+  <si>
+    <t>_6_</t>
+  </si>
+  <si>
+    <t>s2_out01</t>
+  </si>
+  <si>
+    <t>s2_in06</t>
+  </si>
+  <si>
+    <t>s2_in01</t>
+  </si>
+  <si>
+    <t>s2_in02</t>
+  </si>
+  <si>
+    <t>s2_in03</t>
+  </si>
+  <si>
+    <t>s2_in04</t>
+  </si>
+  <si>
+    <t>s2_in05</t>
+  </si>
+  <si>
+    <t>s2_in07</t>
+  </si>
+  <si>
+    <t>s2_in08</t>
+  </si>
+  <si>
+    <t>s2_in09</t>
+  </si>
+  <si>
+    <t>s2_in10</t>
+  </si>
+  <si>
+    <t>s2_in11</t>
+  </si>
+  <si>
+    <t>s2_in12</t>
+  </si>
+  <si>
+    <t>s2_out02</t>
+  </si>
+  <si>
+    <t>s2_out03</t>
+  </si>
+  <si>
+    <t>s2_out04</t>
+  </si>
+  <si>
+    <t>s2_out05</t>
+  </si>
+  <si>
+    <t>s2_out06</t>
+  </si>
+  <si>
+    <t>s2_out07</t>
+  </si>
+  <si>
+    <t>s2_out08</t>
+  </si>
+  <si>
+    <t>s2_out09</t>
+  </si>
+  <si>
+    <t>s2_out10</t>
+  </si>
+  <si>
+    <t>s2_out11</t>
+  </si>
+  <si>
+    <t>s2_out12</t>
+  </si>
+  <si>
+    <t>s2_out13</t>
+  </si>
+  <si>
+    <t>s2_out14</t>
+  </si>
+  <si>
+    <t>s2_out15</t>
+  </si>
+  <si>
+    <t>s2_out16</t>
+  </si>
+  <si>
+    <t>Stream L</t>
+  </si>
+  <si>
+    <t>Stream R</t>
+  </si>
+  <si>
+    <t>Ref Mon L</t>
+  </si>
+  <si>
+    <t>Ref Mon R</t>
+  </si>
+  <si>
+    <t>vmavio</t>
+  </si>
+  <si>
+    <t>rmavio</t>
+  </si>
+  <si>
+    <t>out_01</t>
+  </si>
+  <si>
+    <t>out_02</t>
+  </si>
+  <si>
+    <t>out_03</t>
+  </si>
+  <si>
+    <t>out_04</t>
+  </si>
+  <si>
+    <t>in_01</t>
+  </si>
+  <si>
+    <t>in_02</t>
+  </si>
+  <si>
+    <t>in_03</t>
+  </si>
+  <si>
+    <t>in_04</t>
+  </si>
+  <si>
+    <t>in_05</t>
+  </si>
+  <si>
+    <t>in_06</t>
+  </si>
+  <si>
+    <t>in_07</t>
+  </si>
+  <si>
+    <t>in_08</t>
+  </si>
+  <si>
+    <t>in_09</t>
+  </si>
+  <si>
+    <t>in_10</t>
+  </si>
+  <si>
+    <t>in_11</t>
+  </si>
+  <si>
+    <t>in_12</t>
+  </si>
+  <si>
+    <t>in_13</t>
+  </si>
+  <si>
+    <t>in_14</t>
+  </si>
+  <si>
+    <t>in_15</t>
+  </si>
+  <si>
+    <t>in_16</t>
+  </si>
+  <si>
+    <t>in_17</t>
+  </si>
+  <si>
+    <t>in_18</t>
+  </si>
+  <si>
+    <t>in_19</t>
+  </si>
+  <si>
+    <t>in_20</t>
+  </si>
+  <si>
+    <t>in_21</t>
+  </si>
+  <si>
+    <t>in_22</t>
+  </si>
+  <si>
+    <t>in_23</t>
+  </si>
+  <si>
+    <t>in_24</t>
+  </si>
+  <si>
+    <t>in_25</t>
+  </si>
+  <si>
+    <t>in_26</t>
+  </si>
+  <si>
+    <t>in_27</t>
+  </si>
+  <si>
+    <t>in_28</t>
+  </si>
+  <si>
+    <t>in_29</t>
+  </si>
+  <si>
+    <t>in_30</t>
+  </si>
+  <si>
+    <t>in_31</t>
+  </si>
+  <si>
+    <t>in_32</t>
+  </si>
+  <si>
+    <t>in_33</t>
+  </si>
+  <si>
+    <t>in_34</t>
+  </si>
+  <si>
+    <t>in_35</t>
+  </si>
+  <si>
+    <t>in_36</t>
+  </si>
+  <si>
+    <t>in_37</t>
+  </si>
+  <si>
+    <t>in_38</t>
+  </si>
+  <si>
+    <t>in_39</t>
+  </si>
+  <si>
+    <t>in_40</t>
+  </si>
+  <si>
+    <t>in_41</t>
+  </si>
+  <si>
+    <t>in_42</t>
+  </si>
+  <si>
+    <t>in_43</t>
+  </si>
+  <si>
+    <t>in_44</t>
+  </si>
+  <si>
+    <t>in_45</t>
+  </si>
+  <si>
+    <t>in_46</t>
+  </si>
+  <si>
+    <t>in_47</t>
+  </si>
+  <si>
+    <t>in_48</t>
+  </si>
+  <si>
+    <t>2309-1002</t>
+  </si>
+  <si>
+    <t>2309-1003</t>
+  </si>
+  <si>
+    <t>2309-1004</t>
+  </si>
+  <si>
+    <t>2309-1005</t>
+  </si>
+  <si>
+    <t>2309-1006</t>
+  </si>
+  <si>
+    <t>2309-1007</t>
+  </si>
+  <si>
+    <t>2309-1008</t>
+  </si>
+  <si>
+    <t>2309-1009</t>
+  </si>
+  <si>
+    <t>2309-1010</t>
+  </si>
+  <si>
+    <t>2309-1011</t>
+  </si>
+  <si>
+    <t>2309-1012</t>
+  </si>
+  <si>
+    <t>2309-1013</t>
+  </si>
+  <si>
+    <t>2309-1014</t>
+  </si>
+  <si>
+    <t>2309-1015</t>
+  </si>
+  <si>
+    <t>2309-1016</t>
+  </si>
+  <si>
+    <t>2309-1017</t>
+  </si>
+  <si>
+    <t>2309-1018</t>
+  </si>
+  <si>
+    <t>2309-1019</t>
+  </si>
+  <si>
+    <t>2309-1020</t>
+  </si>
+  <si>
+    <t>2309-1021</t>
+  </si>
+  <si>
+    <t>2309-1022</t>
+  </si>
+  <si>
+    <t>2309-1023</t>
+  </si>
+  <si>
+    <t>2309-1024</t>
+  </si>
+  <si>
+    <t>2309-1025</t>
+  </si>
+  <si>
+    <t>2309-1026</t>
+  </si>
+  <si>
+    <t>2309-1027</t>
+  </si>
+  <si>
+    <t>2309-1028</t>
+  </si>
+  <si>
+    <t>2309-1029</t>
+  </si>
+  <si>
+    <t>2309-1030</t>
+  </si>
+  <si>
+    <t>2309-1031</t>
+  </si>
+  <si>
+    <t>2309-1032</t>
+  </si>
+  <si>
+    <t>2309-1033</t>
+  </si>
+  <si>
+    <t>2309-1034</t>
+  </si>
+  <si>
+    <t>2309-1035</t>
+  </si>
+  <si>
+    <t>2309-1036</t>
+  </si>
+  <si>
+    <t>2309-1037</t>
+  </si>
+  <si>
+    <t>2309-1038</t>
+  </si>
+  <si>
+    <t>2309-1039</t>
+  </si>
+  <si>
+    <t>2309-1040</t>
+  </si>
+  <si>
+    <t>2309-1041</t>
+  </si>
+  <si>
+    <t>2309-1042</t>
+  </si>
+  <si>
+    <t>2309-1043</t>
+  </si>
+  <si>
+    <t>2309-1044</t>
+  </si>
+  <si>
+    <t>2309-1045</t>
+  </si>
+  <si>
+    <t>2309-1046</t>
+  </si>
+  <si>
+    <t>2309-1047</t>
+  </si>
+  <si>
+    <t>2309-1048</t>
+  </si>
+  <si>
+    <t>2309-1049</t>
+  </si>
+  <si>
+    <t>2309-1050</t>
+  </si>
+  <si>
+    <t>2309-1051</t>
+  </si>
+  <si>
+    <t>2309-1052</t>
+  </si>
+  <si>
+    <t>2309-1053</t>
+  </si>
+  <si>
+    <t>2309-1054</t>
+  </si>
+  <si>
+    <t>2309-1055</t>
+  </si>
+  <si>
+    <t>2309-1056</t>
+  </si>
+  <si>
+    <t>2309-1057</t>
+  </si>
+  <si>
+    <t>2309-1058</t>
+  </si>
+  <si>
+    <t>2309-1059</t>
+  </si>
+  <si>
+    <t>2309-1060</t>
+  </si>
+  <si>
+    <t>2309-1061</t>
+  </si>
+  <si>
+    <t>2309-1062</t>
+  </si>
+  <si>
+    <t>2309-1063</t>
+  </si>
+  <si>
+    <t>2309-1064</t>
+  </si>
+  <si>
+    <t>2309-1065</t>
+  </si>
+  <si>
+    <t>2309-1066</t>
+  </si>
+  <si>
+    <t>2309-1067</t>
+  </si>
+  <si>
+    <t>2309-1068</t>
+  </si>
+  <si>
+    <t>2309-1069</t>
+  </si>
+  <si>
+    <t>2309-1070</t>
+  </si>
+  <si>
+    <t>2309-1071</t>
+  </si>
+  <si>
+    <t>2309-1072</t>
+  </si>
+  <si>
+    <t>2309-1073</t>
+  </si>
+  <si>
+    <t>2309-1074</t>
+  </si>
+  <si>
+    <t>2309-1075</t>
+  </si>
+  <si>
+    <t>2309-1076</t>
+  </si>
+  <si>
+    <t>2309-1077</t>
   </si>
 </sst>
 </file>
@@ -1385,7 +1988,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1398,8 +2001,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1418,11 +2027,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -1437,7 +2057,14 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3242,6 +3869,68 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{331FD294-EE6F-3D4E-A534-813A4D9D566E}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="E5:F10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="11">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="7"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Tag" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C06BC8A8-0124-C241-ADED-B97F2CE891ED}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B26" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
@@ -3380,71 +4069,9 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{331FD294-EE6F-3D4E-A534-813A4D9D566E}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="E5:F10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="11">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="7"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Tag" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{04D71FDC-83F7-5749-A2BA-4DE157ADFDC1}" name="Table1" displayName="Table1" ref="A1:K136" totalsRowShown="0">
-  <autoFilter ref="A1:K136" xr:uid="{04D71FDC-83F7-5749-A2BA-4DE157ADFDC1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{04D71FDC-83F7-5749-A2BA-4DE157ADFDC1}" name="Table1" displayName="Table1" ref="A1:K151" totalsRowShown="0">
+  <autoFilter ref="A1:K151" xr:uid="{04D71FDC-83F7-5749-A2BA-4DE157ADFDC1}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{6484B3DB-2BD1-7D46-B226-BA8DA8EE99F0}" name="Tag"/>
     <tableColumn id="2" xr3:uid="{4D4529CA-209A-6349-82DA-698D5E6A0E61}" name="SrcTag" dataDxfId="2"/>
@@ -4021,13 +4648,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B91ADC-4569-1C4E-B002-1ED2E647C959}">
-  <dimension ref="A1:K136"/>
+  <dimension ref="A1:K213"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="247" zoomScaleNormal="247" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B173" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I30" sqref="I30"/>
+      <selection pane="bottomRight" activeCell="D181" sqref="D181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8050,7 +8677,7 @@
       <c r="E136" t="s">
         <v>431</v>
       </c>
-      <c r="K136" s="10" t="str">
+      <c r="K136" t="str">
         <f>_xlfn.CONCAT(
 SUBSTITUTE(LOWER(B136),"-",""),
 ":",  C136,
@@ -8063,6 +8690,2101 @@
         <v>: -&gt; :unk [label='']</v>
       </c>
     </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>437</v>
+      </c>
+      <c r="B137" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="C137" t="s">
+        <v>251</v>
+      </c>
+      <c r="D137" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="E137" t="s">
+        <v>478</v>
+      </c>
+      <c r="F137" t="s">
+        <v>440</v>
+      </c>
+      <c r="G137" t="s">
+        <v>29</v>
+      </c>
+      <c r="H137" t="s">
+        <v>29</v>
+      </c>
+      <c r="I137" t="s">
+        <v>449</v>
+      </c>
+      <c r="K137" s="12" t="str">
+        <f>_xlfn.CONCAT(
+SUBSTITUTE(LOWER(B137),"-",""),
+":",  C137,
+ " -&gt; ",
+SUBSTITUTE(LOWER(D137),"-",""),
+ ":", E137,
+" [label='",
+ A137,
+"']")</f>
+        <v>zamua001:ch1 -&gt; zaiub001:s2_in01 [label='2309-1001']</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>562</v>
+      </c>
+      <c r="B138" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="C138" t="s">
+        <v>254</v>
+      </c>
+      <c r="D138" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="E138" t="s">
+        <v>479</v>
+      </c>
+      <c r="F138" t="s">
+        <v>440</v>
+      </c>
+      <c r="G138" t="s">
+        <v>29</v>
+      </c>
+      <c r="H138" t="s">
+        <v>29</v>
+      </c>
+      <c r="I138" t="s">
+        <v>450</v>
+      </c>
+      <c r="K138" s="12" t="str">
+        <f>_xlfn.CONCAT(
+SUBSTITUTE(LOWER(B138),"-",""),
+":",  C138,
+ " -&gt; ",
+SUBSTITUTE(LOWER(D138),"-",""),
+ ":", E138,
+" [label='",
+ A138,
+"']")</f>
+        <v>zamua001:ch2 -&gt; zaiub001:s2_in02 [label='2309-1002']</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>563</v>
+      </c>
+      <c r="B139" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="C139" t="s">
+        <v>441</v>
+      </c>
+      <c r="D139" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="E139" t="s">
+        <v>480</v>
+      </c>
+      <c r="F139" t="s">
+        <v>440</v>
+      </c>
+      <c r="G139" t="s">
+        <v>29</v>
+      </c>
+      <c r="H139" t="s">
+        <v>29</v>
+      </c>
+      <c r="I139" t="s">
+        <v>447</v>
+      </c>
+      <c r="K139" s="12" t="str">
+        <f>_xlfn.CONCAT(
+SUBSTITUTE(LOWER(B139),"-",""),
+":",  C139,
+ " -&gt; ",
+SUBSTITUTE(LOWER(D139),"-",""),
+ ":", E139,
+" [label='",
+ A139,
+"']")</f>
+        <v>zamua001:ch3 -&gt; zaiub001:s2_in03 [label='2309-1003']</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>564</v>
+      </c>
+      <c r="B140" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="C140" t="s">
+        <v>442</v>
+      </c>
+      <c r="D140" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="E140" t="s">
+        <v>481</v>
+      </c>
+      <c r="F140" t="s">
+        <v>440</v>
+      </c>
+      <c r="G140" t="s">
+        <v>29</v>
+      </c>
+      <c r="H140" t="s">
+        <v>29</v>
+      </c>
+      <c r="I140" t="s">
+        <v>448</v>
+      </c>
+      <c r="K140" s="12" t="str">
+        <f>_xlfn.CONCAT(
+SUBSTITUTE(LOWER(B140),"-",""),
+":",  C140,
+ " -&gt; ",
+SUBSTITUTE(LOWER(D140),"-",""),
+ ":", E140,
+" [label='",
+ A140,
+"']")</f>
+        <v>zamua001:ch4 -&gt; zaiub001:s2_in04 [label='2309-1004']</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>565</v>
+      </c>
+      <c r="B141" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="C141" t="s">
+        <v>251</v>
+      </c>
+      <c r="D141" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="E141" t="s">
+        <v>482</v>
+      </c>
+      <c r="F141" t="s">
+        <v>440</v>
+      </c>
+      <c r="G141" t="s">
+        <v>29</v>
+      </c>
+      <c r="H141" t="s">
+        <v>29</v>
+      </c>
+      <c r="I141" t="s">
+        <v>451</v>
+      </c>
+      <c r="K141" s="12" t="str">
+        <f>_xlfn.CONCAT(
+SUBSTITUTE(LOWER(B141),"-",""),
+":",  C141,
+ " -&gt; ",
+SUBSTITUTE(LOWER(D141),"-",""),
+ ":", E141,
+" [label='",
+ A141,
+"']")</f>
+        <v>zamub001:ch1 -&gt; zaiub001:s2_in05 [label='2309-1005']</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>566</v>
+      </c>
+      <c r="B142" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="C142" t="s">
+        <v>254</v>
+      </c>
+      <c r="D142" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="E142" t="s">
+        <v>477</v>
+      </c>
+      <c r="F142" t="s">
+        <v>440</v>
+      </c>
+      <c r="G142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H142" t="s">
+        <v>29</v>
+      </c>
+      <c r="I142" t="s">
+        <v>452</v>
+      </c>
+      <c r="K142" s="12" t="str">
+        <f t="shared" ref="K142:K144" si="10">_xlfn.CONCAT(
+SUBSTITUTE(LOWER(B142),"-",""),
+":",  C142,
+ " -&gt; ",
+SUBSTITUTE(LOWER(D142),"-",""),
+ ":", E142,
+" [label='",
+ A142,
+"']")</f>
+        <v>zamub001:ch2 -&gt; zaiub001:s2_in06 [label='2309-1006']</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>567</v>
+      </c>
+      <c r="B143" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="C143" t="s">
+        <v>441</v>
+      </c>
+      <c r="D143" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="E143" t="s">
+        <v>483</v>
+      </c>
+      <c r="F143" t="s">
+        <v>440</v>
+      </c>
+      <c r="G143" t="s">
+        <v>29</v>
+      </c>
+      <c r="H143" t="s">
+        <v>29</v>
+      </c>
+      <c r="I143" t="s">
+        <v>453</v>
+      </c>
+      <c r="K143" s="12" t="str">
+        <f t="shared" si="10"/>
+        <v>zamub001:ch3 -&gt; zaiub001:s2_in07 [label='2309-1007']</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>568</v>
+      </c>
+      <c r="B144" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="C144" t="s">
+        <v>442</v>
+      </c>
+      <c r="D144" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="E144" t="s">
+        <v>484</v>
+      </c>
+      <c r="F144" t="s">
+        <v>440</v>
+      </c>
+      <c r="G144" t="s">
+        <v>29</v>
+      </c>
+      <c r="H144" t="s">
+        <v>29</v>
+      </c>
+      <c r="I144" t="s">
+        <v>454</v>
+      </c>
+      <c r="K144" s="12" t="str">
+        <f t="shared" si="10"/>
+        <v>zamub001:ch4 -&gt; zaiub001:s2_in08 [label='2309-1008']</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>569</v>
+      </c>
+      <c r="B145" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="C145" t="s">
+        <v>251</v>
+      </c>
+      <c r="D145" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="E145" t="s">
+        <v>485</v>
+      </c>
+      <c r="F145" t="s">
+        <v>440</v>
+      </c>
+      <c r="G145" t="s">
+        <v>29</v>
+      </c>
+      <c r="H145" t="s">
+        <v>29</v>
+      </c>
+      <c r="I145" t="s">
+        <v>455</v>
+      </c>
+      <c r="K145" s="12" t="str">
+        <f t="shared" ref="K145:K148" si="11">_xlfn.CONCAT(
+SUBSTITUTE(LOWER(B145),"-",""),
+":",  C145,
+ " -&gt; ",
+SUBSTITUTE(LOWER(D145),"-",""),
+ ":", E145,
+" [label='",
+ A145,
+"']")</f>
+        <v>zamub002:ch1 -&gt; zaiub001:s2_in09 [label='2309-1009']</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>570</v>
+      </c>
+      <c r="B146" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="C146" t="s">
+        <v>254</v>
+      </c>
+      <c r="D146" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="E146" t="s">
+        <v>486</v>
+      </c>
+      <c r="F146" t="s">
+        <v>440</v>
+      </c>
+      <c r="G146" t="s">
+        <v>29</v>
+      </c>
+      <c r="H146" t="s">
+        <v>29</v>
+      </c>
+      <c r="I146" t="s">
+        <v>456</v>
+      </c>
+      <c r="K146" s="12" t="str">
+        <f t="shared" si="11"/>
+        <v>zamub002:ch2 -&gt; zaiub001:s2_in10 [label='2309-1010']</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>571</v>
+      </c>
+      <c r="B147" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="C147" t="s">
+        <v>441</v>
+      </c>
+      <c r="D147" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="E147" t="s">
+        <v>487</v>
+      </c>
+      <c r="F147" t="s">
+        <v>440</v>
+      </c>
+      <c r="G147" t="s">
+        <v>29</v>
+      </c>
+      <c r="H147" t="s">
+        <v>29</v>
+      </c>
+      <c r="I147" t="s">
+        <v>457</v>
+      </c>
+      <c r="K147" s="12" t="str">
+        <f t="shared" si="11"/>
+        <v>zamub002:ch3 -&gt; zaiub001:s2_in11 [label='2309-1011']</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>572</v>
+      </c>
+      <c r="B148" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="C148" t="s">
+        <v>442</v>
+      </c>
+      <c r="D148" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="E148" t="s">
+        <v>488</v>
+      </c>
+      <c r="F148" t="s">
+        <v>440</v>
+      </c>
+      <c r="G148" t="s">
+        <v>29</v>
+      </c>
+      <c r="H148" t="s">
+        <v>29</v>
+      </c>
+      <c r="I148" t="s">
+        <v>458</v>
+      </c>
+      <c r="K148" s="12" t="str">
+        <f t="shared" si="11"/>
+        <v>zamub002:ch4 -&gt; zaiub001:s2_in12 [label='2309-1012']</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>573</v>
+      </c>
+      <c r="B149" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="C149" t="s">
+        <v>442</v>
+      </c>
+      <c r="D149" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="E149" t="s">
+        <v>466</v>
+      </c>
+      <c r="F149" t="s">
+        <v>440</v>
+      </c>
+      <c r="G149" t="s">
+        <v>29</v>
+      </c>
+      <c r="H149" t="s">
+        <v>29</v>
+      </c>
+      <c r="I149" t="s">
+        <v>459</v>
+      </c>
+      <c r="K149" s="12" t="str">
+        <f>_xlfn.CONCAT(
+SUBSTITUTE(LOWER(B149),"-",""),
+":",  C149,
+ " -&gt; ",
+SUBSTITUTE(LOWER(D149),"-",""),
+ ":", E149,
+" [label='",
+ A149,
+"']")</f>
+        <v>zamub003:ch4 -&gt; zaiub001:s2___ [label='2309-1013']</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>574</v>
+      </c>
+      <c r="B150" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="C150" t="s">
+        <v>441</v>
+      </c>
+      <c r="D150" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="E150" t="s">
+        <v>478</v>
+      </c>
+      <c r="F150" t="s">
+        <v>440</v>
+      </c>
+      <c r="G150" t="s">
+        <v>29</v>
+      </c>
+      <c r="H150" t="s">
+        <v>29</v>
+      </c>
+      <c r="I150" t="s">
+        <v>460</v>
+      </c>
+      <c r="K150" s="12" t="str">
+        <f t="shared" ref="K150:K151" si="12">_xlfn.CONCAT(
+SUBSTITUTE(LOWER(B150),"-",""),
+":",  C150,
+ " -&gt; ",
+SUBSTITUTE(LOWER(D150),"-",""),
+ ":", E150,
+" [label='",
+ A150,
+"']")</f>
+        <v>zamub002:ch3 -&gt; zaiub002:s2_in01 [label='2309-1014']</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>575</v>
+      </c>
+      <c r="B151" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="C151" t="s">
+        <v>442</v>
+      </c>
+      <c r="D151" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="E151" t="s">
+        <v>479</v>
+      </c>
+      <c r="F151" t="s">
+        <v>440</v>
+      </c>
+      <c r="G151" t="s">
+        <v>29</v>
+      </c>
+      <c r="H151" t="s">
+        <v>29</v>
+      </c>
+      <c r="I151" t="s">
+        <v>461</v>
+      </c>
+      <c r="K151" s="12" t="str">
+        <f t="shared" si="12"/>
+        <v>zamub002:ch4 -&gt; zaiub002:s2_in02 [label='2309-1015']</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>576</v>
+      </c>
+      <c r="B152" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="C152" t="s">
+        <v>251</v>
+      </c>
+      <c r="D152" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="E152" t="s">
+        <v>480</v>
+      </c>
+      <c r="F152" t="s">
+        <v>440</v>
+      </c>
+      <c r="G152" t="s">
+        <v>29</v>
+      </c>
+      <c r="H152" t="s">
+        <v>29</v>
+      </c>
+      <c r="I152" s="10" t="s">
+        <v>462</v>
+      </c>
+      <c r="K152" s="12" t="str">
+        <f t="shared" ref="K152:K154" si="13">_xlfn.CONCAT(
+SUBSTITUTE(LOWER(B152),"-",""),
+":",  C152,
+ " -&gt; ",
+SUBSTITUTE(LOWER(D152),"-",""),
+ ":", E152,
+" [label='",
+ A152,
+"']")</f>
+        <v>zamub003:ch1 -&gt; zaiub002:s2_in03 [label='2309-1016']</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>577</v>
+      </c>
+      <c r="B153" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="C153" t="s">
+        <v>254</v>
+      </c>
+      <c r="D153" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="E153" t="s">
+        <v>481</v>
+      </c>
+      <c r="F153" t="s">
+        <v>440</v>
+      </c>
+      <c r="G153" t="s">
+        <v>29</v>
+      </c>
+      <c r="H153" t="s">
+        <v>29</v>
+      </c>
+      <c r="I153" s="10" t="s">
+        <v>463</v>
+      </c>
+      <c r="K153" s="12" t="str">
+        <f t="shared" si="13"/>
+        <v>zamub003:ch2 -&gt; zaiub002:s2_in04 [label='2309-1017']</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>578</v>
+      </c>
+      <c r="B154" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="C154" t="s">
+        <v>441</v>
+      </c>
+      <c r="D154" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="E154" t="s">
+        <v>482</v>
+      </c>
+      <c r="F154" t="s">
+        <v>440</v>
+      </c>
+      <c r="G154" t="s">
+        <v>29</v>
+      </c>
+      <c r="H154" t="s">
+        <v>29</v>
+      </c>
+      <c r="I154" s="10" t="s">
+        <v>464</v>
+      </c>
+      <c r="K154" s="12" t="str">
+        <f t="shared" si="13"/>
+        <v>zamub003:ch3 -&gt; zaiub002:s2_in05 [label='2309-1018']</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>579</v>
+      </c>
+      <c r="B155" s="13" t="s">
+        <v>445</v>
+      </c>
+      <c r="C155" s="11" t="s">
+        <v>442</v>
+      </c>
+      <c r="D155" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="E155" t="s">
+        <v>477</v>
+      </c>
+      <c r="F155" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G155" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H155" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I155" s="14" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>580</v>
+      </c>
+      <c r="B156" s="6" t="s">
+        <v>467</v>
+      </c>
+      <c r="C156" s="15" t="s">
+        <v>468</v>
+      </c>
+      <c r="D156" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E156" t="s">
+        <v>469</v>
+      </c>
+      <c r="F156" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G156" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H156" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>581</v>
+      </c>
+      <c r="B157" s="6" t="s">
+        <v>467</v>
+      </c>
+      <c r="C157" s="15" t="s">
+        <v>470</v>
+      </c>
+      <c r="D157" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E157" t="s">
+        <v>471</v>
+      </c>
+      <c r="F157" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G157" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H157" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A158" s="17" t="s">
+        <v>582</v>
+      </c>
+      <c r="B158" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="C158" s="15" t="s">
+        <v>468</v>
+      </c>
+      <c r="D158" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E158" t="s">
+        <v>472</v>
+      </c>
+      <c r="F158" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G158" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H158" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>583</v>
+      </c>
+      <c r="B159" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="C159" s="15" t="s">
+        <v>470</v>
+      </c>
+      <c r="D159" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E159" t="s">
+        <v>473</v>
+      </c>
+      <c r="F159" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G159" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H159" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>584</v>
+      </c>
+      <c r="B160" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C160" s="15" t="s">
+        <v>468</v>
+      </c>
+      <c r="D160" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E160" t="s">
+        <v>474</v>
+      </c>
+      <c r="F160" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G160" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H160" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>585</v>
+      </c>
+      <c r="B161" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C161" s="15" t="s">
+        <v>470</v>
+      </c>
+      <c r="D161" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E161" t="s">
+        <v>475</v>
+      </c>
+      <c r="F161" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G161" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H161" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>586</v>
+      </c>
+      <c r="B162" s="13" t="s">
+        <v>439</v>
+      </c>
+      <c r="C162" s="15" t="s">
+        <v>476</v>
+      </c>
+      <c r="D162" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E162" t="s">
+        <v>514</v>
+      </c>
+      <c r="F162" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G162" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H162" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>587</v>
+      </c>
+      <c r="B163" s="13" t="s">
+        <v>439</v>
+      </c>
+      <c r="C163" s="15" t="s">
+        <v>489</v>
+      </c>
+      <c r="D163" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E163" t="s">
+        <v>515</v>
+      </c>
+      <c r="F163" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G163" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H163" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>588</v>
+      </c>
+      <c r="B164" s="13" t="s">
+        <v>439</v>
+      </c>
+      <c r="C164" s="15" t="s">
+        <v>490</v>
+      </c>
+      <c r="D164" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E164" t="s">
+        <v>516</v>
+      </c>
+      <c r="F164" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G164" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H164" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>589</v>
+      </c>
+      <c r="B165" s="13" t="s">
+        <v>439</v>
+      </c>
+      <c r="C165" s="15" t="s">
+        <v>491</v>
+      </c>
+      <c r="D165" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E165" t="s">
+        <v>517</v>
+      </c>
+      <c r="F165" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G165" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H165" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>590</v>
+      </c>
+      <c r="B166" s="13" t="s">
+        <v>439</v>
+      </c>
+      <c r="C166" s="15" t="s">
+        <v>492</v>
+      </c>
+      <c r="D166" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E166" t="s">
+        <v>518</v>
+      </c>
+      <c r="F166" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G166" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H166" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>591</v>
+      </c>
+      <c r="B167" s="13" t="s">
+        <v>439</v>
+      </c>
+      <c r="C167" s="15" t="s">
+        <v>493</v>
+      </c>
+      <c r="D167" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E167" t="s">
+        <v>519</v>
+      </c>
+      <c r="F167" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G167" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H167" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>592</v>
+      </c>
+      <c r="B168" s="13" t="s">
+        <v>439</v>
+      </c>
+      <c r="C168" s="15" t="s">
+        <v>494</v>
+      </c>
+      <c r="D168" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E168" t="s">
+        <v>520</v>
+      </c>
+      <c r="F168" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G168" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H168" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>593</v>
+      </c>
+      <c r="B169" s="13" t="s">
+        <v>439</v>
+      </c>
+      <c r="C169" s="15" t="s">
+        <v>495</v>
+      </c>
+      <c r="D169" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E169" t="s">
+        <v>521</v>
+      </c>
+      <c r="F169" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G169" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H169" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>594</v>
+      </c>
+      <c r="B170" s="13" t="s">
+        <v>439</v>
+      </c>
+      <c r="C170" s="15" t="s">
+        <v>496</v>
+      </c>
+      <c r="D170" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E170" t="s">
+        <v>522</v>
+      </c>
+      <c r="F170" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G170" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H170" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>595</v>
+      </c>
+      <c r="B171" s="13" t="s">
+        <v>439</v>
+      </c>
+      <c r="C171" s="15" t="s">
+        <v>497</v>
+      </c>
+      <c r="D171" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E171" t="s">
+        <v>523</v>
+      </c>
+      <c r="F171" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G171" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H171" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>596</v>
+      </c>
+      <c r="B172" s="13" t="s">
+        <v>439</v>
+      </c>
+      <c r="C172" s="15" t="s">
+        <v>498</v>
+      </c>
+      <c r="D172" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E172" t="s">
+        <v>524</v>
+      </c>
+      <c r="F172" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G172" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H172" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>597</v>
+      </c>
+      <c r="B173" s="13" t="s">
+        <v>439</v>
+      </c>
+      <c r="C173" s="15" t="s">
+        <v>499</v>
+      </c>
+      <c r="D173" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E173" t="s">
+        <v>525</v>
+      </c>
+      <c r="F173" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G173" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H173" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>598</v>
+      </c>
+      <c r="B174" s="13" t="s">
+        <v>439</v>
+      </c>
+      <c r="C174" s="15" t="s">
+        <v>500</v>
+      </c>
+      <c r="D174" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E174" t="s">
+        <v>526</v>
+      </c>
+      <c r="F174" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G174" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H174" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>599</v>
+      </c>
+      <c r="B175" s="13" t="s">
+        <v>439</v>
+      </c>
+      <c r="C175" s="15" t="s">
+        <v>501</v>
+      </c>
+      <c r="D175" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E175" t="s">
+        <v>527</v>
+      </c>
+      <c r="F175" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G175" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H175" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>600</v>
+      </c>
+      <c r="B176" s="13" t="s">
+        <v>439</v>
+      </c>
+      <c r="C176" s="15" t="s">
+        <v>502</v>
+      </c>
+      <c r="D176" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E176" t="s">
+        <v>528</v>
+      </c>
+      <c r="F176" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G176" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H176" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>601</v>
+      </c>
+      <c r="B177" s="13" t="s">
+        <v>439</v>
+      </c>
+      <c r="C177" s="15" t="s">
+        <v>503</v>
+      </c>
+      <c r="D177" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E177" t="s">
+        <v>529</v>
+      </c>
+      <c r="F177" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G177" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H177" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>602</v>
+      </c>
+      <c r="B178" s="16"/>
+      <c r="C178" s="15"/>
+      <c r="D178" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E178" t="s">
+        <v>530</v>
+      </c>
+      <c r="F178" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G178" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H178" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>603</v>
+      </c>
+      <c r="B179" s="16"/>
+      <c r="C179" s="15"/>
+      <c r="D179" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E179" t="s">
+        <v>531</v>
+      </c>
+      <c r="F179" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G179" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H179" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>604</v>
+      </c>
+      <c r="B180" s="16"/>
+      <c r="C180" s="15"/>
+      <c r="D180" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E180" t="s">
+        <v>532</v>
+      </c>
+      <c r="F180" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G180" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H180" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>605</v>
+      </c>
+      <c r="B181" s="16"/>
+      <c r="C181" s="15"/>
+      <c r="D181" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E181" t="s">
+        <v>533</v>
+      </c>
+      <c r="F181" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G181" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H181" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>606</v>
+      </c>
+      <c r="B182" s="16"/>
+      <c r="C182" s="15"/>
+      <c r="D182" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E182" t="s">
+        <v>534</v>
+      </c>
+      <c r="F182" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G182" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H182" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>607</v>
+      </c>
+      <c r="B183" s="16"/>
+      <c r="C183" s="15"/>
+      <c r="D183" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E183" t="s">
+        <v>535</v>
+      </c>
+      <c r="F183" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G183" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H183" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>608</v>
+      </c>
+      <c r="B184" s="16"/>
+      <c r="C184" s="15"/>
+      <c r="D184" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E184" t="s">
+        <v>536</v>
+      </c>
+      <c r="F184" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G184" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H184" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>609</v>
+      </c>
+      <c r="B185" s="16"/>
+      <c r="C185" s="15"/>
+      <c r="D185" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E185" t="s">
+        <v>537</v>
+      </c>
+      <c r="F185" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G185" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H185" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>610</v>
+      </c>
+      <c r="B186" s="16"/>
+      <c r="C186" s="15"/>
+      <c r="D186" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E186" t="s">
+        <v>538</v>
+      </c>
+      <c r="F186" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G186" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H186" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>611</v>
+      </c>
+      <c r="B187" s="16"/>
+      <c r="C187" s="15"/>
+      <c r="D187" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E187" t="s">
+        <v>539</v>
+      </c>
+      <c r="F187" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G187" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H187" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>612</v>
+      </c>
+      <c r="B188" s="16"/>
+      <c r="C188" s="15"/>
+      <c r="D188" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E188" t="s">
+        <v>540</v>
+      </c>
+      <c r="F188" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G188" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H188" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>613</v>
+      </c>
+      <c r="B189" s="16"/>
+      <c r="C189" s="15"/>
+      <c r="D189" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E189" t="s">
+        <v>541</v>
+      </c>
+      <c r="F189" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G189" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H189" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>614</v>
+      </c>
+      <c r="B190" s="16"/>
+      <c r="C190" s="15"/>
+      <c r="D190" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E190" t="s">
+        <v>542</v>
+      </c>
+      <c r="F190" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G190" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H190" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>615</v>
+      </c>
+      <c r="B191" s="16"/>
+      <c r="C191" s="15"/>
+      <c r="D191" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E191" t="s">
+        <v>543</v>
+      </c>
+      <c r="F191" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G191" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H191" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>616</v>
+      </c>
+      <c r="B192" s="16"/>
+      <c r="C192" s="15"/>
+      <c r="D192" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E192" t="s">
+        <v>544</v>
+      </c>
+      <c r="F192" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G192" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H192" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>617</v>
+      </c>
+      <c r="B193" s="16"/>
+      <c r="C193" s="15"/>
+      <c r="D193" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E193" t="s">
+        <v>545</v>
+      </c>
+      <c r="F193" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G193" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H193" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>618</v>
+      </c>
+      <c r="B194" s="16"/>
+      <c r="C194" s="15"/>
+      <c r="D194" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E194" t="s">
+        <v>546</v>
+      </c>
+      <c r="F194" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G194" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H194" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>619</v>
+      </c>
+      <c r="B195" s="16"/>
+      <c r="C195" s="15"/>
+      <c r="D195" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E195" t="s">
+        <v>547</v>
+      </c>
+      <c r="F195" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G195" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H195" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>620</v>
+      </c>
+      <c r="B196" s="16"/>
+      <c r="C196" s="15"/>
+      <c r="D196" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E196" t="s">
+        <v>548</v>
+      </c>
+      <c r="F196" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G196" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H196" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>621</v>
+      </c>
+      <c r="B197" s="16"/>
+      <c r="C197" s="15"/>
+      <c r="D197" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E197" t="s">
+        <v>549</v>
+      </c>
+      <c r="F197" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G197" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H197" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>622</v>
+      </c>
+      <c r="B198" s="16"/>
+      <c r="C198" s="15"/>
+      <c r="D198" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E198" t="s">
+        <v>550</v>
+      </c>
+      <c r="F198" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G198" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H198" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>623</v>
+      </c>
+      <c r="B199" s="16"/>
+      <c r="C199" s="15"/>
+      <c r="D199" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E199" t="s">
+        <v>551</v>
+      </c>
+      <c r="F199" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G199" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H199" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>624</v>
+      </c>
+      <c r="B200" s="16"/>
+      <c r="C200" s="15"/>
+      <c r="D200" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E200" t="s">
+        <v>552</v>
+      </c>
+      <c r="F200" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G200" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H200" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>625</v>
+      </c>
+      <c r="B201" s="16"/>
+      <c r="C201" s="15"/>
+      <c r="D201" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E201" t="s">
+        <v>553</v>
+      </c>
+      <c r="F201" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G201" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H201" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>626</v>
+      </c>
+      <c r="B202" s="16"/>
+      <c r="C202" s="15"/>
+      <c r="D202" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E202" t="s">
+        <v>554</v>
+      </c>
+      <c r="F202" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G202" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H202" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>627</v>
+      </c>
+      <c r="B203" s="16"/>
+      <c r="C203" s="15"/>
+      <c r="D203" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E203" t="s">
+        <v>555</v>
+      </c>
+      <c r="F203" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G203" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H203" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>628</v>
+      </c>
+      <c r="B204" s="16"/>
+      <c r="C204" s="15"/>
+      <c r="D204" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E204" t="s">
+        <v>556</v>
+      </c>
+      <c r="F204" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G204" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H204" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>629</v>
+      </c>
+      <c r="B205" s="16"/>
+      <c r="C205" s="15"/>
+      <c r="D205" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E205" t="s">
+        <v>557</v>
+      </c>
+      <c r="F205" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G205" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H205" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>630</v>
+      </c>
+      <c r="B206" s="16"/>
+      <c r="C206" s="15"/>
+      <c r="D206" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E206" t="s">
+        <v>558</v>
+      </c>
+      <c r="F206" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G206" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H206" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>631</v>
+      </c>
+      <c r="B207" s="16"/>
+      <c r="C207" s="15"/>
+      <c r="D207" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E207" t="s">
+        <v>559</v>
+      </c>
+      <c r="F207" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G207" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H207" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>632</v>
+      </c>
+      <c r="B208" s="16"/>
+      <c r="C208" s="15"/>
+      <c r="D208" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E208" t="s">
+        <v>560</v>
+      </c>
+      <c r="F208" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G208" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H208" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>633</v>
+      </c>
+      <c r="B209" s="16"/>
+      <c r="C209" s="15"/>
+      <c r="D209" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E209" t="s">
+        <v>561</v>
+      </c>
+      <c r="F209" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G209" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H209" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>634</v>
+      </c>
+      <c r="B210" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C210" t="s">
+        <v>510</v>
+      </c>
+      <c r="D210" s="6" t="s">
+        <v>508</v>
+      </c>
+      <c r="E210" t="s">
+        <v>251</v>
+      </c>
+      <c r="F210" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G210" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H210" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I210" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>635</v>
+      </c>
+      <c r="B211" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C211" t="s">
+        <v>511</v>
+      </c>
+      <c r="D211" s="6" t="s">
+        <v>508</v>
+      </c>
+      <c r="E211" t="s">
+        <v>254</v>
+      </c>
+      <c r="F211" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G211" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H211" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I211" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>636</v>
+      </c>
+      <c r="B212" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C212" t="s">
+        <v>512</v>
+      </c>
+      <c r="D212" s="6" t="s">
+        <v>509</v>
+      </c>
+      <c r="E212" t="s">
+        <v>251</v>
+      </c>
+      <c r="F212" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G212" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H212" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I212" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="213" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>637</v>
+      </c>
+      <c r="B213" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C213" t="s">
+        <v>513</v>
+      </c>
+      <c r="D213" s="6" t="s">
+        <v>509</v>
+      </c>
+      <c r="E213" t="s">
+        <v>254</v>
+      </c>
+      <c r="F213" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="G213" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H213" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I213" t="s">
+        <v>507</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Round of revisions on sdl
</commit_message>
<xml_diff>
--- a/data/uac_cables.xlsx
+++ b/data/uac_cables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/donert/Documents/UACTech/SystemDocumentation/github/uactechdoc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD739D39-229B-5646-9418-E136554699E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33849117-E40E-AC4F-AD99-D91B3DEB4365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-59200" yWindow="-27800" windowWidth="50440" windowHeight="28420" xr2:uid="{288904EE-D384-EA4C-9B98-052B972FB267}"/>
+    <workbookView xWindow="-53660" yWindow="-31600" windowWidth="51200" windowHeight="36160" xr2:uid="{288904EE-D384-EA4C-9B98-052B972FB267}"/>
   </bookViews>
   <sheets>
     <sheet name="Cables" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1825" uniqueCount="728">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2071" uniqueCount="837">
   <si>
     <t>Tag</t>
   </si>
@@ -2224,6 +2224,333 @@
   </si>
   <si>
     <t xml:space="preserve">Stage Cam </t>
+  </si>
+  <si>
+    <t>2309-3001</t>
+  </si>
+  <si>
+    <t>loop_out</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>empty port</t>
+  </si>
+  <si>
+    <t>ZLKU-C001</t>
+  </si>
+  <si>
+    <t>dmx_out_n</t>
+  </si>
+  <si>
+    <t>ZLIU-0003</t>
+  </si>
+  <si>
+    <t>dmx_in</t>
+  </si>
+  <si>
+    <t>dmx5</t>
+  </si>
+  <si>
+    <t>2309-3004</t>
+  </si>
+  <si>
+    <t>dmx_out</t>
+  </si>
+  <si>
+    <t>dmx3</t>
+  </si>
+  <si>
+    <t>2309-3003</t>
+  </si>
+  <si>
+    <t>2309-3002</t>
+  </si>
+  <si>
+    <t>a243</t>
+  </si>
+  <si>
+    <t>a244</t>
+  </si>
+  <si>
+    <t>a245</t>
+  </si>
+  <si>
+    <t>a246</t>
+  </si>
+  <si>
+    <t>balcony east</t>
+  </si>
+  <si>
+    <t>dmx</t>
+  </si>
+  <si>
+    <t>a250</t>
+  </si>
+  <si>
+    <t>a251</t>
+  </si>
+  <si>
+    <t>a252</t>
+  </si>
+  <si>
+    <t>ZLKU-B002</t>
+  </si>
+  <si>
+    <t>4wire</t>
+  </si>
+  <si>
+    <t>bluetooth</t>
+  </si>
+  <si>
+    <t>echo_app</t>
+  </si>
+  <si>
+    <t>ZLIU-A001</t>
+  </si>
+  <si>
+    <t>dmx_out_x3</t>
+  </si>
+  <si>
+    <t>dmx_out_x4</t>
+  </si>
+  <si>
+    <t>ZLIU-A003</t>
+  </si>
+  <si>
+    <t>stage</t>
+  </si>
+  <si>
+    <t>topbar</t>
+  </si>
+  <si>
+    <t>thrustbar</t>
+  </si>
+  <si>
+    <t>dmx_out_x5</t>
+  </si>
+  <si>
+    <t>ZLIU-A004</t>
+  </si>
+  <si>
+    <t>ZLIU-B001</t>
+  </si>
+  <si>
+    <t>ZLIU-B002</t>
+  </si>
+  <si>
+    <t>ZLIU-B003</t>
+  </si>
+  <si>
+    <t>ZLIU-A002</t>
+  </si>
+  <si>
+    <t>ketranet</t>
+  </si>
+  <si>
+    <t>all_ketra</t>
+  </si>
+  <si>
+    <t>a263</t>
+  </si>
+  <si>
+    <t>a262</t>
+  </si>
+  <si>
+    <t>a258</t>
+  </si>
+  <si>
+    <t>a257</t>
+  </si>
+  <si>
+    <t>a256</t>
+  </si>
+  <si>
+    <t>aa254</t>
+  </si>
+  <si>
+    <t>2310-0220</t>
+  </si>
+  <si>
+    <t>dmx_b</t>
+  </si>
+  <si>
+    <t>2310-0226</t>
+  </si>
+  <si>
+    <t>2310-0227</t>
+  </si>
+  <si>
+    <t>2310-0228</t>
+  </si>
+  <si>
+    <t>2310-0229</t>
+  </si>
+  <si>
+    <t>dmx_thru</t>
+  </si>
+  <si>
+    <t>2310-0223</t>
+  </si>
+  <si>
+    <t>2310-0224</t>
+  </si>
+  <si>
+    <t>rockville</t>
+  </si>
+  <si>
+    <t>dmx_a</t>
+  </si>
+  <si>
+    <t>2310-0225</t>
+  </si>
+  <si>
+    <t>free</t>
+  </si>
+  <si>
+    <t>dmx_c</t>
+  </si>
+  <si>
+    <t>dmx_e</t>
+  </si>
+  <si>
+    <t>dmx_f</t>
+  </si>
+  <si>
+    <t>dmx_g</t>
+  </si>
+  <si>
+    <t>dmx_h</t>
+  </si>
+  <si>
+    <t>dmx_d</t>
+  </si>
+  <si>
+    <t>attic_1</t>
+  </si>
+  <si>
+    <t>attic_2</t>
+  </si>
+  <si>
+    <t>attic_3</t>
+  </si>
+  <si>
+    <t>attic_4</t>
+  </si>
+  <si>
+    <t>attic_5</t>
+  </si>
+  <si>
+    <t>attic_6</t>
+  </si>
+  <si>
+    <t>a267</t>
+  </si>
+  <si>
+    <t>a268</t>
+  </si>
+  <si>
+    <t>a269</t>
+  </si>
+  <si>
+    <t>a270</t>
+  </si>
+  <si>
+    <t>a271</t>
+  </si>
+  <si>
+    <t>a272</t>
+  </si>
+  <si>
+    <t>2310-0201</t>
+  </si>
+  <si>
+    <t>2310-0209</t>
+  </si>
+  <si>
+    <t>2310-0210</t>
+  </si>
+  <si>
+    <t>2310-0202</t>
+  </si>
+  <si>
+    <t>2310-0211</t>
+  </si>
+  <si>
+    <t>2310-0203</t>
+  </si>
+  <si>
+    <t>red heat shrink</t>
+  </si>
+  <si>
+    <t>dmx53</t>
+  </si>
+  <si>
+    <t>0.3m</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>2310-0204</t>
+  </si>
+  <si>
+    <t>2310-0205</t>
+  </si>
+  <si>
+    <t>dmx35</t>
+  </si>
+  <si>
+    <t>2310-0212</t>
+  </si>
+  <si>
+    <t>ZLLU-B051</t>
+  </si>
+  <si>
+    <t>2310-0214</t>
+  </si>
+  <si>
+    <t>ZLLU-B054</t>
+  </si>
+  <si>
+    <t>rj45-dmx5</t>
+  </si>
+  <si>
+    <t>ZLLU-B052</t>
+  </si>
+  <si>
+    <t>2310-0217</t>
+  </si>
+  <si>
+    <t>ZLLU-B053</t>
+  </si>
+  <si>
+    <t>2310-0218</t>
+  </si>
+  <si>
+    <t>terminator</t>
+  </si>
+  <si>
+    <t>balcony west</t>
+  </si>
+  <si>
+    <t>extension</t>
+  </si>
+  <si>
+    <t>out_1_closet</t>
+  </si>
+  <si>
+    <t>out_2_west</t>
+  </si>
+  <si>
+    <t>out_3_east</t>
+  </si>
+  <si>
+    <t>2310-0501</t>
+  </si>
+  <si>
+    <t>2310-0502</t>
   </si>
 </sst>
 </file>
@@ -2266,7 +2593,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2297,8 +2624,14 @@
         <bgColor rgb="FFD9E1F2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFD9E1F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -2414,11 +2747,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF8EA9DB"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF8EA9DB"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2458,6 +2802,14 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4316,7 +4668,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C06BC8A8-0124-C241-ADED-B97F2CE891ED}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C06BC8A8-0124-C241-ADED-B97F2CE891ED}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B26" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField dataField="1" showAll="0"/>
@@ -4455,7 +4807,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{331FD294-EE6F-3D4E-A534-813A4D9D566E}" name="PivotTable2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{331FD294-EE6F-3D4E-A534-813A4D9D566E}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="E5:F10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField dataField="1" showAll="0"/>
@@ -4517,8 +4869,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD7E3698-8860-904B-8BDB-00EF1039C49C}" name="Table1" displayName="Table1" ref="A1:L240" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="5">
-  <autoFilter ref="A1:L240" xr:uid="{BD7E3698-8860-904B-8BDB-00EF1039C49C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD7E3698-8860-904B-8BDB-00EF1039C49C}" name="Table1" displayName="Table1" ref="A1:L279" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="5">
+  <autoFilter ref="A1:L279" xr:uid="{BD7E3698-8860-904B-8BDB-00EF1039C49C}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{4D442337-BE86-B24A-84A4-338FB80A6A49}" name="Tag"/>
     <tableColumn id="2" xr3:uid="{74A36D7B-C989-3B4B-B1E5-AB1FA4C2DD45}" name="SrcTag" dataDxfId="4"/>
@@ -4834,13 +5186,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B91ADC-4569-1C4E-B002-1ED2E647C959}">
-  <dimension ref="A1:L240"/>
+  <dimension ref="A1:L280"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="310" zoomScaleNormal="310" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B238" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B27" sqref="B27"/>
+      <selection pane="bottomRight" activeCell="F258" sqref="F258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5769,11 +6121,9 @@
         <v>50</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>35</v>
-      </c>
+        <v>410</v>
+      </c>
+      <c r="C28" s="13"/>
       <c r="D28" s="12" t="s">
         <v>24</v>
       </c>
@@ -5796,7 +6146,7 @@
       <c r="K28" s="13"/>
       <c r="L28" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>zviud001:sdi -&gt; 23071821:barrel [label='2307-1826']</v>
+        <v>unknown: -&gt; 23071821:barrel [label='2307-1826']</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
@@ -12037,6 +12387,901 @@
       </c>
       <c r="F240" s="3"/>
       <c r="K240" s="3"/>
+    </row>
+    <row r="241" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A241" t="s">
+        <v>728</v>
+      </c>
+      <c r="B241" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C241" t="s">
+        <v>729</v>
+      </c>
+      <c r="F241" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H241" t="s">
+        <v>730</v>
+      </c>
+      <c r="I241" t="s">
+        <v>731</v>
+      </c>
+      <c r="K241" s="3"/>
+    </row>
+    <row r="242" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A242" t="s">
+        <v>807</v>
+      </c>
+      <c r="B242" s="3" t="s">
+        <v>732</v>
+      </c>
+      <c r="C242" t="s">
+        <v>733</v>
+      </c>
+      <c r="D242" s="3" t="s">
+        <v>734</v>
+      </c>
+      <c r="E242" t="s">
+        <v>735</v>
+      </c>
+      <c r="F242" s="3" t="s">
+        <v>736</v>
+      </c>
+      <c r="G242" t="s">
+        <v>34</v>
+      </c>
+      <c r="H242" t="s">
+        <v>730</v>
+      </c>
+      <c r="K242" s="3"/>
+    </row>
+    <row r="243" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A243" t="s">
+        <v>742</v>
+      </c>
+      <c r="D243" s="3" t="s">
+        <v>737</v>
+      </c>
+      <c r="E243" t="s">
+        <v>738</v>
+      </c>
+      <c r="F243" s="3" t="s">
+        <v>739</v>
+      </c>
+      <c r="K243" s="3"/>
+    </row>
+    <row r="244" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A244" t="s">
+        <v>743</v>
+      </c>
+      <c r="B244" s="3" t="s">
+        <v>737</v>
+      </c>
+      <c r="C244" t="s">
+        <v>735</v>
+      </c>
+      <c r="D244" s="3" t="s">
+        <v>740</v>
+      </c>
+      <c r="E244" t="s">
+        <v>738</v>
+      </c>
+      <c r="F244" s="3" t="s">
+        <v>739</v>
+      </c>
+      <c r="K244" s="3"/>
+    </row>
+    <row r="245" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A245" t="s">
+        <v>744</v>
+      </c>
+      <c r="B245" s="3" t="s">
+        <v>740</v>
+      </c>
+      <c r="C245" t="s">
+        <v>735</v>
+      </c>
+      <c r="D245" s="3" t="s">
+        <v>741</v>
+      </c>
+      <c r="E245" t="s">
+        <v>738</v>
+      </c>
+      <c r="F245" s="3" t="s">
+        <v>739</v>
+      </c>
+      <c r="K245" s="3"/>
+    </row>
+    <row r="246" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A246" t="s">
+        <v>745</v>
+      </c>
+      <c r="B246" s="3" t="s">
+        <v>741</v>
+      </c>
+      <c r="C246" t="s">
+        <v>735</v>
+      </c>
+      <c r="D246" s="3" t="s">
+        <v>728</v>
+      </c>
+      <c r="E246" t="s">
+        <v>738</v>
+      </c>
+      <c r="F246" s="3" t="s">
+        <v>739</v>
+      </c>
+      <c r="K246" s="3"/>
+    </row>
+    <row r="247" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A247" t="s">
+        <v>808</v>
+      </c>
+      <c r="B247" s="3" t="s">
+        <v>734</v>
+      </c>
+      <c r="C247" t="s">
+        <v>834</v>
+      </c>
+      <c r="D247" s="3" t="s">
+        <v>825</v>
+      </c>
+      <c r="E247" t="s">
+        <v>721</v>
+      </c>
+      <c r="F247" s="35" t="s">
+        <v>293</v>
+      </c>
+      <c r="G247" s="36"/>
+      <c r="I247" t="s">
+        <v>746</v>
+      </c>
+      <c r="K247" s="35"/>
+    </row>
+    <row r="248" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A248" t="s">
+        <v>826</v>
+      </c>
+      <c r="B248" s="3" t="s">
+        <v>825</v>
+      </c>
+      <c r="C248" t="s">
+        <v>256</v>
+      </c>
+      <c r="D248" s="3" t="s">
+        <v>827</v>
+      </c>
+      <c r="E248" t="s">
+        <v>721</v>
+      </c>
+      <c r="F248" s="35" t="s">
+        <v>824</v>
+      </c>
+      <c r="G248" s="36"/>
+      <c r="I248" t="s">
+        <v>746</v>
+      </c>
+      <c r="K248" s="35"/>
+    </row>
+    <row r="249" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A249" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="B249" s="3" t="s">
+        <v>827</v>
+      </c>
+      <c r="C249" t="s">
+        <v>256</v>
+      </c>
+      <c r="D249" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="E249" t="s">
+        <v>721</v>
+      </c>
+      <c r="F249" s="35" t="s">
+        <v>736</v>
+      </c>
+      <c r="G249" s="36">
+        <v>0</v>
+      </c>
+      <c r="H249" t="s">
+        <v>133</v>
+      </c>
+      <c r="I249" t="s">
+        <v>829</v>
+      </c>
+      <c r="K249" s="35"/>
+    </row>
+    <row r="250" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A250" t="s">
+        <v>822</v>
+      </c>
+      <c r="B250" s="3" t="s">
+        <v>823</v>
+      </c>
+      <c r="C250" t="s">
+        <v>256</v>
+      </c>
+      <c r="D250" s="3" t="s">
+        <v>821</v>
+      </c>
+      <c r="E250" t="s">
+        <v>721</v>
+      </c>
+      <c r="F250" s="35" t="s">
+        <v>824</v>
+      </c>
+      <c r="G250" s="36" t="s">
+        <v>403</v>
+      </c>
+      <c r="I250" t="s">
+        <v>830</v>
+      </c>
+      <c r="K250" s="35"/>
+    </row>
+    <row r="251" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A251" t="s">
+        <v>809</v>
+      </c>
+      <c r="B251" s="3" t="s">
+        <v>734</v>
+      </c>
+      <c r="C251" t="s">
+        <v>833</v>
+      </c>
+      <c r="D251" s="3" t="s">
+        <v>823</v>
+      </c>
+      <c r="E251" t="s">
+        <v>747</v>
+      </c>
+      <c r="F251" s="35" t="s">
+        <v>293</v>
+      </c>
+      <c r="G251" s="36"/>
+      <c r="I251" t="s">
+        <v>830</v>
+      </c>
+      <c r="K251" s="35"/>
+    </row>
+    <row r="252" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A252" t="s">
+        <v>810</v>
+      </c>
+      <c r="B252" s="3" t="s">
+        <v>734</v>
+      </c>
+      <c r="C252" t="s">
+        <v>832</v>
+      </c>
+      <c r="D252" t="s">
+        <v>812</v>
+      </c>
+      <c r="E252" t="s">
+        <v>747</v>
+      </c>
+      <c r="F252" s="35" t="s">
+        <v>747</v>
+      </c>
+      <c r="G252" s="36" t="s">
+        <v>816</v>
+      </c>
+      <c r="H252" t="s">
+        <v>133</v>
+      </c>
+      <c r="J252" t="s">
+        <v>813</v>
+      </c>
+      <c r="K252" s="35"/>
+    </row>
+    <row r="253" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A253" t="s">
+        <v>812</v>
+      </c>
+      <c r="B253" t="s">
+        <v>810</v>
+      </c>
+      <c r="C253" t="s">
+        <v>747</v>
+      </c>
+      <c r="D253" s="3" t="s">
+        <v>811</v>
+      </c>
+      <c r="E253" t="s">
+        <v>747</v>
+      </c>
+      <c r="F253" s="35" t="s">
+        <v>814</v>
+      </c>
+      <c r="G253" s="36" t="s">
+        <v>815</v>
+      </c>
+      <c r="H253" t="s">
+        <v>133</v>
+      </c>
+      <c r="K253" s="35"/>
+    </row>
+    <row r="255" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A255" t="s">
+        <v>748</v>
+      </c>
+      <c r="B255" s="3" t="s">
+        <v>820</v>
+      </c>
+      <c r="C255" t="s">
+        <v>738</v>
+      </c>
+      <c r="D255" s="41" t="s">
+        <v>776</v>
+      </c>
+      <c r="E255" t="s">
+        <v>735</v>
+      </c>
+      <c r="F255" s="35" t="s">
+        <v>274</v>
+      </c>
+      <c r="G255" s="36"/>
+      <c r="K255" s="35"/>
+    </row>
+    <row r="256" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A256" t="s">
+        <v>749</v>
+      </c>
+      <c r="B256" s="42" t="s">
+        <v>776</v>
+      </c>
+      <c r="C256" t="s">
+        <v>738</v>
+      </c>
+      <c r="D256" s="3" t="s">
+        <v>755</v>
+      </c>
+      <c r="E256" t="s">
+        <v>735</v>
+      </c>
+      <c r="F256" s="35"/>
+      <c r="G256" s="36"/>
+      <c r="K256" s="35"/>
+    </row>
+    <row r="257" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A257" t="s">
+        <v>750</v>
+      </c>
+      <c r="B257" s="3" t="s">
+        <v>751</v>
+      </c>
+      <c r="C257" t="s">
+        <v>256</v>
+      </c>
+      <c r="D257" s="42" t="s">
+        <v>776</v>
+      </c>
+      <c r="E257" t="s">
+        <v>721</v>
+      </c>
+      <c r="F257" s="35" t="s">
+        <v>752</v>
+      </c>
+      <c r="G257" s="36"/>
+      <c r="K257" s="35"/>
+    </row>
+    <row r="258" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A258" t="s">
+        <v>836</v>
+      </c>
+      <c r="B258" s="3" t="s">
+        <v>754</v>
+      </c>
+      <c r="C258" t="s">
+        <v>753</v>
+      </c>
+      <c r="D258" s="3" t="s">
+        <v>835</v>
+      </c>
+      <c r="E258" t="s">
+        <v>753</v>
+      </c>
+      <c r="F258" s="35" t="s">
+        <v>753</v>
+      </c>
+      <c r="G258" s="36"/>
+      <c r="K258" s="35"/>
+    </row>
+    <row r="259" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A259" t="s">
+        <v>775</v>
+      </c>
+      <c r="B259" s="3" t="s">
+        <v>835</v>
+      </c>
+      <c r="C259" t="s">
+        <v>256</v>
+      </c>
+      <c r="D259" s="42" t="s">
+        <v>776</v>
+      </c>
+      <c r="E259" t="s">
+        <v>721</v>
+      </c>
+      <c r="F259" s="35"/>
+      <c r="G259" s="36"/>
+      <c r="K259" s="35"/>
+    </row>
+    <row r="260" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A260" t="s">
+        <v>781</v>
+      </c>
+      <c r="B260" s="3" t="s">
+        <v>765</v>
+      </c>
+      <c r="C260" t="s">
+        <v>738</v>
+      </c>
+      <c r="D260" s="3" t="s">
+        <v>766</v>
+      </c>
+      <c r="E260" t="s">
+        <v>735</v>
+      </c>
+      <c r="F260" s="35" t="s">
+        <v>747</v>
+      </c>
+      <c r="G260" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="H260" t="s">
+        <v>133</v>
+      </c>
+      <c r="K260" s="35"/>
+    </row>
+    <row r="261" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A261" t="s">
+        <v>774</v>
+      </c>
+      <c r="B261" s="3" t="s">
+        <v>755</v>
+      </c>
+      <c r="C261" t="s">
+        <v>756</v>
+      </c>
+      <c r="D261" s="3" t="s">
+        <v>760</v>
+      </c>
+      <c r="E261" t="s">
+        <v>735</v>
+      </c>
+      <c r="F261" s="35"/>
+      <c r="G261" s="36"/>
+      <c r="K261" s="35"/>
+    </row>
+    <row r="262" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A262" t="s">
+        <v>773</v>
+      </c>
+      <c r="B262" s="3" t="s">
+        <v>755</v>
+      </c>
+      <c r="C262" t="s">
+        <v>757</v>
+      </c>
+      <c r="D262" s="3" t="s">
+        <v>761</v>
+      </c>
+      <c r="E262" t="s">
+        <v>735</v>
+      </c>
+      <c r="F262" s="35"/>
+      <c r="G262" s="36"/>
+      <c r="K262" s="35"/>
+    </row>
+    <row r="263" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A263" s="37" t="s">
+        <v>772</v>
+      </c>
+      <c r="B263" s="3" t="s">
+        <v>755</v>
+      </c>
+      <c r="C263" s="37" t="s">
+        <v>762</v>
+      </c>
+      <c r="D263" s="38" t="s">
+        <v>763</v>
+      </c>
+      <c r="E263" s="37" t="s">
+        <v>735</v>
+      </c>
+      <c r="F263" s="39"/>
+      <c r="G263" s="40"/>
+      <c r="H263" s="37"/>
+      <c r="I263" s="37"/>
+      <c r="J263" s="37"/>
+      <c r="K263" s="39"/>
+      <c r="L263" s="37"/>
+    </row>
+    <row r="264" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A264" t="s">
+        <v>778</v>
+      </c>
+      <c r="B264" s="3" t="s">
+        <v>755</v>
+      </c>
+      <c r="C264" t="s">
+        <v>777</v>
+      </c>
+      <c r="D264" s="3" t="s">
+        <v>764</v>
+      </c>
+      <c r="E264" s="37" t="s">
+        <v>735</v>
+      </c>
+      <c r="F264" s="35" t="s">
+        <v>747</v>
+      </c>
+      <c r="G264" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="H264" t="s">
+        <v>133</v>
+      </c>
+      <c r="K264" s="35"/>
+    </row>
+    <row r="265" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A265" t="s">
+        <v>779</v>
+      </c>
+      <c r="B265" s="3" t="s">
+        <v>764</v>
+      </c>
+      <c r="C265" t="s">
+        <v>738</v>
+      </c>
+      <c r="D265" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="E265" s="37" t="s">
+        <v>735</v>
+      </c>
+      <c r="F265" s="35" t="s">
+        <v>747</v>
+      </c>
+      <c r="G265" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="H265" t="s">
+        <v>133</v>
+      </c>
+      <c r="K265" s="35"/>
+    </row>
+    <row r="266" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A266" t="s">
+        <v>780</v>
+      </c>
+      <c r="B266" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="C266" t="s">
+        <v>738</v>
+      </c>
+      <c r="D266" s="3" t="s">
+        <v>765</v>
+      </c>
+      <c r="E266" s="37" t="s">
+        <v>735</v>
+      </c>
+      <c r="F266" s="35" t="s">
+        <v>747</v>
+      </c>
+      <c r="G266" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="H266" t="s">
+        <v>133</v>
+      </c>
+      <c r="K266" s="35"/>
+    </row>
+    <row r="267" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A267" t="s">
+        <v>771</v>
+      </c>
+      <c r="B267" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C267" t="s">
+        <v>72</v>
+      </c>
+      <c r="D267" s="3" t="s">
+        <v>767</v>
+      </c>
+      <c r="E267" t="s">
+        <v>768</v>
+      </c>
+      <c r="F267" s="35"/>
+      <c r="G267" s="36"/>
+      <c r="K267" s="35"/>
+    </row>
+    <row r="268" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A268" t="s">
+        <v>770</v>
+      </c>
+      <c r="B268" s="3" t="s">
+        <v>767</v>
+      </c>
+      <c r="C268" t="s">
+        <v>768</v>
+      </c>
+      <c r="D268" s="3" t="s">
+        <v>769</v>
+      </c>
+      <c r="E268" t="s">
+        <v>768</v>
+      </c>
+      <c r="F268" s="35"/>
+      <c r="G268" s="36"/>
+      <c r="K268" s="35"/>
+    </row>
+    <row r="269" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A269" t="s">
+        <v>783</v>
+      </c>
+      <c r="B269" s="3" t="s">
+        <v>755</v>
+      </c>
+      <c r="C269" t="s">
+        <v>782</v>
+      </c>
+      <c r="D269" s="3" t="s">
+        <v>784</v>
+      </c>
+      <c r="E269" t="s">
+        <v>747</v>
+      </c>
+      <c r="F269" s="35" t="s">
+        <v>747</v>
+      </c>
+      <c r="G269" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="H269" t="s">
+        <v>133</v>
+      </c>
+      <c r="I269" t="s">
+        <v>759</v>
+      </c>
+      <c r="K269" s="35"/>
+    </row>
+    <row r="270" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A270" t="s">
+        <v>784</v>
+      </c>
+      <c r="B270" t="s">
+        <v>784</v>
+      </c>
+      <c r="C270" t="s">
+        <v>747</v>
+      </c>
+      <c r="D270" s="3" t="s">
+        <v>759</v>
+      </c>
+      <c r="E270" t="s">
+        <v>747</v>
+      </c>
+      <c r="F270" s="35" t="s">
+        <v>747</v>
+      </c>
+      <c r="G270" s="36"/>
+      <c r="J270" t="s">
+        <v>785</v>
+      </c>
+      <c r="K270" s="35"/>
+    </row>
+    <row r="271" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A271" t="s">
+        <v>787</v>
+      </c>
+      <c r="B271" s="3" t="s">
+        <v>755</v>
+      </c>
+      <c r="C271" t="s">
+        <v>786</v>
+      </c>
+      <c r="D271" s="3" t="s">
+        <v>788</v>
+      </c>
+      <c r="E271" t="s">
+        <v>747</v>
+      </c>
+      <c r="F271" s="35" t="s">
+        <v>747</v>
+      </c>
+      <c r="G271" s="36"/>
+      <c r="K271" s="35"/>
+    </row>
+    <row r="272" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A272" t="s">
+        <v>801</v>
+      </c>
+      <c r="B272" s="3" t="s">
+        <v>755</v>
+      </c>
+      <c r="C272" t="s">
+        <v>789</v>
+      </c>
+      <c r="D272" s="3" t="s">
+        <v>795</v>
+      </c>
+      <c r="E272" t="s">
+        <v>747</v>
+      </c>
+      <c r="F272" s="35" t="s">
+        <v>747</v>
+      </c>
+      <c r="G272" s="36"/>
+      <c r="K272" s="35"/>
+    </row>
+    <row r="273" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A273" t="s">
+        <v>802</v>
+      </c>
+      <c r="B273" s="3" t="s">
+        <v>755</v>
+      </c>
+      <c r="C273" t="s">
+        <v>794</v>
+      </c>
+      <c r="D273" s="3" t="s">
+        <v>796</v>
+      </c>
+      <c r="E273" t="s">
+        <v>747</v>
+      </c>
+      <c r="F273" s="35" t="s">
+        <v>747</v>
+      </c>
+      <c r="G273" s="36"/>
+      <c r="K273" s="35"/>
+    </row>
+    <row r="274" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A274" t="s">
+        <v>803</v>
+      </c>
+      <c r="B274" s="3" t="s">
+        <v>755</v>
+      </c>
+      <c r="C274" t="s">
+        <v>790</v>
+      </c>
+      <c r="D274" s="3" t="s">
+        <v>797</v>
+      </c>
+      <c r="E274" t="s">
+        <v>747</v>
+      </c>
+      <c r="F274" s="35" t="s">
+        <v>747</v>
+      </c>
+      <c r="G274" s="36"/>
+      <c r="K274" s="35"/>
+    </row>
+    <row r="275" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A275" t="s">
+        <v>804</v>
+      </c>
+      <c r="B275" s="3" t="s">
+        <v>755</v>
+      </c>
+      <c r="C275" t="s">
+        <v>791</v>
+      </c>
+      <c r="D275" s="3" t="s">
+        <v>798</v>
+      </c>
+      <c r="E275" t="s">
+        <v>747</v>
+      </c>
+      <c r="F275" s="35" t="s">
+        <v>747</v>
+      </c>
+      <c r="G275" s="36"/>
+      <c r="K275" s="35"/>
+    </row>
+    <row r="276" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A276" t="s">
+        <v>805</v>
+      </c>
+      <c r="B276" s="3" t="s">
+        <v>755</v>
+      </c>
+      <c r="C276" t="s">
+        <v>792</v>
+      </c>
+      <c r="D276" s="3" t="s">
+        <v>799</v>
+      </c>
+      <c r="E276" t="s">
+        <v>747</v>
+      </c>
+      <c r="F276" s="35" t="s">
+        <v>747</v>
+      </c>
+      <c r="G276" s="36"/>
+      <c r="K276" s="35"/>
+    </row>
+    <row r="277" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A277" t="s">
+        <v>806</v>
+      </c>
+      <c r="B277" s="3" t="s">
+        <v>755</v>
+      </c>
+      <c r="C277" t="s">
+        <v>793</v>
+      </c>
+      <c r="D277" s="3" t="s">
+        <v>800</v>
+      </c>
+      <c r="E277" t="s">
+        <v>747</v>
+      </c>
+      <c r="F277" s="35" t="s">
+        <v>747</v>
+      </c>
+      <c r="G277" s="36"/>
+      <c r="K277" s="35"/>
+    </row>
+    <row r="278" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A278" t="s">
+        <v>817</v>
+      </c>
+      <c r="B278" s="3" t="s">
+        <v>811</v>
+      </c>
+      <c r="C278" t="s">
+        <v>738</v>
+      </c>
+      <c r="D278" s="3" t="s">
+        <v>818</v>
+      </c>
+      <c r="E278" t="s">
+        <v>747</v>
+      </c>
+      <c r="F278" s="35" t="s">
+        <v>819</v>
+      </c>
+      <c r="G278" s="36" t="s">
+        <v>815</v>
+      </c>
+      <c r="K278" s="35"/>
+    </row>
+    <row r="279" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A279" t="s">
+        <v>818</v>
+      </c>
+      <c r="B279" t="s">
+        <v>817</v>
+      </c>
+      <c r="D279" s="3" t="s">
+        <v>820</v>
+      </c>
+      <c r="E279" t="s">
+        <v>747</v>
+      </c>
+      <c r="F279" s="35" t="s">
+        <v>747</v>
+      </c>
+      <c r="G279" s="36" t="s">
+        <v>403</v>
+      </c>
+      <c r="K279" s="35"/>
+    </row>
+    <row r="280" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F280" s="35"/>
+      <c r="G280" s="36"/>
+      <c r="I280" t="s">
+        <v>831</v>
+      </c>
+      <c r="K280" s="35"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Updated inventory of video cables
</commit_message>
<xml_diff>
--- a/data/uac_cables.xlsx
+++ b/data/uac_cables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/donert/Documents/UACTech/SystemDocumentation/github/uactechdoc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33849117-E40E-AC4F-AD99-D91B3DEB4365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375F27D2-6F3E-3345-A3CD-33A91F62CB80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-53660" yWindow="-31600" windowWidth="51200" windowHeight="36160" xr2:uid="{288904EE-D384-EA4C-9B98-052B972FB267}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{288904EE-D384-EA4C-9B98-052B972FB267}"/>
   </bookViews>
   <sheets>
     <sheet name="Cables" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2071" uniqueCount="837">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2132" uniqueCount="860">
   <si>
     <t>Tag</t>
   </si>
@@ -2001,9 +2001,6 @@
     <t>Matrix Communications circa 2018</t>
   </si>
   <si>
-    <t>2309-xxxx</t>
-  </si>
-  <si>
     <t>30.4m</t>
   </si>
   <si>
@@ -2551,6 +2548,78 @@
   </si>
   <si>
     <t>2310-0502</t>
+  </si>
+  <si>
+    <t>2310-0900</t>
+  </si>
+  <si>
+    <t>55m</t>
+  </si>
+  <si>
+    <t>2310-0901</t>
+  </si>
+  <si>
+    <t>60m</t>
+  </si>
+  <si>
+    <t>2310-0902</t>
+  </si>
+  <si>
+    <t>18m</t>
+  </si>
+  <si>
+    <t>2310-0903</t>
+  </si>
+  <si>
+    <t>2310-0904</t>
+  </si>
+  <si>
+    <t>2310-0905</t>
+  </si>
+  <si>
+    <t>13m</t>
+  </si>
+  <si>
+    <t>7.5m</t>
+  </si>
+  <si>
+    <t>4.6m</t>
+  </si>
+  <si>
+    <t>2310-0906</t>
+  </si>
+  <si>
+    <t>2310-0907</t>
+  </si>
+  <si>
+    <t>2310-0908</t>
+  </si>
+  <si>
+    <t>30.5m</t>
+  </si>
+  <si>
+    <t>belden 1694f</t>
+  </si>
+  <si>
+    <t>2310-1000</t>
+  </si>
+  <si>
+    <t>16m</t>
+  </si>
+  <si>
+    <t>Small nick in jacket under red tape</t>
+  </si>
+  <si>
+    <t>2310-1001</t>
+  </si>
+  <si>
+    <t>2310-1002</t>
+  </si>
+  <si>
+    <t>dmx3f5m</t>
+  </si>
+  <si>
+    <t>2310-1003</t>
   </si>
 </sst>
 </file>
@@ -4869,8 +4938,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD7E3698-8860-904B-8BDB-00EF1039C49C}" name="Table1" displayName="Table1" ref="A1:L279" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="5">
-  <autoFilter ref="A1:L279" xr:uid="{BD7E3698-8860-904B-8BDB-00EF1039C49C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD7E3698-8860-904B-8BDB-00EF1039C49C}" name="Table1" displayName="Table1" ref="A1:L278" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="5">
+  <autoFilter ref="A1:L278" xr:uid="{BD7E3698-8860-904B-8BDB-00EF1039C49C}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{4D442337-BE86-B24A-84A4-338FB80A6A49}" name="Tag"/>
     <tableColumn id="2" xr3:uid="{74A36D7B-C989-3B4B-B1E5-AB1FA4C2DD45}" name="SrcTag" dataDxfId="4"/>
@@ -5186,13 +5255,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B91ADC-4569-1C4E-B002-1ED2E647C959}">
-  <dimension ref="A1:L280"/>
+  <dimension ref="A1:L290"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="310" zoomScaleNormal="310" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B238" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F258" sqref="F258"/>
+      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5469,14 +5538,16 @@
         <v>9</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>377</v>
+        <v>619</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="12"/>
       <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
+      <c r="F8" s="13" t="s">
+        <v>35</v>
+      </c>
       <c r="G8" s="13" t="s">
-        <v>48</v>
+        <v>244</v>
       </c>
       <c r="H8" s="13" t="s">
         <v>133</v>
@@ -5486,7 +5557,7 @@
       <c r="K8" s="13"/>
       <c r="L8" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>not used: -&gt; : [label='2307-1806']</v>
+        <v>unused: -&gt; : [label='2307-1806']</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -6550,7 +6621,7 @@
         <v>133</v>
       </c>
       <c r="I40" s="13" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="J40" s="13" t="s">
         <v>281</v>
@@ -8338,7 +8409,7 @@
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A93" s="11" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B93" s="12"/>
       <c r="C93" s="13"/>
@@ -8356,7 +8427,7 @@
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A94" s="15" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B94" s="16"/>
       <c r="C94" s="17"/>
@@ -8374,7 +8445,7 @@
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A95" s="11" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B95" s="12" t="s">
         <v>255</v>
@@ -8417,7 +8488,7 @@
         <v>255</v>
       </c>
       <c r="E96" s="17" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="F96" s="17" t="s">
         <v>181</v>
@@ -8438,7 +8509,7 @@
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A97" s="11" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B97" s="12" t="s">
         <v>171</v>
@@ -8450,7 +8521,7 @@
         <v>255</v>
       </c>
       <c r="E97" s="13" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="F97" s="13" t="s">
         <v>181</v>
@@ -8469,7 +8540,7 @@
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A98" s="15" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B98" s="16" t="s">
         <v>171</v>
@@ -8481,7 +8552,7 @@
         <v>255</v>
       </c>
       <c r="E98" s="17" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="F98" s="17" t="s">
         <v>181</v>
@@ -8510,7 +8581,7 @@
         <v>255</v>
       </c>
       <c r="E99" s="13" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="F99" s="13" t="s">
         <v>181</v>
@@ -8539,7 +8610,7 @@
         <v>255</v>
       </c>
       <c r="E100" s="17" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="F100" s="17" t="s">
         <v>181</v>
@@ -9468,8 +9539,8 @@
       <c r="A129" s="15" t="s">
         <v>393</v>
       </c>
-      <c r="B129" s="16" t="s">
-        <v>377</v>
+      <c r="B129" s="3" t="s">
+        <v>619</v>
       </c>
       <c r="C129" s="17"/>
       <c r="D129" s="16"/>
@@ -9486,7 +9557,7 @@
       <c r="K129" s="17"/>
       <c r="L129" s="18" t="str">
         <f t="shared" si="5"/>
-        <v>not used: -&gt; : [label='2308-2702']</v>
+        <v>unused: -&gt; : [label='2308-2702']</v>
       </c>
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.2">
@@ -11699,7 +11770,7 @@
         <v>35</v>
       </c>
       <c r="G213" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="H213" s="3" t="s">
         <v>85</v>
@@ -11858,7 +11929,7 @@
     </row>
     <row r="220" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>653</v>
+        <v>843</v>
       </c>
       <c r="B220" s="3" t="s">
         <v>619</v>
@@ -11867,13 +11938,13 @@
         <v>35</v>
       </c>
       <c r="G220" t="s">
+        <v>653</v>
+      </c>
+      <c r="H220" t="s">
+        <v>133</v>
+      </c>
+      <c r="J220" s="3" t="s">
         <v>654</v>
-      </c>
-      <c r="H220" t="s">
-        <v>85</v>
-      </c>
-      <c r="J220" s="3" t="s">
-        <v>655</v>
       </c>
       <c r="K220" s="3" t="s">
         <v>631</v>
@@ -11881,22 +11952,22 @@
     </row>
     <row r="221" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B221" s="3" t="s">
         <v>172</v>
       </c>
       <c r="C221" t="s">
+        <v>658</v>
+      </c>
+      <c r="D221" s="3" t="s">
         <v>659</v>
       </c>
-      <c r="D221" s="3" t="s">
+      <c r="E221" t="s">
         <v>660</v>
       </c>
-      <c r="E221" t="s">
-        <v>661</v>
-      </c>
       <c r="F221" s="3" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="G221" t="s">
         <v>244</v>
@@ -11905,28 +11976,28 @@
         <v>133</v>
       </c>
       <c r="J221" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="K221" s="3"/>
     </row>
     <row r="222" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
+        <v>661</v>
+      </c>
+      <c r="B222" s="3" t="s">
+        <v>659</v>
+      </c>
+      <c r="C222" t="s">
         <v>662</v>
       </c>
-      <c r="B222" s="3" t="s">
-        <v>660</v>
-      </c>
-      <c r="C222" t="s">
-        <v>663</v>
-      </c>
       <c r="D222" s="3" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="E222" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="F222" s="3" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="G222" t="s">
         <v>214</v>
@@ -11935,28 +12006,28 @@
         <v>133</v>
       </c>
       <c r="I222" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="K222" s="3"/>
     </row>
     <row r="223" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B223" s="3" t="s">
         <v>255</v>
       </c>
       <c r="C223" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="D223" s="3" t="s">
         <v>206</v>
       </c>
       <c r="E223" t="s">
+        <v>666</v>
+      </c>
+      <c r="F223" s="3" t="s">
         <v>667</v>
-      </c>
-      <c r="F223" s="3" t="s">
-        <v>668</v>
       </c>
       <c r="G223" t="s">
         <v>34</v>
@@ -11968,22 +12039,22 @@
     </row>
     <row r="224" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B224" s="3" t="s">
         <v>255</v>
       </c>
       <c r="C224" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="D224" s="3" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="E224" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="F224" s="3" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="G224" t="s">
         <v>34</v>
@@ -11995,22 +12066,22 @@
     </row>
     <row r="225" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B225" s="3" t="s">
         <v>255</v>
       </c>
       <c r="C225" t="s">
+        <v>671</v>
+      </c>
+      <c r="D225" s="3" t="s">
         <v>672</v>
       </c>
-      <c r="D225" s="3" t="s">
-        <v>673</v>
-      </c>
       <c r="E225" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="F225" s="3" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="G225" t="s">
         <v>34</v>
@@ -12022,22 +12093,22 @@
     </row>
     <row r="226" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B226" s="3" t="s">
         <v>255</v>
       </c>
       <c r="C226" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="D226" s="3" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="E226" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="F226" s="3" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="G226" t="s">
         <v>394</v>
@@ -12052,22 +12123,22 @@
     </row>
     <row r="227" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B227" s="3" t="s">
         <v>255</v>
       </c>
       <c r="C227" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="D227" s="3" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="E227" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="F227" s="3" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="G227" t="s">
         <v>394</v>
@@ -12082,22 +12153,22 @@
     </row>
     <row r="228" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B228" s="3" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="C228" t="s">
         <v>256</v>
       </c>
       <c r="D228" s="3" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="E228" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="F228" s="3" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="G228" t="s">
         <v>34</v>
@@ -12109,22 +12180,22 @@
     </row>
     <row r="229" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B229" s="3" t="s">
+        <v>681</v>
+      </c>
+      <c r="C229" t="s">
+        <v>662</v>
+      </c>
+      <c r="D229" s="3" t="s">
         <v>682</v>
       </c>
-      <c r="C229" t="s">
-        <v>663</v>
-      </c>
-      <c r="D229" s="3" t="s">
-        <v>683</v>
-      </c>
       <c r="E229" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="F229" s="3" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="G229" t="s">
         <v>214</v>
@@ -12136,22 +12207,22 @@
     </row>
     <row r="230" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
+        <v>685</v>
+      </c>
+      <c r="B230" s="3" t="s">
         <v>686</v>
-      </c>
-      <c r="B230" s="3" t="s">
-        <v>687</v>
       </c>
       <c r="C230" t="s">
         <v>256</v>
       </c>
       <c r="D230" s="3" t="s">
+        <v>659</v>
+      </c>
+      <c r="E230" t="s">
         <v>660</v>
       </c>
-      <c r="E230" t="s">
-        <v>661</v>
-      </c>
       <c r="F230" s="3" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="G230" t="s">
         <v>34</v>
@@ -12163,25 +12234,25 @@
     </row>
     <row r="231" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C231" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="D231" s="3" t="s">
         <v>255</v>
       </c>
       <c r="E231" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="F231" s="3" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="G231" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="H231" t="s">
         <v>85</v>
@@ -12190,25 +12261,25 @@
     </row>
     <row r="232" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C232" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="D232" s="3" t="s">
         <v>255</v>
       </c>
       <c r="E232" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="F232" s="3" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="G232" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="H232" t="s">
         <v>85</v>
@@ -12217,25 +12288,25 @@
     </row>
     <row r="233" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="C233" t="s">
+        <v>688</v>
+      </c>
+      <c r="D233" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="E233" t="s">
+        <v>712</v>
+      </c>
+      <c r="F233" s="3" t="s">
         <v>689</v>
       </c>
-      <c r="D233" s="3" t="s">
-        <v>683</v>
-      </c>
-      <c r="E233" t="s">
-        <v>713</v>
-      </c>
-      <c r="F233" s="3" t="s">
-        <v>690</v>
-      </c>
       <c r="G233" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="H233" t="s">
         <v>85</v>
@@ -12244,25 +12315,25 @@
     </row>
     <row r="234" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="C234" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="D234" s="3" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="E234" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="F234" s="3" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="G234" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="H234" t="s">
         <v>85</v>
@@ -12271,22 +12342,22 @@
     </row>
     <row r="235" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D235" s="3" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="E235" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="F235" s="3" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="G235" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="H235" t="s">
         <v>85</v>
@@ -12295,293 +12366,293 @@
     </row>
     <row r="236" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="C236" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="D236" s="3" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="E236" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="F236" s="3"/>
       <c r="K236" s="3"/>
     </row>
     <row r="237" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
+        <v>716</v>
+      </c>
+      <c r="B237" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="C237" t="s">
+        <v>715</v>
+      </c>
+      <c r="D237" s="3" t="s">
         <v>717</v>
       </c>
-      <c r="B237" s="3" t="s">
-        <v>683</v>
-      </c>
-      <c r="C237" t="s">
-        <v>716</v>
-      </c>
-      <c r="D237" s="3" t="s">
-        <v>718</v>
-      </c>
       <c r="E237" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="F237" s="3"/>
       <c r="K237" s="3"/>
     </row>
     <row r="238" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
+        <v>719</v>
+      </c>
+      <c r="B238" s="3" t="s">
+        <v>710</v>
+      </c>
+      <c r="C238" t="s">
+        <v>691</v>
+      </c>
+      <c r="D238" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="E238" t="s">
         <v>720</v>
-      </c>
-      <c r="B238" s="3" t="s">
-        <v>711</v>
-      </c>
-      <c r="C238" t="s">
-        <v>692</v>
-      </c>
-      <c r="D238" s="3" t="s">
-        <v>719</v>
-      </c>
-      <c r="E238" t="s">
-        <v>721</v>
       </c>
       <c r="F238" s="3"/>
       <c r="K238" s="3"/>
     </row>
     <row r="239" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C239" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="D239" s="3" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="E239" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="F239" s="3"/>
       <c r="K239" s="3"/>
     </row>
     <row r="240" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
+        <v>724</v>
+      </c>
+      <c r="B240" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="C240" t="s">
+        <v>722</v>
+      </c>
+      <c r="D240" s="3" t="s">
         <v>725</v>
       </c>
-      <c r="B240" s="3" t="s">
-        <v>683</v>
-      </c>
-      <c r="C240" t="s">
-        <v>723</v>
-      </c>
-      <c r="D240" s="3" t="s">
-        <v>726</v>
-      </c>
       <c r="E240" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="F240" s="3"/>
       <c r="K240" s="3"/>
     </row>
     <row r="241" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B241" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C241" t="s">
+        <v>728</v>
+      </c>
+      <c r="F241" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H241" t="s">
         <v>729</v>
       </c>
-      <c r="F241" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H241" t="s">
+      <c r="I241" t="s">
         <v>730</v>
-      </c>
-      <c r="I241" t="s">
-        <v>731</v>
       </c>
       <c r="K241" s="3"/>
     </row>
     <row r="242" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B242" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="C242" t="s">
         <v>732</v>
       </c>
-      <c r="C242" t="s">
+      <c r="D242" s="3" t="s">
         <v>733</v>
       </c>
-      <c r="D242" s="3" t="s">
+      <c r="E242" t="s">
         <v>734</v>
       </c>
-      <c r="E242" t="s">
+      <c r="F242" s="3" t="s">
         <v>735</v>
-      </c>
-      <c r="F242" s="3" t="s">
-        <v>736</v>
       </c>
       <c r="G242" t="s">
         <v>34</v>
       </c>
       <c r="H242" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="K242" s="3"/>
     </row>
     <row r="243" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="D243" s="3" t="s">
+        <v>736</v>
+      </c>
+      <c r="E243" t="s">
         <v>737</v>
       </c>
-      <c r="E243" t="s">
+      <c r="F243" s="3" t="s">
         <v>738</v>
-      </c>
-      <c r="F243" s="3" t="s">
-        <v>739</v>
       </c>
       <c r="K243" s="3"/>
     </row>
     <row r="244" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B244" s="3" t="s">
+        <v>736</v>
+      </c>
+      <c r="C244" t="s">
+        <v>734</v>
+      </c>
+      <c r="D244" s="3" t="s">
+        <v>739</v>
+      </c>
+      <c r="E244" t="s">
         <v>737</v>
       </c>
-      <c r="C244" t="s">
-        <v>735</v>
-      </c>
-      <c r="D244" s="3" t="s">
-        <v>740</v>
-      </c>
-      <c r="E244" t="s">
+      <c r="F244" s="3" t="s">
         <v>738</v>
-      </c>
-      <c r="F244" s="3" t="s">
-        <v>739</v>
       </c>
       <c r="K244" s="3"/>
     </row>
     <row r="245" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B245" s="3" t="s">
+        <v>739</v>
+      </c>
+      <c r="C245" t="s">
+        <v>734</v>
+      </c>
+      <c r="D245" s="3" t="s">
         <v>740</v>
       </c>
-      <c r="C245" t="s">
-        <v>735</v>
-      </c>
-      <c r="D245" s="3" t="s">
-        <v>741</v>
-      </c>
       <c r="E245" t="s">
+        <v>737</v>
+      </c>
+      <c r="F245" s="3" t="s">
         <v>738</v>
-      </c>
-      <c r="F245" s="3" t="s">
-        <v>739</v>
       </c>
       <c r="K245" s="3"/>
     </row>
     <row r="246" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="C246" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="D246" s="3" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="E246" t="s">
+        <v>737</v>
+      </c>
+      <c r="F246" s="3" t="s">
         <v>738</v>
-      </c>
-      <c r="F246" s="3" t="s">
-        <v>739</v>
       </c>
       <c r="K246" s="3"/>
     </row>
     <row r="247" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C247" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="D247" s="3" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="E247" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="F247" s="35" t="s">
         <v>293</v>
       </c>
       <c r="G247" s="36"/>
       <c r="I247" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K247" s="35"/>
     </row>
     <row r="248" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C248" t="s">
         <v>256</v>
       </c>
       <c r="D248" s="3" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="E248" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="F248" s="35" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="G248" s="36"/>
       <c r="I248" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K248" s="35"/>
     </row>
     <row r="249" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A249" s="3" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="C249" t="s">
         <v>256</v>
       </c>
       <c r="D249" s="3" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="E249" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="F249" s="35" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="G249" s="36">
         <v>0</v>
@@ -12590,138 +12661,158 @@
         <v>133</v>
       </c>
       <c r="I249" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="K249" s="35"/>
     </row>
     <row r="250" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
+        <v>821</v>
+      </c>
+      <c r="B250" s="3" t="s">
         <v>822</v>
-      </c>
-      <c r="B250" s="3" t="s">
-        <v>823</v>
       </c>
       <c r="C250" t="s">
         <v>256</v>
       </c>
       <c r="D250" s="3" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="E250" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="F250" s="35" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="G250" s="36" t="s">
         <v>403</v>
       </c>
       <c r="I250" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="K250" s="35"/>
     </row>
     <row r="251" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C251" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="D251" s="3" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="E251" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="F251" s="35" t="s">
         <v>293</v>
       </c>
       <c r="G251" s="36"/>
       <c r="I251" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="K251" s="35"/>
     </row>
     <row r="252" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C252" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="D252" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="E252" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="F252" s="35" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="G252" s="36" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="H252" t="s">
         <v>133</v>
       </c>
       <c r="J252" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="K252" s="35"/>
     </row>
     <row r="253" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="B253" t="s">
+        <v>809</v>
+      </c>
+      <c r="C253" t="s">
+        <v>746</v>
+      </c>
+      <c r="D253" s="3" t="s">
         <v>810</v>
       </c>
-      <c r="C253" t="s">
-        <v>747</v>
-      </c>
-      <c r="D253" s="3" t="s">
-        <v>811</v>
-      </c>
       <c r="E253" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="F253" s="35" t="s">
+        <v>813</v>
+      </c>
+      <c r="G253" s="36" t="s">
         <v>814</v>
-      </c>
-      <c r="G253" s="36" t="s">
-        <v>815</v>
       </c>
       <c r="H253" t="s">
         <v>133</v>
       </c>
       <c r="K253" s="35"/>
+    </row>
+    <row r="254" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A254" t="s">
+        <v>747</v>
+      </c>
+      <c r="B254" s="3" t="s">
+        <v>819</v>
+      </c>
+      <c r="C254" t="s">
+        <v>737</v>
+      </c>
+      <c r="D254" s="41" t="s">
+        <v>775</v>
+      </c>
+      <c r="E254" t="s">
+        <v>734</v>
+      </c>
+      <c r="F254" s="35" t="s">
+        <v>274</v>
+      </c>
+      <c r="G254" s="36"/>
+      <c r="K254" s="35"/>
     </row>
     <row r="255" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>748</v>
       </c>
-      <c r="B255" s="3" t="s">
-        <v>820</v>
+      <c r="B255" s="42" t="s">
+        <v>775</v>
       </c>
       <c r="C255" t="s">
-        <v>738</v>
-      </c>
-      <c r="D255" s="41" t="s">
-        <v>776</v>
+        <v>737</v>
+      </c>
+      <c r="D255" s="3" t="s">
+        <v>754</v>
       </c>
       <c r="E255" t="s">
-        <v>735</v>
-      </c>
-      <c r="F255" s="35" t="s">
-        <v>274</v>
-      </c>
+        <v>734</v>
+      </c>
+      <c r="F255" s="35"/>
       <c r="G255" s="36"/>
       <c r="K255" s="35"/>
     </row>
@@ -12729,37 +12820,39 @@
       <c r="A256" t="s">
         <v>749</v>
       </c>
-      <c r="B256" s="42" t="s">
-        <v>776</v>
+      <c r="B256" s="3" t="s">
+        <v>750</v>
       </c>
       <c r="C256" t="s">
-        <v>738</v>
-      </c>
-      <c r="D256" s="3" t="s">
-        <v>755</v>
+        <v>256</v>
+      </c>
+      <c r="D256" s="42" t="s">
+        <v>775</v>
       </c>
       <c r="E256" t="s">
-        <v>735</v>
-      </c>
-      <c r="F256" s="35"/>
+        <v>720</v>
+      </c>
+      <c r="F256" s="35" t="s">
+        <v>751</v>
+      </c>
       <c r="G256" s="36"/>
       <c r="K256" s="35"/>
     </row>
     <row r="257" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>750</v>
+        <v>835</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="C257" t="s">
-        <v>256</v>
-      </c>
-      <c r="D257" s="42" t="s">
-        <v>776</v>
+        <v>752</v>
+      </c>
+      <c r="D257" s="3" t="s">
+        <v>834</v>
       </c>
       <c r="E257" t="s">
-        <v>721</v>
+        <v>752</v>
       </c>
       <c r="F257" s="35" t="s">
         <v>752</v>
@@ -12769,79 +12862,77 @@
     </row>
     <row r="258" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>836</v>
+        <v>774</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>754</v>
+        <v>834</v>
       </c>
       <c r="C258" t="s">
-        <v>753</v>
-      </c>
-      <c r="D258" s="3" t="s">
-        <v>835</v>
+        <v>256</v>
+      </c>
+      <c r="D258" s="42" t="s">
+        <v>775</v>
       </c>
       <c r="E258" t="s">
-        <v>753</v>
-      </c>
-      <c r="F258" s="35" t="s">
-        <v>753</v>
-      </c>
+        <v>720</v>
+      </c>
+      <c r="F258" s="35"/>
       <c r="G258" s="36"/>
       <c r="K258" s="35"/>
     </row>
     <row r="259" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>775</v>
+        <v>780</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>835</v>
+        <v>764</v>
       </c>
       <c r="C259" t="s">
-        <v>256</v>
-      </c>
-      <c r="D259" s="42" t="s">
-        <v>776</v>
+        <v>737</v>
+      </c>
+      <c r="D259" s="3" t="s">
+        <v>765</v>
       </c>
       <c r="E259" t="s">
-        <v>721</v>
-      </c>
-      <c r="F259" s="35"/>
-      <c r="G259" s="36"/>
+        <v>734</v>
+      </c>
+      <c r="F259" s="35" t="s">
+        <v>746</v>
+      </c>
+      <c r="G259" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="H259" t="s">
+        <v>133</v>
+      </c>
       <c r="K259" s="35"/>
     </row>
     <row r="260" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>781</v>
+        <v>773</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>765</v>
+        <v>754</v>
       </c>
       <c r="C260" t="s">
-        <v>738</v>
+        <v>755</v>
       </c>
       <c r="D260" s="3" t="s">
-        <v>766</v>
+        <v>759</v>
       </c>
       <c r="E260" t="s">
-        <v>735</v>
-      </c>
-      <c r="F260" s="35" t="s">
-        <v>747</v>
-      </c>
-      <c r="G260" s="36" t="s">
-        <v>48</v>
-      </c>
-      <c r="H260" t="s">
-        <v>133</v>
-      </c>
+        <v>734</v>
+      </c>
+      <c r="F260" s="35"/>
+      <c r="G260" s="36"/>
       <c r="K260" s="35"/>
     </row>
     <row r="261" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C261" t="s">
         <v>756</v>
@@ -12850,74 +12941,81 @@
         <v>760</v>
       </c>
       <c r="E261" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="F261" s="35"/>
       <c r="G261" s="36"/>
       <c r="K261" s="35"/>
     </row>
     <row r="262" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A262" t="s">
-        <v>773</v>
+      <c r="A262" s="37" t="s">
+        <v>771</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>755</v>
-      </c>
-      <c r="C262" t="s">
-        <v>757</v>
-      </c>
-      <c r="D262" s="3" t="s">
+        <v>754</v>
+      </c>
+      <c r="C262" s="37" t="s">
         <v>761</v>
       </c>
-      <c r="E262" t="s">
-        <v>735</v>
-      </c>
-      <c r="F262" s="35"/>
-      <c r="G262" s="36"/>
-      <c r="K262" s="35"/>
+      <c r="D262" s="38" t="s">
+        <v>762</v>
+      </c>
+      <c r="E262" s="37" t="s">
+        <v>734</v>
+      </c>
+      <c r="F262" s="39"/>
+      <c r="G262" s="40"/>
+      <c r="H262" s="37"/>
+      <c r="I262" s="37"/>
+      <c r="J262" s="37"/>
+      <c r="K262" s="39"/>
+      <c r="L262" s="37"/>
     </row>
     <row r="263" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A263" s="37" t="s">
-        <v>772</v>
+      <c r="A263" t="s">
+        <v>777</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>755</v>
-      </c>
-      <c r="C263" s="37" t="s">
-        <v>762</v>
-      </c>
-      <c r="D263" s="38" t="s">
+        <v>754</v>
+      </c>
+      <c r="C263" t="s">
+        <v>776</v>
+      </c>
+      <c r="D263" s="3" t="s">
         <v>763</v>
       </c>
       <c r="E263" s="37" t="s">
-        <v>735</v>
-      </c>
-      <c r="F263" s="39"/>
-      <c r="G263" s="40"/>
-      <c r="H263" s="37"/>
-      <c r="I263" s="37"/>
-      <c r="J263" s="37"/>
-      <c r="K263" s="39"/>
-      <c r="L263" s="37"/>
+        <v>734</v>
+      </c>
+      <c r="F263" s="35" t="s">
+        <v>746</v>
+      </c>
+      <c r="G263" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="H263" t="s">
+        <v>133</v>
+      </c>
+      <c r="K263" s="35"/>
     </row>
     <row r="264" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>778</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>755</v>
+        <v>763</v>
       </c>
       <c r="C264" t="s">
-        <v>777</v>
+        <v>737</v>
       </c>
       <c r="D264" s="3" t="s">
-        <v>764</v>
+        <v>757</v>
       </c>
       <c r="E264" s="37" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="F264" s="35" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="G264" s="36" t="s">
         <v>48</v>
@@ -12932,19 +13030,19 @@
         <v>779</v>
       </c>
       <c r="B265" s="3" t="s">
+        <v>757</v>
+      </c>
+      <c r="C265" t="s">
+        <v>737</v>
+      </c>
+      <c r="D265" s="3" t="s">
         <v>764</v>
       </c>
-      <c r="C265" t="s">
-        <v>738</v>
-      </c>
-      <c r="D265" s="3" t="s">
-        <v>758</v>
-      </c>
       <c r="E265" s="37" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="F265" s="35" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="G265" s="36" t="s">
         <v>48</v>
@@ -12956,46 +13054,39 @@
     </row>
     <row r="266" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
-        <v>780</v>
+        <v>770</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>758</v>
+        <v>283</v>
       </c>
       <c r="C266" t="s">
-        <v>738</v>
+        <v>72</v>
       </c>
       <c r="D266" s="3" t="s">
-        <v>765</v>
-      </c>
-      <c r="E266" s="37" t="s">
-        <v>735</v>
-      </c>
-      <c r="F266" s="35" t="s">
-        <v>747</v>
-      </c>
-      <c r="G266" s="36" t="s">
-        <v>48</v>
-      </c>
-      <c r="H266" t="s">
-        <v>133</v>
-      </c>
+        <v>766</v>
+      </c>
+      <c r="E266" t="s">
+        <v>767</v>
+      </c>
+      <c r="F266" s="35"/>
+      <c r="G266" s="36"/>
       <c r="K266" s="35"/>
     </row>
     <row r="267" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>283</v>
+        <v>766</v>
       </c>
       <c r="C267" t="s">
-        <v>72</v>
+        <v>767</v>
       </c>
       <c r="D267" s="3" t="s">
+        <v>768</v>
+      </c>
+      <c r="E267" t="s">
         <v>767</v>
-      </c>
-      <c r="E267" t="s">
-        <v>768</v>
       </c>
       <c r="F267" s="35"/>
       <c r="G267" s="36"/>
@@ -13003,97 +13094,99 @@
     </row>
     <row r="268" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
-        <v>770</v>
+        <v>782</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>767</v>
+        <v>754</v>
       </c>
       <c r="C268" t="s">
-        <v>768</v>
+        <v>781</v>
       </c>
       <c r="D268" s="3" t="s">
-        <v>769</v>
+        <v>783</v>
       </c>
       <c r="E268" t="s">
-        <v>768</v>
-      </c>
-      <c r="F268" s="35"/>
-      <c r="G268" s="36"/>
+        <v>746</v>
+      </c>
+      <c r="F268" s="35" t="s">
+        <v>746</v>
+      </c>
+      <c r="G268" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="H268" t="s">
+        <v>133</v>
+      </c>
+      <c r="I268" t="s">
+        <v>758</v>
+      </c>
       <c r="K268" s="35"/>
     </row>
     <row r="269" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>783</v>
       </c>
-      <c r="B269" s="3" t="s">
-        <v>755</v>
+      <c r="B269" t="s">
+        <v>783</v>
       </c>
       <c r="C269" t="s">
-        <v>782</v>
+        <v>746</v>
       </c>
       <c r="D269" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="E269" t="s">
+        <v>746</v>
+      </c>
+      <c r="F269" s="35" t="s">
+        <v>746</v>
+      </c>
+      <c r="G269" s="36"/>
+      <c r="J269" t="s">
         <v>784</v>
-      </c>
-      <c r="E269" t="s">
-        <v>747</v>
-      </c>
-      <c r="F269" s="35" t="s">
-        <v>747</v>
-      </c>
-      <c r="G269" s="36" t="s">
-        <v>48</v>
-      </c>
-      <c r="H269" t="s">
-        <v>133</v>
-      </c>
-      <c r="I269" t="s">
-        <v>759</v>
       </c>
       <c r="K269" s="35"/>
     </row>
     <row r="270" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
-        <v>784</v>
-      </c>
-      <c r="B270" t="s">
-        <v>784</v>
+        <v>786</v>
+      </c>
+      <c r="B270" s="3" t="s">
+        <v>754</v>
       </c>
       <c r="C270" t="s">
-        <v>747</v>
+        <v>785</v>
       </c>
       <c r="D270" s="3" t="s">
-        <v>759</v>
+        <v>787</v>
       </c>
       <c r="E270" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="F270" s="35" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="G270" s="36"/>
-      <c r="J270" t="s">
-        <v>785</v>
-      </c>
       <c r="K270" s="35"/>
     </row>
     <row r="271" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
-        <v>787</v>
+        <v>800</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C271" t="s">
-        <v>786</v>
+        <v>788</v>
       </c>
       <c r="D271" s="3" t="s">
-        <v>788</v>
+        <v>794</v>
       </c>
       <c r="E271" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="F271" s="35" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="G271" s="36"/>
       <c r="K271" s="35"/>
@@ -13103,19 +13196,19 @@
         <v>801</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C272" t="s">
-        <v>789</v>
+        <v>793</v>
       </c>
       <c r="D272" s="3" t="s">
         <v>795</v>
       </c>
       <c r="E272" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="F272" s="35" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="G272" s="36"/>
       <c r="K272" s="35"/>
@@ -13125,19 +13218,19 @@
         <v>802</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C273" t="s">
-        <v>794</v>
+        <v>789</v>
       </c>
       <c r="D273" s="3" t="s">
         <v>796</v>
       </c>
       <c r="E273" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="F273" s="35" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="G273" s="36"/>
       <c r="K273" s="35"/>
@@ -13147,7 +13240,7 @@
         <v>803</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C274" t="s">
         <v>790</v>
@@ -13156,10 +13249,10 @@
         <v>797</v>
       </c>
       <c r="E274" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="F274" s="35" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="G274" s="36"/>
       <c r="K274" s="35"/>
@@ -13169,7 +13262,7 @@
         <v>804</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C275" t="s">
         <v>791</v>
@@ -13178,10 +13271,10 @@
         <v>798</v>
       </c>
       <c r="E275" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="F275" s="35" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="G275" s="36"/>
       <c r="K275" s="35"/>
@@ -13191,7 +13284,7 @@
         <v>805</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C276" t="s">
         <v>792</v>
@@ -13200,88 +13293,266 @@
         <v>799</v>
       </c>
       <c r="E276" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="F276" s="35" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="G276" s="36"/>
       <c r="K276" s="35"/>
     </row>
     <row r="277" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
-        <v>806</v>
+        <v>816</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>755</v>
+        <v>810</v>
       </c>
       <c r="C277" t="s">
-        <v>793</v>
+        <v>737</v>
       </c>
       <c r="D277" s="3" t="s">
-        <v>800</v>
+        <v>817</v>
       </c>
       <c r="E277" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="F277" s="35" t="s">
-        <v>747</v>
-      </c>
-      <c r="G277" s="36"/>
+        <v>818</v>
+      </c>
+      <c r="G277" s="36" t="s">
+        <v>814</v>
+      </c>
       <c r="K277" s="35"/>
     </row>
     <row r="278" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>817</v>
       </c>
-      <c r="B278" s="3" t="s">
-        <v>811</v>
-      </c>
-      <c r="C278" t="s">
-        <v>738</v>
+      <c r="B278" t="s">
+        <v>816</v>
       </c>
       <c r="D278" s="3" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="E278" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="F278" s="35" t="s">
-        <v>819</v>
+        <v>746</v>
       </c>
       <c r="G278" s="36" t="s">
-        <v>815</v>
+        <v>403</v>
       </c>
       <c r="K278" s="35"/>
     </row>
     <row r="279" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
-        <v>818</v>
-      </c>
-      <c r="B279" t="s">
-        <v>817</v>
-      </c>
-      <c r="D279" s="3" t="s">
-        <v>820</v>
-      </c>
-      <c r="E279" t="s">
-        <v>747</v>
+        <v>836</v>
+      </c>
+      <c r="B279" s="3" t="s">
+        <v>619</v>
       </c>
       <c r="F279" s="35" t="s">
-        <v>747</v>
+        <v>288</v>
       </c>
       <c r="G279" s="36" t="s">
+        <v>837</v>
+      </c>
+      <c r="H279" t="s">
+        <v>133</v>
+      </c>
+      <c r="I279" t="s">
+        <v>830</v>
+      </c>
+      <c r="K279" s="35"/>
+    </row>
+    <row r="280" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A280" t="s">
+        <v>838</v>
+      </c>
+      <c r="B280" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="F280" t="s">
+        <v>293</v>
+      </c>
+      <c r="G280" t="s">
+        <v>839</v>
+      </c>
+      <c r="H280" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="281" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A281" t="s">
+        <v>840</v>
+      </c>
+      <c r="B281" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="F281" t="s">
+        <v>288</v>
+      </c>
+      <c r="G281" t="s">
+        <v>841</v>
+      </c>
+      <c r="H281" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="282" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A282" t="s">
+        <v>842</v>
+      </c>
+      <c r="B282" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="F282" t="s">
+        <v>288</v>
+      </c>
+      <c r="G282" t="s">
+        <v>841</v>
+      </c>
+      <c r="H282" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="283" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A283" t="s">
+        <v>844</v>
+      </c>
+      <c r="B283" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="F283" t="s">
+        <v>35</v>
+      </c>
+      <c r="G283" t="s">
+        <v>845</v>
+      </c>
+      <c r="H283" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="284" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A284" t="s">
+        <v>848</v>
+      </c>
+      <c r="B284" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="F284" t="s">
+        <v>35</v>
+      </c>
+      <c r="G284" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="285" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A285" t="s">
+        <v>849</v>
+      </c>
+      <c r="B285" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="F285" t="s">
+        <v>35</v>
+      </c>
+      <c r="G285" t="s">
+        <v>847</v>
+      </c>
+      <c r="J285" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="286" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A286" t="s">
+        <v>850</v>
+      </c>
+      <c r="B286" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="F286" t="s">
+        <v>35</v>
+      </c>
+      <c r="G286" t="s">
+        <v>851</v>
+      </c>
+      <c r="H286" t="s">
+        <v>133</v>
+      </c>
+      <c r="J286" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="287" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A287" t="s">
+        <v>853</v>
+      </c>
+      <c r="B287" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="F287" t="s">
+        <v>738</v>
+      </c>
+      <c r="G287" t="s">
+        <v>854</v>
+      </c>
+      <c r="H287" t="s">
+        <v>133</v>
+      </c>
+      <c r="J287" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="288" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A288" t="s">
+        <v>856</v>
+      </c>
+      <c r="B288" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="F288" t="s">
+        <v>735</v>
+      </c>
+      <c r="G288" t="s">
+        <v>632</v>
+      </c>
+      <c r="H288" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="289" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A289" t="s">
+        <v>857</v>
+      </c>
+      <c r="B289" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="F289" t="s">
+        <v>858</v>
+      </c>
+      <c r="G289" t="s">
         <v>403</v>
       </c>
-      <c r="K279" s="35"/>
-    </row>
-    <row r="280" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F280" s="35"/>
-      <c r="G280" s="36"/>
-      <c r="I280" t="s">
-        <v>831</v>
-      </c>
-      <c r="K280" s="35"/>
+      <c r="H289" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="290" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A290" t="s">
+        <v>859</v>
+      </c>
+      <c r="F290" t="s">
+        <v>858</v>
+      </c>
+      <c r="G290" t="s">
+        <v>403</v>
+      </c>
+      <c r="H290" t="s">
+        <v>133</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
changes to the video input to Propresenter
</commit_message>
<xml_diff>
--- a/data/uac_cables.xlsx
+++ b/data/uac_cables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/donert/Documents/UACTech/SystemDocumentation/github/uactechdoc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A08B20-5AE0-C541-AAC1-F036FFB6D773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D555E6-3B38-D44B-ABAB-E713B90C8048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{288904EE-D384-EA4C-9B98-052B972FB267}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2147" uniqueCount="863">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2156" uniqueCount="866">
   <si>
     <t>Tag</t>
   </si>
@@ -2629,6 +2629,15 @@
   </si>
   <si>
     <t>2310-1005</t>
+  </si>
+  <si>
+    <t>barrel-sdi7</t>
+  </si>
+  <si>
+    <t>a286</t>
+  </si>
+  <si>
+    <t>out8</t>
   </si>
 </sst>
 </file>
@@ -2840,7 +2849,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2880,14 +2889,9 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4948,13 +4952,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD7E3698-8860-904B-8BDB-00EF1039C49C}" name="Table1" displayName="Table1" ref="A1:L278" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="5">
-  <autoFilter ref="A1:L278" xr:uid="{BD7E3698-8860-904B-8BDB-00EF1039C49C}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="2308-2901"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:L278" xr:uid="{BD7E3698-8860-904B-8BDB-00EF1039C49C}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{4D442337-BE86-B24A-84A4-338FB80A6A49}" name="Tag"/>
     <tableColumn id="2" xr3:uid="{74A36D7B-C989-3B4B-B1E5-AB1FA4C2DD45}" name="SrcTag" dataDxfId="4"/>
@@ -5270,13 +5268,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B91ADC-4569-1C4E-B002-1ED2E647C959}">
-  <dimension ref="A1:L292"/>
+  <dimension ref="A1:L293"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="310" zoomScaleNormal="310" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E286" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B279" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I292" sqref="I292"/>
+      <selection pane="bottomRight" activeCell="A285" sqref="A285"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5330,7 +5328,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>25</v>
       </c>
@@ -5373,7 +5371,7 @@
         <v>cdmua001:Key -&gt; zviue004:sw1 [label='2307-1800']</v>
       </c>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>4</v>
       </c>
@@ -5408,7 +5406,7 @@
         <v>cdmua001:Fill -&gt; zviue004:sw2 [label='2307-1801']</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>5</v>
       </c>
@@ -5443,7 +5441,7 @@
         <v>cdmua001:ProjA -&gt; zviue004:sw4 [label='2307-1802']</v>
       </c>
     </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>6</v>
       </c>
@@ -5478,7 +5476,7 @@
         <v>cdmua001:ProjB -&gt; zviue004:sw6 [label='2307-1803']</v>
       </c>
     </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>7</v>
       </c>
@@ -5513,7 +5511,7 @@
         <v>cdmua001:ProjC -&gt; zviue004:sw8 [label='2307-1804']</v>
       </c>
     </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>8</v>
       </c>
@@ -5548,7 +5546,7 @@
         <v>cdmua001:RearDeckLink -&gt; zviue004:sw3 [label='2307-1805']</v>
       </c>
     </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>9</v>
       </c>
@@ -5575,7 +5573,7 @@
         <v>unused: -&gt; : [label='2307-1806']</v>
       </c>
     </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
         <v>10</v>
       </c>
@@ -5610,7 +5608,7 @@
         <v>cdmua001:in1 -&gt; zviue004:sw5 [label='2307-1807']</v>
       </c>
     </row>
-    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>11</v>
       </c>
@@ -5645,7 +5643,7 @@
         <v>zvkua003:aux -&gt; zviud001:sdi in [label='2307-1808']</v>
       </c>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
         <v>12</v>
       </c>
@@ -5688,7 +5686,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>13</v>
       </c>
@@ -5733,7 +5731,7 @@
         <v>zviue004:sdi1 -&gt; 23081204:sdi in [label='2307-1810']</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>14</v>
       </c>
@@ -5770,7 +5768,7 @@
         <v>zviue004:sdi2 -&gt; 23081205:sdi in [label='2307-1811']</v>
       </c>
     </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>15</v>
       </c>
@@ -5805,7 +5803,7 @@
         <v>zviue004:sdi4 -&gt; zviug003:sdi in [label='2307-1812']</v>
       </c>
     </row>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
         <v>16</v>
       </c>
@@ -5840,7 +5838,7 @@
         <v>zviue004:sdi6 -&gt; zviug004:sdi in [label='2307-1813']</v>
       </c>
     </row>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>17</v>
       </c>
@@ -5875,7 +5873,7 @@
         <v>zviue004:sdi8 -&gt; zviug005:sdi in [label='2307-1814']</v>
       </c>
     </row>
-    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
         <v>18</v>
       </c>
@@ -5910,7 +5908,7 @@
         <v>zviue004:sdi3 -&gt; zviue001:sdi in [label='2307-1815']</v>
       </c>
     </row>
-    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>19</v>
       </c>
@@ -5931,7 +5929,7 @@
         <v>: -&gt; : [label='2307-1816']</v>
       </c>
     </row>
-    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
         <v>20</v>
       </c>
@@ -5952,7 +5950,7 @@
         <v>: -&gt; : [label='2307-1817']</v>
       </c>
     </row>
-    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>21</v>
       </c>
@@ -5973,7 +5971,7 @@
         <v>: -&gt; : [label='2307-1818']</v>
       </c>
     </row>
-    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
         <v>22</v>
       </c>
@@ -6000,7 +5998,7 @@
         <v>not used: -&gt; : [label='2307-1819']</v>
       </c>
     </row>
-    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>23</v>
       </c>
@@ -6035,7 +6033,7 @@
         <v>23071825:barrel -&gt; zviue004:sdi5 [label='2307-1820']</v>
       </c>
     </row>
-    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
         <v>24</v>
       </c>
@@ -6070,7 +6068,7 @@
         <v>23071826:barrel -&gt; zviue004:sdi7 [label='2307-1821']</v>
       </c>
     </row>
-    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>30</v>
       </c>
@@ -6099,7 +6097,7 @@
         <v>unused: -&gt; : [label='2307-1822']</v>
       </c>
     </row>
-    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
         <v>52</v>
       </c>
@@ -6134,7 +6132,7 @@
         <v>zviua008:hdmi -&gt; zvkua003:in4 [label='2307-1828']</v>
       </c>
     </row>
-    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>47</v>
       </c>
@@ -6167,7 +6165,7 @@
         <v>cdmua001:usbc -&gt; zviue005:usbc [label='2307-1824']</v>
       </c>
     </row>
-    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="23" t="s">
         <v>49</v>
       </c>
@@ -6202,7 +6200,7 @@
         <v>zviua005:sdi -&gt; 23071820:barrel [label='2307-1825']</v>
       </c>
     </row>
-    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
         <v>50</v>
       </c>
@@ -6235,7 +6233,7 @@
         <v>unknown: -&gt; 23071821:barrel [label='2307-1826']</v>
       </c>
     </row>
-    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
         <v>65</v>
       </c>
@@ -6268,7 +6266,7 @@
         <v>zviua004:usb -&gt; cumug001:usb_3 [label='2307-2100']</v>
       </c>
     </row>
-    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
         <v>66</v>
       </c>
@@ -6303,7 +6301,7 @@
         <v>cumug001:ndi -&gt; cumue001:obs [label='2307-2101']</v>
       </c>
     </row>
-    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="s">
         <v>67</v>
       </c>
@@ -6336,7 +6334,7 @@
         <v>camera left: -&gt; cumue001:obs [label='2307-2102']</v>
       </c>
     </row>
-    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>68</v>
       </c>
@@ -6369,7 +6367,7 @@
         <v>camera centre: -&gt; cumue001:obs [label='2307-2103']</v>
       </c>
     </row>
-    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="15" t="s">
         <v>69</v>
       </c>
@@ -6402,7 +6400,7 @@
         <v>camera right: -&gt; cumue001:obs [label='2307-2104']</v>
       </c>
     </row>
-    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
         <v>70</v>
       </c>
@@ -6435,7 +6433,7 @@
         <v>cdmua001:ndi -&gt; cumue001:obs [label='2307-2105']</v>
       </c>
     </row>
-    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="15" t="s">
         <v>82</v>
       </c>
@@ -6468,7 +6466,7 @@
         <v>zvkua001:out_5_hdmi -&gt; zviuc001:hdmi in [label='2307-2300']</v>
       </c>
     </row>
-    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
         <v>86</v>
       </c>
@@ -6505,7 +6503,7 @@
         <v>zviuc001:hdmi out -&gt; zvkua003:in1 [label='2307-2301']</v>
       </c>
     </row>
-    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="15" t="s">
         <v>89</v>
       </c>
@@ -6540,7 +6538,7 @@
         <v>zvcua001:sdi -&gt; zvkua003:in5 [label='2307-2304']</v>
       </c>
     </row>
-    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
         <v>88</v>
       </c>
@@ -6575,7 +6573,7 @@
         <v>zvcua002:sdi -&gt; zvkua003:in6 [label='2307-2303']</v>
       </c>
     </row>
-    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="15" t="s">
         <v>87</v>
       </c>
@@ -6610,7 +6608,7 @@
         <v>zvcua003:sdi -&gt; zvkua003:in7 [label='2307-2302']</v>
       </c>
     </row>
-    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
         <v>96</v>
       </c>
@@ -6647,7 +6645,7 @@
         <v>23072306:barrel -&gt; zvkua003:in8 [label='2307-2305']</v>
       </c>
     </row>
-    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="15" t="s">
         <v>97</v>
       </c>
@@ -6682,7 +6680,7 @@
         <v>z150:sdi -&gt; 23072305:barrel [label='2307-2306']</v>
       </c>
     </row>
-    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
         <v>98</v>
       </c>
@@ -6709,7 +6707,7 @@
         <v>: -&gt; : [label='2307-2307']</v>
       </c>
     </row>
-    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="15" t="s">
         <v>102</v>
       </c>
@@ -6744,7 +6742,7 @@
         <v>zvkua004:sw -&gt; zvcua001:sw [label='2307-2308']</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
         <v>103</v>
       </c>
@@ -6787,7 +6785,7 @@
         <v>zvkua004:sw -&gt; zvcua002:sw [label='2307-2309']</v>
       </c>
     </row>
-    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="15" t="s">
         <v>104</v>
       </c>
@@ -6822,7 +6820,7 @@
         <v>zvkua004:sw -&gt; zvcua003:sw [label='2307-2310']</v>
       </c>
     </row>
-    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
         <v>107</v>
       </c>
@@ -6841,7 +6839,7 @@
         <v>: -&gt; : [label='2307-2311']</v>
       </c>
     </row>
-    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="15" t="s">
         <v>110</v>
       </c>
@@ -6860,7 +6858,7 @@
         <v>: -&gt; : [label='2307-2312']</v>
       </c>
     </row>
-    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
         <v>111</v>
       </c>
@@ -6879,7 +6877,7 @@
         <v>: -&gt; : [label='2307-2313']</v>
       </c>
     </row>
-    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="15" t="s">
         <v>112</v>
       </c>
@@ -6912,7 +6910,7 @@
         <v>zvkua001:out_4_HDbT -&gt; zvvu0001:HDbT [label='2307-2314']</v>
       </c>
     </row>
-    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
         <v>121</v>
       </c>
@@ -6947,7 +6945,7 @@
         <v>zvkua001:out_7_HDbT -&gt; zviua001:HDbT [label='2307-2315']</v>
       </c>
     </row>
-    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="15" t="s">
         <v>122</v>
       </c>
@@ -6980,7 +6978,7 @@
         <v>zviua001:hdmi -&gt; zvvulobby tv :hdmi 1 [label='2307-2316']</v>
       </c>
     </row>
-    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
         <v>123</v>
       </c>
@@ -7007,7 +7005,7 @@
         <v>: -&gt; : [label='2307-2317']</v>
       </c>
     </row>
-    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="15" t="s">
         <v>127</v>
       </c>
@@ -7042,7 +7040,7 @@
         <v>zvkua001:out_8_HDbT -&gt; zviua002:HDbT [label='2307-2318']</v>
       </c>
     </row>
-    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="11" t="s">
         <v>413</v>
       </c>
@@ -7073,7 +7071,7 @@
         <v>zviua002:hdmi -&gt; 23082900:input [label='2308-3001']</v>
       </c>
     </row>
-    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="15" t="s">
         <v>130</v>
       </c>
@@ -7100,7 +7098,7 @@
         <v>: -&gt; : [label='2307-2320']</v>
       </c>
     </row>
-    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
         <v>135</v>
       </c>
@@ -7133,7 +7131,7 @@
         <v>cdmua001:PP_Front_SW -&gt; hdmi_dongle: [label='2307-3000']</v>
       </c>
     </row>
-    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="15" t="s">
         <v>137</v>
       </c>
@@ -7166,7 +7164,7 @@
         <v>zvrua001:OutB -&gt; zvrua002:SDI In [label='2307-3001']</v>
       </c>
     </row>
-    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
         <v>139</v>
       </c>
@@ -7199,7 +7197,7 @@
         <v>zvrua001:OutA -&gt; zviua004:SDI In [label='2307-3002']</v>
       </c>
     </row>
-    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="15" t="s">
         <v>142</v>
       </c>
@@ -7234,7 +7232,7 @@
         <v>zviua004:hdmi out -&gt; zvkua001:in7 [label='2307-3003']</v>
       </c>
     </row>
-    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="11" t="s">
         <v>143</v>
       </c>
@@ -7253,7 +7251,7 @@
         <v>: -&gt; : [label='2307-3004']</v>
       </c>
     </row>
-    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="15" t="s">
         <v>144</v>
       </c>
@@ -7290,7 +7288,7 @@
         <v>zvkua003:out5 -&gt; zvrua001:sdi in [label='2307-3005']</v>
       </c>
     </row>
-    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" s="11" t="s">
         <v>145</v>
       </c>
@@ -7327,7 +7325,7 @@
         <v>zvkua003:out6 -&gt; zviud002:sdi in [label='2307-3006']</v>
       </c>
     </row>
-    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" s="15" t="s">
         <v>148</v>
       </c>
@@ -7360,7 +7358,7 @@
         <v>zviud001:hdmi -&gt; zviua004:hdmi in [label='2307-3007']</v>
       </c>
     </row>
-    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">
         <v>161</v>
       </c>
@@ -7395,7 +7393,7 @@
         <v>zviua005:hdmi -&gt; zvkua001:in6 [label='2308-0800']</v>
       </c>
     </row>
-    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" s="15" t="s">
         <v>204</v>
       </c>
@@ -7427,7 +7425,7 @@
         <v>unused:  -&gt; : [label='2308-0004']</v>
       </c>
     </row>
-    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="11" t="s">
         <v>205</v>
       </c>
@@ -7460,7 +7458,7 @@
         <v>frontguest: -&gt; 23080003:InputC [label='2308-0005']</v>
       </c>
     </row>
-    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" s="15" t="s">
         <v>206</v>
       </c>
@@ -7495,7 +7493,7 @@
         <v>cdwua002:HdmiOut -&gt; 23080002:In2 [label='2308-0006']</v>
       </c>
     </row>
-    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" s="11" t="s">
         <v>207</v>
       </c>
@@ -7528,7 +7526,7 @@
         <v>rearguest:hdmi_out -&gt; 23080002:In1 [label='2308-0007']</v>
       </c>
     </row>
-    <row r="69" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" s="15" t="s">
         <v>208</v>
       </c>
@@ -7561,7 +7559,7 @@
         <v>cdwua002:vga -&gt; vmnu0029:vga [label='2308-0009']</v>
       </c>
     </row>
-    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" s="11" t="s">
         <v>209</v>
       </c>
@@ -7594,7 +7592,7 @@
         <v>cdwua002:usb -&gt; 23080008:usb [label='2308-0010']</v>
       </c>
     </row>
-    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" s="11" t="s">
         <v>184</v>
       </c>
@@ -7627,7 +7625,7 @@
         <v>zviug003:hdmi_out -&gt; zvkua001:in1 [label='2308-0915']</v>
       </c>
     </row>
-    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72" s="15" t="s">
         <v>185</v>
       </c>
@@ -7660,7 +7658,7 @@
         <v>zviug004:hdmi_out -&gt; zvkua001:in2 [label='2308-0916']</v>
       </c>
     </row>
-    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" s="11" t="s">
         <v>186</v>
       </c>
@@ -7693,7 +7691,7 @@
         <v>zviug005:hdmi_out -&gt; zvkua001:in3 [label='2308-0917']</v>
       </c>
     </row>
-    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" s="15" t="s">
         <v>187</v>
       </c>
@@ -7723,7 +7721,7 @@
       <c r="K74" s="17"/>
       <c r="L74" s="18"/>
     </row>
-    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" s="11" t="s">
         <v>194</v>
       </c>
@@ -7764,7 +7762,7 @@
         <v>zvkua001:out_1_HDbT -&gt; zvvua001:InputD [label='PROJ0001']</v>
       </c>
     </row>
-    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" s="15" t="s">
         <v>195</v>
       </c>
@@ -7805,7 +7803,7 @@
         <v>zvkua001:out_2_HDbT -&gt; zvvua002:InputD [label='PROJ0002']</v>
       </c>
     </row>
-    <row r="77" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" s="11" t="s">
         <v>196</v>
       </c>
@@ -7846,7 +7844,7 @@
         <v>zvkua001:out_3_HDbT -&gt; zvvua003:InputD [label='PROJ0003']</v>
       </c>
     </row>
-    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78" s="15" t="s">
         <v>202</v>
       </c>
@@ -7889,7 +7887,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" s="11" t="s">
         <v>215</v>
       </c>
@@ -7930,7 +7928,7 @@
         <v>cumue001:usba_2 -&gt; 23081110:usb_in [label='2308-1111']</v>
       </c>
     </row>
-    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80" s="15" t="s">
         <v>230</v>
       </c>
@@ -7963,7 +7961,7 @@
         <v>23081110:usb_1 -&gt; 23081104:usb [label='2308-1112']</v>
       </c>
     </row>
-    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" s="11" t="s">
         <v>231</v>
       </c>
@@ -7996,7 +7994,7 @@
         <v>23081110:usb_2 -&gt; 23081105:usb [label='2308-1113']</v>
       </c>
     </row>
-    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82" s="15" t="s">
         <v>232</v>
       </c>
@@ -8033,7 +8031,7 @@
         <v>cumue001:usbc -&gt; 23081106:hdmi [label='2308-1114']</v>
       </c>
     </row>
-    <row r="83" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" s="11" t="s">
         <v>233</v>
       </c>
@@ -8068,7 +8066,7 @@
         <v>cumue001:hdmi -&gt; 23081107:hdmi [label='2308-1115']</v>
       </c>
     </row>
-    <row r="84" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84" s="15" t="s">
         <v>234</v>
       </c>
@@ -8101,7 +8099,7 @@
         <v>23081110:usb  -&gt; 23081103:usb [label='2308-1116']</v>
       </c>
     </row>
-    <row r="85" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A85" s="11" t="s">
         <v>235</v>
       </c>
@@ -8142,7 +8140,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86" s="15" t="s">
         <v>236</v>
       </c>
@@ -8183,7 +8181,7 @@
         <v>23081100:port3 -&gt; zaiue002:ether [label='2308-1118']</v>
       </c>
     </row>
-    <row r="87" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87" s="11" t="s">
         <v>237</v>
       </c>
@@ -8224,7 +8222,7 @@
         <v>23081100:port4 -&gt; daw_guest:ether [label='2308-1119']</v>
       </c>
     </row>
-    <row r="88" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88" s="15" t="s">
         <v>238</v>
       </c>
@@ -8260,7 +8258,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="89" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89" s="11" t="s">
         <v>239</v>
       </c>
@@ -8301,7 +8299,7 @@
         <v>zaiue002:Ch2 -&gt; 23081102:right [label='2308-1121']</v>
       </c>
     </row>
-    <row r="90" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A90" s="15" t="s">
         <v>240</v>
       </c>
@@ -8344,7 +8342,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="91" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A91" s="11" t="s">
         <v>245</v>
       </c>
@@ -8387,7 +8385,7 @@
         <v>23081124:ch1 -&gt; zvkua003:ch1_audio [label='2308-1124L']</v>
       </c>
     </row>
-    <row r="92" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A92" s="15" t="s">
         <v>249</v>
       </c>
@@ -8422,7 +8420,7 @@
         <v>23081124:ch2 -&gt; zvkua003:ch2_audio [label='2308-1124R']</v>
       </c>
     </row>
-    <row r="93" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A93" s="11" t="s">
         <v>706</v>
       </c>
@@ -8440,7 +8438,7 @@
         <v>: -&gt; : [label='x93']</v>
       </c>
     </row>
-    <row r="94" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A94" s="15" t="s">
         <v>707</v>
       </c>
@@ -8458,7 +8456,7 @@
         <v>: -&gt; : [label='x94']</v>
       </c>
     </row>
-    <row r="95" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A95" s="11" t="s">
         <v>708</v>
       </c>
@@ -8491,7 +8489,7 @@
         <v>zakua001:aux4 -&gt; 23080008:Mic_In [label='x95']</v>
       </c>
     </row>
-    <row r="96" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A96" s="15"/>
       <c r="B96" s="16" t="s">
         <v>183</v>
@@ -8522,7 +8520,7 @@
         <v>23080906:out -&gt; zakua001:ch_12 [label='']</v>
       </c>
     </row>
-    <row r="97" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A97" s="11" t="s">
         <v>704</v>
       </c>
@@ -8553,7 +8551,7 @@
         <v>rearguest:left -&gt; zakua001:ch_13 [label='x97']</v>
       </c>
     </row>
-    <row r="98" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A98" s="15" t="s">
         <v>705</v>
       </c>
@@ -8584,7 +8582,7 @@
         <v>rearguest:right -&gt; zakua001:ch_14 [label='x98']</v>
       </c>
     </row>
-    <row r="99" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A99" s="11"/>
       <c r="B99" s="12" t="s">
         <v>168</v>
@@ -8613,7 +8611,7 @@
         <v>cdwua002:left -&gt; zakua001:ch_15 [label='']</v>
       </c>
     </row>
-    <row r="100" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A100" s="15"/>
       <c r="B100" s="16" t="s">
         <v>168</v>
@@ -8642,7 +8640,7 @@
         <v>cdwua002:right -&gt; zakua001:ch_16 [label='']</v>
       </c>
     </row>
-    <row r="101" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A101" s="11"/>
       <c r="B101" s="12" t="s">
         <v>73</v>
@@ -8681,7 +8679,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="102" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A102" s="15"/>
       <c r="B102" s="16" t="s">
         <v>73</v>
@@ -8720,7 +8718,7 @@
         <v>cumug001:usb_2 -&gt; zviug001:usb_in [label='']</v>
       </c>
     </row>
-    <row r="103" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A103" s="11"/>
       <c r="B103" s="12" t="s">
         <v>73</v>
@@ -8761,7 +8759,7 @@
         <v>cumug001:usb_1 -&gt; 23081202:usb [label='']</v>
       </c>
     </row>
-    <row r="104" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A104" s="15"/>
       <c r="B104" s="16" t="s">
         <v>261</v>
@@ -8802,7 +8800,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="105" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A105" s="11" t="s">
         <v>337</v>
       </c>
@@ -8845,7 +8843,7 @@
         <v>23081204:sdi_out -&gt; zviue003:sdi_in [label='2307-1201']</v>
       </c>
     </row>
-    <row r="106" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A106" s="15" t="s">
         <v>338</v>
       </c>
@@ -8880,7 +8878,7 @@
         <v>23081205:sdi_out -&gt; zviua008:sdi_in [label='2307-1202']</v>
       </c>
     </row>
-    <row r="107" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A107" s="11" t="s">
         <v>51</v>
       </c>
@@ -8915,7 +8913,7 @@
         <v>zviue003:hdmi_out -&gt; zvkua003:in2 [label='2307-1827']</v>
       </c>
     </row>
-    <row r="108" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A108" s="15"/>
       <c r="B108" s="16" t="s">
         <v>283</v>
@@ -8946,7 +8944,7 @@
         <v>cdwu0009:vga -&gt; mon:vga [label='']</v>
       </c>
     </row>
-    <row r="109" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A109" s="11" t="s">
         <v>285</v>
       </c>
@@ -8981,7 +8979,7 @@
         <v>prwall3:label3 -&gt; 23081100:port1 [label='2308-2001']</v>
       </c>
     </row>
-    <row r="110" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A110" s="15" t="s">
         <v>296</v>
       </c>
@@ -9014,7 +9012,7 @@
         <v>23081102:Right -&gt; 23082003:Right [label='2308-2002']</v>
       </c>
     </row>
-    <row r="111" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A111" s="11" t="s">
         <v>307</v>
       </c>
@@ -9047,7 +9045,7 @@
         <v>patchpanel:a -&gt; prwall3:b1 [label='a']</v>
       </c>
     </row>
-    <row r="112" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A112" s="15" t="s">
         <v>308</v>
       </c>
@@ -9080,7 +9078,7 @@
         <v>modem:c -&gt; router:d [label='b']</v>
       </c>
     </row>
-    <row r="113" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A113" s="11" t="s">
         <v>309</v>
       </c>
@@ -9113,7 +9111,7 @@
         <v>router:e -&gt; nscua001:f [label='c']</v>
       </c>
     </row>
-    <row r="114" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A114" s="15" t="s">
         <v>314</v>
       </c>
@@ -9146,7 +9144,7 @@
         <v>nscua001:h -&gt; patchpanel:i [label='g']</v>
       </c>
     </row>
-    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A115" s="11"/>
       <c r="B115" s="12" t="s">
         <v>306</v>
@@ -9173,7 +9171,7 @@
         <v>nscua001:a  -&gt; nscua002:f [label='']</v>
       </c>
     </row>
-    <row r="116" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A116" s="15"/>
       <c r="B116" s="16" t="s">
         <v>306</v>
@@ -9200,7 +9198,7 @@
         <v>nscua001:b  -&gt; nscua005:g [label='']</v>
       </c>
     </row>
-    <row r="117" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A117" s="11"/>
       <c r="B117" s="12" t="s">
         <v>325</v>
@@ -9225,7 +9223,7 @@
         <v>nscua005:c  -&gt; nscua003:h  [label='']</v>
       </c>
     </row>
-    <row r="118" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A118" s="15"/>
       <c r="B118" s="16" t="s">
         <v>327</v>
@@ -9254,7 +9252,7 @@
         <v>nscua003:d  -&gt; nscua004:i [label='']</v>
       </c>
     </row>
-    <row r="119" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A119" s="11"/>
       <c r="B119" s="12" t="s">
         <v>328</v>
@@ -9279,7 +9277,7 @@
         <v>nscua004:e  -&gt; 23081124:ether [label='']</v>
       </c>
     </row>
-    <row r="120" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A120" s="15" t="s">
         <v>372</v>
       </c>
@@ -9312,7 +9310,7 @@
         <v>cumug001:usb -&gt; zviuc002:usbc [label='future1']</v>
       </c>
     </row>
-    <row r="121" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A121" s="15" t="s">
         <v>375</v>
       </c>
@@ -9345,7 +9343,7 @@
         <v>cdwu0009:hdmi_out -&gt; zvkua001:in5 [label='2308-2500']</v>
       </c>
     </row>
-    <row r="122" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A122" s="11" t="s">
         <v>378</v>
       </c>
@@ -9380,7 +9378,7 @@
         <v>zviue001:hdmi_out -&gt; zvkua001:in4 [label='2308-2501']</v>
       </c>
     </row>
-    <row r="123" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A123" s="15" t="s">
         <v>379</v>
       </c>
@@ -9409,7 +9407,7 @@
         <v>not used: -&gt; : [label='2308-2502']</v>
       </c>
     </row>
-    <row r="124" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A124" s="11" t="s">
         <v>382</v>
       </c>
@@ -9438,7 +9436,7 @@
         <v>not used: -&gt; : [label='2308-2503']</v>
       </c>
     </row>
-    <row r="125" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A125" s="15" t="s">
         <v>389</v>
       </c>
@@ -9465,7 +9463,7 @@
         <v>not used: -&gt; : [label='2308-2504']</v>
       </c>
     </row>
-    <row r="126" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A126" s="11" t="s">
         <v>390</v>
       </c>
@@ -9500,7 +9498,7 @@
         <v>ncsua004:portxx -&gt; cdmua001:ether [label='2308-2600']</v>
       </c>
     </row>
-    <row r="127" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A127" s="15" t="s">
         <v>391</v>
       </c>
@@ -9525,7 +9523,7 @@
         <v>not used: -&gt; : [label='2308-2700']</v>
       </c>
     </row>
-    <row r="128" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A128" s="11" t="s">
         <v>392</v>
       </c>
@@ -9550,7 +9548,7 @@
         <v>not used: -&gt; : [label='2308-2701']</v>
       </c>
     </row>
-    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A129" s="15" t="s">
         <v>393</v>
       </c>
@@ -9612,7 +9610,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="131" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A131" s="15" t="s">
         <v>22</v>
       </c>
@@ -9655,7 +9653,7 @@
         <v>23082900:output2 -&gt; zvvu0003:hdmi1 [label='2307-1819']</v>
       </c>
     </row>
-    <row r="132" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A132" s="11" t="s">
         <v>412</v>
       </c>
@@ -9696,7 +9694,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A133" s="15" t="s">
         <v>409</v>
       </c>
@@ -9737,7 +9735,7 @@
         <v>zvkua001:out6 -&gt; unknown:unk [label='future135']</v>
       </c>
     </row>
-    <row r="134" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A134" s="11"/>
       <c r="B134" s="12"/>
       <c r="C134" s="13"/>
@@ -9756,7 +9754,7 @@
         <v>: -&gt; :unk [label='']</v>
       </c>
     </row>
-    <row r="135" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A135" s="15" t="s">
         <v>417</v>
       </c>
@@ -9791,7 +9789,7 @@
         <v>zamua001:ch1 -&gt; zaiub001:s2_in01 [label='2309-1001']</v>
       </c>
     </row>
-    <row r="136" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A136" s="11" t="s">
         <v>542</v>
       </c>
@@ -9826,7 +9824,7 @@
         <v>zamua001:ch2 -&gt; zaiub001:s2_in02 [label='2309-1002']</v>
       </c>
     </row>
-    <row r="137" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A137" s="15" t="s">
         <v>543</v>
       </c>
@@ -9861,7 +9859,7 @@
         <v>zamua001:ch3 -&gt; zaiub001:s2_in03 [label='2309-1003']</v>
       </c>
     </row>
-    <row r="138" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A138" s="11" t="s">
         <v>544</v>
       </c>
@@ -9896,7 +9894,7 @@
         <v>zamua001:ch4 -&gt; zaiub001:s2_in04 [label='2309-1004']</v>
       </c>
     </row>
-    <row r="139" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A139" s="15" t="s">
         <v>545</v>
       </c>
@@ -9931,7 +9929,7 @@
         <v>zamub001:ch1 -&gt; zaiub001:s2_in05 [label='2309-1005']</v>
       </c>
     </row>
-    <row r="140" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A140" s="11" t="s">
         <v>546</v>
       </c>
@@ -9966,7 +9964,7 @@
         <v>zamub001:ch2 -&gt; zaiub001:s2_in06 [label='2309-1006']</v>
       </c>
     </row>
-    <row r="141" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A141" s="15" t="s">
         <v>547</v>
       </c>
@@ -10001,7 +9999,7 @@
         <v>zamub001:ch3 -&gt; zaiub001:s2_in07 [label='2309-1007']</v>
       </c>
     </row>
-    <row r="142" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A142" s="11" t="s">
         <v>548</v>
       </c>
@@ -10036,7 +10034,7 @@
         <v>zamub001:ch4 -&gt; zaiub001:s2_in08 [label='2309-1008']</v>
       </c>
     </row>
-    <row r="143" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A143" s="15" t="s">
         <v>549</v>
       </c>
@@ -10071,7 +10069,7 @@
         <v>zamub002:ch1 -&gt; zaiub001:s2_in09 [label='2309-1009']</v>
       </c>
     </row>
-    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A144" s="11" t="s">
         <v>550</v>
       </c>
@@ -10106,7 +10104,7 @@
         <v>zamub002:ch2 -&gt; zaiub001:s2_in10 [label='2309-1010']</v>
       </c>
     </row>
-    <row r="145" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A145" s="15" t="s">
         <v>551</v>
       </c>
@@ -10141,7 +10139,7 @@
         <v>zamub002:ch3 -&gt; zaiub001:s2_in11 [label='2309-1011']</v>
       </c>
     </row>
-    <row r="146" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A146" s="11" t="s">
         <v>552</v>
       </c>
@@ -10176,7 +10174,7 @@
         <v>zamub002:ch4 -&gt; zaiub001:s2_in12 [label='2309-1012']</v>
       </c>
     </row>
-    <row r="147" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A147" s="15" t="s">
         <v>553</v>
       </c>
@@ -10211,7 +10209,7 @@
         <v>zamub003:ch4 -&gt; zaiub001:s2___ [label='2309-1013']</v>
       </c>
     </row>
-    <row r="148" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A148" s="11" t="s">
         <v>554</v>
       </c>
@@ -10246,7 +10244,7 @@
         <v>zamub002:ch3 -&gt; zaiub002:s2_in01 [label='2309-1014']</v>
       </c>
     </row>
-    <row r="149" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A149" s="9" t="s">
         <v>555</v>
       </c>
@@ -10281,7 +10279,7 @@
         <v>zamub002:ch4 -&gt; zaiub002:s2_in02 [label='2309-1015']</v>
       </c>
     </row>
-    <row r="150" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>556</v>
       </c>
@@ -10314,7 +10312,7 @@
         <v>zamub003:ch1 -&gt; zaiub002:s2_in03 [label='2309-1016']</v>
       </c>
     </row>
-    <row r="151" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>557</v>
       </c>
@@ -10347,7 +10345,7 @@
         <v>zamub003:ch2 -&gt; zaiub002:s2_in04 [label='2309-1017']</v>
       </c>
     </row>
-    <row r="152" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>558</v>
       </c>
@@ -10380,7 +10378,7 @@
         <v>zamub003:ch3 -&gt; zaiub002:s2_in05 [label='2309-1018']</v>
       </c>
     </row>
-    <row r="153" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>559</v>
       </c>
@@ -10409,7 +10407,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="154" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>560</v>
       </c>
@@ -10435,7 +10433,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="155" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>561</v>
       </c>
@@ -10461,7 +10459,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="156" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A156" s="8" t="s">
         <v>562</v>
       </c>
@@ -10487,7 +10485,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="157" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>563</v>
       </c>
@@ -10513,7 +10511,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="158" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>564</v>
       </c>
@@ -10539,7 +10537,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="159" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>565</v>
       </c>
@@ -10565,7 +10563,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="160" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>566</v>
       </c>
@@ -10591,7 +10589,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="161" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>567</v>
       </c>
@@ -10617,7 +10615,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="162" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>568</v>
       </c>
@@ -10643,7 +10641,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="163" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>569</v>
       </c>
@@ -10669,7 +10667,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="164" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>570</v>
       </c>
@@ -10695,7 +10693,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="165" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>571</v>
       </c>
@@ -10721,7 +10719,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="166" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>572</v>
       </c>
@@ -10747,7 +10745,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="167" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>573</v>
       </c>
@@ -10773,7 +10771,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="168" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>574</v>
       </c>
@@ -10799,7 +10797,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="169" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>575</v>
       </c>
@@ -10825,7 +10823,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="170" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>576</v>
       </c>
@@ -10851,7 +10849,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="171" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>577</v>
       </c>
@@ -10877,7 +10875,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="172" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>578</v>
       </c>
@@ -10903,7 +10901,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="173" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>579</v>
       </c>
@@ -10929,7 +10927,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="174" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>580</v>
       </c>
@@ -10955,7 +10953,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="175" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>581</v>
       </c>
@@ -10981,7 +10979,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="176" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>582</v>
       </c>
@@ -11001,7 +10999,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="177" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>583</v>
       </c>
@@ -11021,7 +11019,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="178" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>584</v>
       </c>
@@ -11041,7 +11039,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="179" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>585</v>
       </c>
@@ -11061,7 +11059,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="180" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>586</v>
       </c>
@@ -11081,7 +11079,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="181" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>587</v>
       </c>
@@ -11101,7 +11099,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="182" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>588</v>
       </c>
@@ -11121,7 +11119,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="183" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>589</v>
       </c>
@@ -11141,7 +11139,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="184" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>590</v>
       </c>
@@ -11161,7 +11159,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="185" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>591</v>
       </c>
@@ -11181,7 +11179,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="186" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>592</v>
       </c>
@@ -11201,7 +11199,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="187" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>593</v>
       </c>
@@ -11221,7 +11219,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="188" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>594</v>
       </c>
@@ -11241,7 +11239,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>595</v>
       </c>
@@ -11261,7 +11259,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>596</v>
       </c>
@@ -11281,7 +11279,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>597</v>
       </c>
@@ -11301,7 +11299,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="192" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>598</v>
       </c>
@@ -11321,7 +11319,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="193" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>599</v>
       </c>
@@ -11341,7 +11339,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="194" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>600</v>
       </c>
@@ -11361,7 +11359,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="195" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>601</v>
       </c>
@@ -11381,7 +11379,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="196" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>602</v>
       </c>
@@ -11401,7 +11399,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="197" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>603</v>
       </c>
@@ -11421,7 +11419,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="198" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>604</v>
       </c>
@@ -11441,7 +11439,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="199" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>605</v>
       </c>
@@ -11461,7 +11459,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="200" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>606</v>
       </c>
@@ -11481,7 +11479,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="201" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>607</v>
       </c>
@@ -11501,7 +11499,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="202" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>608</v>
       </c>
@@ -11521,7 +11519,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="203" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>609</v>
       </c>
@@ -11541,7 +11539,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="204" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>610</v>
       </c>
@@ -11561,7 +11559,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="205" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>611</v>
       </c>
@@ -11581,7 +11579,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="206" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>612</v>
       </c>
@@ -11601,7 +11599,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="207" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>613</v>
       </c>
@@ -11621,7 +11619,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="208" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>614</v>
       </c>
@@ -11650,7 +11648,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="209" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>615</v>
       </c>
@@ -11679,7 +11677,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="210" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>616</v>
       </c>
@@ -11708,7 +11706,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="211" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>617</v>
       </c>
@@ -11737,7 +11735,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="212" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>624</v>
       </c>
@@ -11769,7 +11767,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="213" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>625</v>
       </c>
@@ -11796,7 +11794,7 @@
       </c>
       <c r="K213" s="3"/>
     </row>
-    <row r="214" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>629</v>
       </c>
@@ -11825,7 +11823,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="215" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>637</v>
       </c>
@@ -11855,7 +11853,7 @@
       </c>
       <c r="K215" s="3"/>
     </row>
-    <row r="216" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>638</v>
       </c>
@@ -11885,7 +11883,7 @@
       </c>
       <c r="K216" s="3"/>
     </row>
-    <row r="217" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B217" s="3" t="s">
         <v>641</v>
       </c>
@@ -11915,7 +11913,7 @@
       </c>
       <c r="K217" s="3"/>
     </row>
-    <row r="218" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B218" s="33" t="s">
         <v>643</v>
       </c>
@@ -11942,11 +11940,11 @@
       </c>
       <c r="K218" s="3"/>
     </row>
-    <row r="219" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:11" x14ac:dyDescent="0.2">
       <c r="F219" s="3"/>
       <c r="K219" s="3"/>
     </row>
-    <row r="220" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>843</v>
       </c>
@@ -11969,7 +11967,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="221" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>655</v>
       </c>
@@ -11999,7 +11997,7 @@
       </c>
       <c r="K221" s="3"/>
     </row>
-    <row r="222" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>661</v>
       </c>
@@ -12029,7 +12027,7 @@
       </c>
       <c r="K222" s="3"/>
     </row>
-    <row r="223" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>664</v>
       </c>
@@ -12056,7 +12054,7 @@
       </c>
       <c r="K223" s="3"/>
     </row>
-    <row r="224" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>668</v>
       </c>
@@ -12083,7 +12081,7 @@
       </c>
       <c r="K224" s="3"/>
     </row>
-    <row r="225" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>669</v>
       </c>
@@ -12110,7 +12108,7 @@
       </c>
       <c r="K225" s="3"/>
     </row>
-    <row r="226" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>676</v>
       </c>
@@ -12140,7 +12138,7 @@
       </c>
       <c r="K226" s="3"/>
     </row>
-    <row r="227" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>677</v>
       </c>
@@ -12170,7 +12168,7 @@
       </c>
       <c r="K227" s="3"/>
     </row>
-    <row r="228" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>683</v>
       </c>
@@ -12197,7 +12195,7 @@
       </c>
       <c r="K228" s="3"/>
     </row>
-    <row r="229" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>684</v>
       </c>
@@ -12224,7 +12222,7 @@
       </c>
       <c r="K229" s="3"/>
     </row>
-    <row r="230" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>685</v>
       </c>
@@ -12251,7 +12249,7 @@
       </c>
       <c r="K230" s="3"/>
     </row>
-    <row r="231" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>690</v>
       </c>
@@ -12278,7 +12276,7 @@
       </c>
       <c r="K231" s="3"/>
     </row>
-    <row r="232" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>692</v>
       </c>
@@ -12305,7 +12303,7 @@
       </c>
       <c r="K232" s="3"/>
     </row>
-    <row r="233" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>700</v>
       </c>
@@ -12332,7 +12330,7 @@
       </c>
       <c r="K233" s="3"/>
     </row>
-    <row r="234" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>701</v>
       </c>
@@ -12359,7 +12357,7 @@
       </c>
       <c r="K234" s="3"/>
     </row>
-    <row r="235" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>702</v>
       </c>
@@ -12383,7 +12381,7 @@
       </c>
       <c r="K235" s="3"/>
     </row>
-    <row r="236" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>711</v>
       </c>
@@ -12402,7 +12400,7 @@
       <c r="F236" s="3"/>
       <c r="K236" s="3"/>
     </row>
-    <row r="237" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>716</v>
       </c>
@@ -12421,7 +12419,7 @@
       <c r="F237" s="3"/>
       <c r="K237" s="3"/>
     </row>
-    <row r="238" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>719</v>
       </c>
@@ -12440,7 +12438,7 @@
       <c r="F238" s="3"/>
       <c r="K238" s="3"/>
     </row>
-    <row r="239" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>723</v>
       </c>
@@ -12459,7 +12457,7 @@
       <c r="F239" s="3"/>
       <c r="K239" s="3"/>
     </row>
-    <row r="240" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>724</v>
       </c>
@@ -12478,7 +12476,7 @@
       <c r="F240" s="3"/>
       <c r="K240" s="3"/>
     </row>
-    <row r="241" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>727</v>
       </c>
@@ -12499,7 +12497,7 @@
       </c>
       <c r="K241" s="3"/>
     </row>
-    <row r="242" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>806</v>
       </c>
@@ -12526,7 +12524,7 @@
       </c>
       <c r="K242" s="3"/>
     </row>
-    <row r="243" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>741</v>
       </c>
@@ -12541,7 +12539,7 @@
       </c>
       <c r="K243" s="3"/>
     </row>
-    <row r="244" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>742</v>
       </c>
@@ -12562,7 +12560,7 @@
       </c>
       <c r="K244" s="3"/>
     </row>
-    <row r="245" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>743</v>
       </c>
@@ -12583,7 +12581,7 @@
       </c>
       <c r="K245" s="3"/>
     </row>
-    <row r="246" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>744</v>
       </c>
@@ -12604,7 +12602,7 @@
       </c>
       <c r="K246" s="3"/>
     </row>
-    <row r="247" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>807</v>
       </c>
@@ -12620,16 +12618,15 @@
       <c r="E247" t="s">
         <v>720</v>
       </c>
-      <c r="F247" s="35" t="s">
+      <c r="F247" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="G247" s="36"/>
       <c r="I247" t="s">
         <v>745</v>
       </c>
-      <c r="K247" s="35"/>
-    </row>
-    <row r="248" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K247" s="3"/>
+    </row>
+    <row r="248" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>825</v>
       </c>
@@ -12645,16 +12642,15 @@
       <c r="E248" t="s">
         <v>720</v>
       </c>
-      <c r="F248" s="35" t="s">
+      <c r="F248" s="3" t="s">
         <v>823</v>
       </c>
-      <c r="G248" s="36"/>
       <c r="I248" t="s">
         <v>745</v>
       </c>
-      <c r="K248" s="35"/>
-    </row>
-    <row r="249" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K248" s="3"/>
+    </row>
+    <row r="249" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A249" s="3" t="s">
         <v>827</v>
       </c>
@@ -12670,10 +12666,10 @@
       <c r="E249" t="s">
         <v>720</v>
       </c>
-      <c r="F249" s="35" t="s">
+      <c r="F249" s="3" t="s">
         <v>735</v>
       </c>
-      <c r="G249" s="36">
+      <c r="G249">
         <v>0</v>
       </c>
       <c r="H249" t="s">
@@ -12682,9 +12678,9 @@
       <c r="I249" t="s">
         <v>828</v>
       </c>
-      <c r="K249" s="35"/>
-    </row>
-    <row r="250" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K249" s="3"/>
+    </row>
+    <row r="250" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>821</v>
       </c>
@@ -12700,18 +12696,18 @@
       <c r="E250" t="s">
         <v>720</v>
       </c>
-      <c r="F250" s="35" t="s">
+      <c r="F250" s="3" t="s">
         <v>823</v>
       </c>
-      <c r="G250" s="36" t="s">
+      <c r="G250" t="s">
         <v>403</v>
       </c>
       <c r="I250" t="s">
         <v>829</v>
       </c>
-      <c r="K250" s="35"/>
-    </row>
-    <row r="251" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K250" s="3"/>
+    </row>
+    <row r="251" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>808</v>
       </c>
@@ -12727,16 +12723,15 @@
       <c r="E251" t="s">
         <v>746</v>
       </c>
-      <c r="F251" s="35" t="s">
+      <c r="F251" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="G251" s="36"/>
       <c r="I251" t="s">
         <v>829</v>
       </c>
-      <c r="K251" s="35"/>
-    </row>
-    <row r="252" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K251" s="3"/>
+    </row>
+    <row r="252" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>809</v>
       </c>
@@ -12752,10 +12747,10 @@
       <c r="E252" t="s">
         <v>746</v>
       </c>
-      <c r="F252" s="35" t="s">
+      <c r="F252" s="3" t="s">
         <v>746</v>
       </c>
-      <c r="G252" s="36" t="s">
+      <c r="G252" t="s">
         <v>815</v>
       </c>
       <c r="H252" t="s">
@@ -12764,9 +12759,9 @@
       <c r="J252" t="s">
         <v>812</v>
       </c>
-      <c r="K252" s="35"/>
-    </row>
-    <row r="253" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K252" s="3"/>
+    </row>
+    <row r="253" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>811</v>
       </c>
@@ -12782,18 +12777,18 @@
       <c r="E253" t="s">
         <v>746</v>
       </c>
-      <c r="F253" s="35" t="s">
+      <c r="F253" s="3" t="s">
         <v>813</v>
       </c>
-      <c r="G253" s="36" t="s">
+      <c r="G253" t="s">
         <v>814</v>
       </c>
       <c r="H253" t="s">
         <v>133</v>
       </c>
-      <c r="K253" s="35"/>
-    </row>
-    <row r="254" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K253" s="3"/>
+    </row>
+    <row r="254" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>747</v>
       </c>
@@ -12803,23 +12798,22 @@
       <c r="C254" t="s">
         <v>737</v>
       </c>
-      <c r="D254" s="41" t="s">
+      <c r="D254" s="35" t="s">
         <v>775</v>
       </c>
       <c r="E254" t="s">
         <v>734</v>
       </c>
-      <c r="F254" s="35" t="s">
+      <c r="F254" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="G254" s="36"/>
-      <c r="K254" s="35"/>
-    </row>
-    <row r="255" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K254" s="3"/>
+    </row>
+    <row r="255" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>748</v>
       </c>
-      <c r="B255" s="42" t="s">
+      <c r="B255" s="36" t="s">
         <v>775</v>
       </c>
       <c r="C255" t="s">
@@ -12831,11 +12825,10 @@
       <c r="E255" t="s">
         <v>734</v>
       </c>
-      <c r="F255" s="35"/>
-      <c r="G255" s="36"/>
-      <c r="K255" s="35"/>
-    </row>
-    <row r="256" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F255" s="3"/>
+      <c r="K255" s="3"/>
+    </row>
+    <row r="256" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>749</v>
       </c>
@@ -12845,19 +12838,18 @@
       <c r="C256" t="s">
         <v>256</v>
       </c>
-      <c r="D256" s="42" t="s">
+      <c r="D256" s="36" t="s">
         <v>775</v>
       </c>
       <c r="E256" t="s">
         <v>720</v>
       </c>
-      <c r="F256" s="35" t="s">
+      <c r="F256" s="3" t="s">
         <v>751</v>
       </c>
-      <c r="G256" s="36"/>
-      <c r="K256" s="35"/>
-    </row>
-    <row r="257" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K256" s="3"/>
+    </row>
+    <row r="257" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>835</v>
       </c>
@@ -12873,13 +12865,12 @@
       <c r="E257" t="s">
         <v>752</v>
       </c>
-      <c r="F257" s="35" t="s">
+      <c r="F257" s="3" t="s">
         <v>752</v>
       </c>
-      <c r="G257" s="36"/>
-      <c r="K257" s="35"/>
-    </row>
-    <row r="258" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K257" s="3"/>
+    </row>
+    <row r="258" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>774</v>
       </c>
@@ -12889,17 +12880,16 @@
       <c r="C258" t="s">
         <v>256</v>
       </c>
-      <c r="D258" s="42" t="s">
+      <c r="D258" s="36" t="s">
         <v>775</v>
       </c>
       <c r="E258" t="s">
         <v>720</v>
       </c>
-      <c r="F258" s="35"/>
-      <c r="G258" s="36"/>
-      <c r="K258" s="35"/>
-    </row>
-    <row r="259" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F258" s="3"/>
+      <c r="K258" s="3"/>
+    </row>
+    <row r="259" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>780</v>
       </c>
@@ -12915,18 +12905,18 @@
       <c r="E259" t="s">
         <v>734</v>
       </c>
-      <c r="F259" s="35" t="s">
+      <c r="F259" s="3" t="s">
         <v>746</v>
       </c>
-      <c r="G259" s="36" t="s">
+      <c r="G259" t="s">
         <v>48</v>
       </c>
       <c r="H259" t="s">
         <v>133</v>
       </c>
-      <c r="K259" s="35"/>
-    </row>
-    <row r="260" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K259" s="3"/>
+    </row>
+    <row r="260" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>773</v>
       </c>
@@ -12942,11 +12932,10 @@
       <c r="E260" t="s">
         <v>734</v>
       </c>
-      <c r="F260" s="35"/>
-      <c r="G260" s="36"/>
-      <c r="K260" s="35"/>
-    </row>
-    <row r="261" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F260" s="3"/>
+      <c r="K260" s="3"/>
+    </row>
+    <row r="261" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>772</v>
       </c>
@@ -12962,35 +12951,29 @@
       <c r="E261" t="s">
         <v>734</v>
       </c>
-      <c r="F261" s="35"/>
-      <c r="G261" s="36"/>
-      <c r="K261" s="35"/>
-    </row>
-    <row r="262" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A262" s="37" t="s">
+      <c r="F261" s="3"/>
+      <c r="K261" s="3"/>
+    </row>
+    <row r="262" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A262" t="s">
         <v>771</v>
       </c>
       <c r="B262" s="3" t="s">
         <v>754</v>
       </c>
-      <c r="C262" s="37" t="s">
+      <c r="C262" t="s">
         <v>761</v>
       </c>
-      <c r="D262" s="38" t="s">
+      <c r="D262" s="3" t="s">
         <v>762</v>
       </c>
-      <c r="E262" s="37" t="s">
+      <c r="E262" t="s">
         <v>734</v>
       </c>
-      <c r="F262" s="39"/>
-      <c r="G262" s="40"/>
-      <c r="H262" s="37"/>
-      <c r="I262" s="37"/>
-      <c r="J262" s="37"/>
-      <c r="K262" s="39"/>
-      <c r="L262" s="37"/>
-    </row>
-    <row r="263" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F262" s="3"/>
+      <c r="K262" s="3"/>
+    </row>
+    <row r="263" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>777</v>
       </c>
@@ -13003,21 +12986,21 @@
       <c r="D263" s="3" t="s">
         <v>763</v>
       </c>
-      <c r="E263" s="37" t="s">
+      <c r="E263" t="s">
         <v>734</v>
       </c>
-      <c r="F263" s="35" t="s">
+      <c r="F263" s="3" t="s">
         <v>746</v>
       </c>
-      <c r="G263" s="36" t="s">
+      <c r="G263" t="s">
         <v>48</v>
       </c>
       <c r="H263" t="s">
         <v>133</v>
       </c>
-      <c r="K263" s="35"/>
-    </row>
-    <row r="264" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K263" s="3"/>
+    </row>
+    <row r="264" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>778</v>
       </c>
@@ -13030,21 +13013,21 @@
       <c r="D264" s="3" t="s">
         <v>757</v>
       </c>
-      <c r="E264" s="37" t="s">
+      <c r="E264" t="s">
         <v>734</v>
       </c>
-      <c r="F264" s="35" t="s">
+      <c r="F264" s="3" t="s">
         <v>746</v>
       </c>
-      <c r="G264" s="36" t="s">
+      <c r="G264" t="s">
         <v>48</v>
       </c>
       <c r="H264" t="s">
         <v>133</v>
       </c>
-      <c r="K264" s="35"/>
-    </row>
-    <row r="265" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K264" s="3"/>
+    </row>
+    <row r="265" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>779</v>
       </c>
@@ -13057,21 +13040,21 @@
       <c r="D265" s="3" t="s">
         <v>764</v>
       </c>
-      <c r="E265" s="37" t="s">
+      <c r="E265" t="s">
         <v>734</v>
       </c>
-      <c r="F265" s="35" t="s">
+      <c r="F265" s="3" t="s">
         <v>746</v>
       </c>
-      <c r="G265" s="36" t="s">
+      <c r="G265" t="s">
         <v>48</v>
       </c>
       <c r="H265" t="s">
         <v>133</v>
       </c>
-      <c r="K265" s="35"/>
-    </row>
-    <row r="266" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K265" s="3"/>
+    </row>
+    <row r="266" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>770</v>
       </c>
@@ -13087,11 +13070,10 @@
       <c r="E266" t="s">
         <v>767</v>
       </c>
-      <c r="F266" s="35"/>
-      <c r="G266" s="36"/>
-      <c r="K266" s="35"/>
-    </row>
-    <row r="267" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F266" s="3"/>
+      <c r="K266" s="3"/>
+    </row>
+    <row r="267" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>769</v>
       </c>
@@ -13107,11 +13089,10 @@
       <c r="E267" t="s">
         <v>767</v>
       </c>
-      <c r="F267" s="35"/>
-      <c r="G267" s="36"/>
-      <c r="K267" s="35"/>
-    </row>
-    <row r="268" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F267" s="3"/>
+      <c r="K267" s="3"/>
+    </row>
+    <row r="268" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>782</v>
       </c>
@@ -13127,10 +13108,10 @@
       <c r="E268" t="s">
         <v>746</v>
       </c>
-      <c r="F268" s="35" t="s">
+      <c r="F268" s="3" t="s">
         <v>746</v>
       </c>
-      <c r="G268" s="36" t="s">
+      <c r="G268" t="s">
         <v>48</v>
       </c>
       <c r="H268" t="s">
@@ -13139,9 +13120,9 @@
       <c r="I268" t="s">
         <v>758</v>
       </c>
-      <c r="K268" s="35"/>
-    </row>
-    <row r="269" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K268" s="3"/>
+    </row>
+    <row r="269" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>783</v>
       </c>
@@ -13157,16 +13138,15 @@
       <c r="E269" t="s">
         <v>746</v>
       </c>
-      <c r="F269" s="35" t="s">
+      <c r="F269" s="3" t="s">
         <v>746</v>
       </c>
-      <c r="G269" s="36"/>
       <c r="J269" t="s">
         <v>784</v>
       </c>
-      <c r="K269" s="35"/>
-    </row>
-    <row r="270" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K269" s="3"/>
+    </row>
+    <row r="270" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>786</v>
       </c>
@@ -13182,13 +13162,12 @@
       <c r="E270" t="s">
         <v>746</v>
       </c>
-      <c r="F270" s="35" t="s">
+      <c r="F270" s="3" t="s">
         <v>746</v>
       </c>
-      <c r="G270" s="36"/>
-      <c r="K270" s="35"/>
-    </row>
-    <row r="271" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K270" s="3"/>
+    </row>
+    <row r="271" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>800</v>
       </c>
@@ -13204,13 +13183,12 @@
       <c r="E271" t="s">
         <v>746</v>
       </c>
-      <c r="F271" s="35" t="s">
+      <c r="F271" s="3" t="s">
         <v>746</v>
       </c>
-      <c r="G271" s="36"/>
-      <c r="K271" s="35"/>
-    </row>
-    <row r="272" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K271" s="3"/>
+    </row>
+    <row r="272" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>801</v>
       </c>
@@ -13226,13 +13204,12 @@
       <c r="E272" t="s">
         <v>746</v>
       </c>
-      <c r="F272" s="35" t="s">
+      <c r="F272" s="3" t="s">
         <v>746</v>
       </c>
-      <c r="G272" s="36"/>
-      <c r="K272" s="35"/>
-    </row>
-    <row r="273" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K272" s="3"/>
+    </row>
+    <row r="273" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>802</v>
       </c>
@@ -13248,13 +13225,12 @@
       <c r="E273" t="s">
         <v>746</v>
       </c>
-      <c r="F273" s="35" t="s">
+      <c r="F273" s="3" t="s">
         <v>746</v>
       </c>
-      <c r="G273" s="36"/>
-      <c r="K273" s="35"/>
-    </row>
-    <row r="274" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K273" s="3"/>
+    </row>
+    <row r="274" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>803</v>
       </c>
@@ -13270,13 +13246,12 @@
       <c r="E274" t="s">
         <v>746</v>
       </c>
-      <c r="F274" s="35" t="s">
+      <c r="F274" s="3" t="s">
         <v>746</v>
       </c>
-      <c r="G274" s="36"/>
-      <c r="K274" s="35"/>
-    </row>
-    <row r="275" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K274" s="3"/>
+    </row>
+    <row r="275" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>804</v>
       </c>
@@ -13292,13 +13267,12 @@
       <c r="E275" t="s">
         <v>746</v>
       </c>
-      <c r="F275" s="35" t="s">
+      <c r="F275" s="3" t="s">
         <v>746</v>
       </c>
-      <c r="G275" s="36"/>
-      <c r="K275" s="35"/>
-    </row>
-    <row r="276" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K275" s="3"/>
+    </row>
+    <row r="276" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>805</v>
       </c>
@@ -13314,13 +13288,12 @@
       <c r="E276" t="s">
         <v>746</v>
       </c>
-      <c r="F276" s="35" t="s">
+      <c r="F276" s="3" t="s">
         <v>746</v>
       </c>
-      <c r="G276" s="36"/>
-      <c r="K276" s="35"/>
-    </row>
-    <row r="277" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K276" s="3"/>
+    </row>
+    <row r="277" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>816</v>
       </c>
@@ -13336,15 +13309,15 @@
       <c r="E277" t="s">
         <v>746</v>
       </c>
-      <c r="F277" s="35" t="s">
+      <c r="F277" s="3" t="s">
         <v>818</v>
       </c>
-      <c r="G277" s="36" t="s">
+      <c r="G277" t="s">
         <v>814</v>
       </c>
-      <c r="K277" s="35"/>
-    </row>
-    <row r="278" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K277" s="3"/>
+    </row>
+    <row r="278" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>817</v>
       </c>
@@ -13357,13 +13330,13 @@
       <c r="E278" t="s">
         <v>746</v>
       </c>
-      <c r="F278" s="35" t="s">
+      <c r="F278" s="3" t="s">
         <v>746</v>
       </c>
-      <c r="G278" s="36" t="s">
+      <c r="G278" t="s">
         <v>403</v>
       </c>
-      <c r="K278" s="35"/>
+      <c r="K278" s="3"/>
     </row>
     <row r="279" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
@@ -13372,10 +13345,10 @@
       <c r="B279" s="3" t="s">
         <v>619</v>
       </c>
-      <c r="F279" s="35" t="s">
+      <c r="F279" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="G279" s="36" t="s">
+      <c r="G279" t="s">
         <v>837</v>
       </c>
       <c r="H279" t="s">
@@ -13384,7 +13357,7 @@
       <c r="I279" t="s">
         <v>830</v>
       </c>
-      <c r="K279" s="35"/>
+      <c r="K279" s="3"/>
     </row>
     <row r="280" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
@@ -13473,7 +13446,16 @@
         <v>849</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>619</v>
+        <v>40</v>
+      </c>
+      <c r="C285" t="s">
+        <v>865</v>
+      </c>
+      <c r="D285" s="3" t="s">
+        <v>863</v>
+      </c>
+      <c r="E285" t="s">
+        <v>720</v>
       </c>
       <c r="F285" t="s">
         <v>35</v>
@@ -13487,73 +13469,76 @@
     </row>
     <row r="286" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
-        <v>850</v>
+        <v>864</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>619</v>
-      </c>
-      <c r="F286" t="s">
-        <v>35</v>
-      </c>
-      <c r="G286" t="s">
-        <v>851</v>
-      </c>
-      <c r="H286" t="s">
-        <v>133</v>
-      </c>
-      <c r="J286" t="s">
-        <v>852</v>
+        <v>863</v>
+      </c>
+      <c r="C286" t="s">
+        <v>256</v>
+      </c>
+      <c r="D286" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E286" t="s">
+        <v>359</v>
+      </c>
+      <c r="F286" s="37" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="287" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
-        <v>853</v>
+        <v>850</v>
       </c>
       <c r="B287" s="3" t="s">
         <v>619</v>
       </c>
       <c r="F287" t="s">
-        <v>738</v>
+        <v>35</v>
       </c>
       <c r="G287" t="s">
-        <v>854</v>
+        <v>851</v>
       </c>
       <c r="H287" t="s">
         <v>133</v>
       </c>
       <c r="J287" t="s">
-        <v>855</v>
+        <v>852</v>
       </c>
     </row>
     <row r="288" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
-        <v>856</v>
+        <v>853</v>
       </c>
       <c r="B288" s="3" t="s">
         <v>619</v>
       </c>
       <c r="F288" t="s">
-        <v>735</v>
+        <v>738</v>
       </c>
       <c r="G288" t="s">
-        <v>632</v>
+        <v>854</v>
       </c>
       <c r="H288" t="s">
         <v>133</v>
       </c>
+      <c r="J288" t="s">
+        <v>855</v>
+      </c>
     </row>
     <row r="289" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="B289" s="3" t="s">
         <v>619</v>
       </c>
       <c r="F289" t="s">
-        <v>858</v>
+        <v>735</v>
       </c>
       <c r="G289" t="s">
-        <v>403</v>
+        <v>632</v>
       </c>
       <c r="H289" t="s">
         <v>133</v>
@@ -13561,7 +13546,7 @@
     </row>
     <row r="290" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="B290" s="3" t="s">
         <v>619</v>
@@ -13578,27 +13563,24 @@
     </row>
     <row r="291" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="B291" s="3" t="s">
         <v>619</v>
       </c>
       <c r="F291" t="s">
-        <v>39</v>
+        <v>858</v>
       </c>
       <c r="G291" t="s">
-        <v>814</v>
+        <v>403</v>
       </c>
       <c r="H291" t="s">
         <v>133</v>
       </c>
-      <c r="J291" t="s">
-        <v>203</v>
-      </c>
     </row>
     <row r="292" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="B292" s="3" t="s">
         <v>619</v>
@@ -13613,6 +13595,26 @@
         <v>133</v>
       </c>
       <c r="J292" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="293" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A293" t="s">
+        <v>862</v>
+      </c>
+      <c r="B293" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="F293" t="s">
+        <v>39</v>
+      </c>
+      <c r="G293" t="s">
+        <v>814</v>
+      </c>
+      <c r="H293" t="s">
+        <v>133</v>
+      </c>
+      <c r="J293" t="s">
         <v>861</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Major revisions of SDV
</commit_message>
<xml_diff>
--- a/data/uac_cables.xlsx
+++ b/data/uac_cables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/donert/Documents/UACTech/SystemDocumentation/github/uactechdoc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD8DEE5-8882-2C45-8BA7-5DA80845CDC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF79886-F4A6-034F-BD84-AFE7332F3FBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{288904EE-D384-EA4C-9B98-052B972FB267}"/>
+    <workbookView xWindow="-40" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{288904EE-D384-EA4C-9B98-052B972FB267}"/>
   </bookViews>
   <sheets>
     <sheet name="Cables" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -2855,7 +2855,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2897,13 +2897,6 @@
     <xf numFmtId="49" fontId="2" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5150,7 +5143,70 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C06BC8A8-0124-C241-ADED-B97F2CE891ED}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{331FD294-EE6F-3D4E-A534-813A4D9D566E}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="E5:F10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="12">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="7"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Tag" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C06BC8A8-0124-C241-ADED-B97F2CE891ED}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B29" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField dataField="1" showAll="0"/>
@@ -5301,72 +5357,15 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{331FD294-EE6F-3D4E-A534-813A4D9D566E}" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="E5:F10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="12">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="7"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Tag" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD7E3698-8860-904B-8BDB-00EF1039C49C}" name="Table1" displayName="Table1" ref="A1:L293" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="5">
-  <autoFilter ref="A1:L293" xr:uid="{BD7E3698-8860-904B-8BDB-00EF1039C49C}"/>
+  <autoFilter ref="A1:L293" xr:uid="{BD7E3698-8860-904B-8BDB-00EF1039C49C}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="ZVKU-A003"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{4D442337-BE86-B24A-84A4-338FB80A6A49}" name="Tag"/>
     <tableColumn id="2" xr3:uid="{74A36D7B-C989-3B4B-B1E5-AB1FA4C2DD45}" name="SrcTag" dataDxfId="4"/>
@@ -5685,10 +5684,10 @@
   <dimension ref="A1:L293"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B258" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H284" sqref="H284"/>
+      <selection pane="bottomRight" activeCell="D297" sqref="D297"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5742,7 +5741,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>25</v>
       </c>
@@ -5785,7 +5784,7 @@
         <v>cdmua001:Key -&gt; zviue004:sw1 [label='2307-1800']</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>4</v>
       </c>
@@ -5820,7 +5819,7 @@
         <v>cdmua001:Fill -&gt; zviue004:sw2 [label='2307-1801']</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>5</v>
       </c>
@@ -5855,7 +5854,7 @@
         <v>cdmua001:ProjA -&gt; zviue004:sw4 [label='2307-1802']</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>6</v>
       </c>
@@ -5890,7 +5889,7 @@
         <v>cdmua001:ProjB -&gt; zviue004:sw6 [label='2307-1803']</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>7</v>
       </c>
@@ -5925,7 +5924,7 @@
         <v>cdmua001:ProjC -&gt; zviue004:sw8 [label='2307-1804']</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>8</v>
       </c>
@@ -5993,7 +5992,7 @@
         <v>zvkua003:PGM -&gt; zviua005:sdi [label='2307-1806']</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
         <v>10</v>
       </c>
@@ -6063,7 +6062,7 @@
         <v>zvkua003:aux -&gt; zviud001:sdi in [label='2307-1808']</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
         <v>12</v>
       </c>
@@ -6106,7 +6105,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>13</v>
       </c>
@@ -6151,7 +6150,7 @@
         <v>zviue004:sdi1 -&gt; 23081204:sdi in [label='2307-1810']</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>14</v>
       </c>
@@ -6188,7 +6187,7 @@
         <v>zviue004:sdi2 -&gt; 23081205:sdi in [label='2307-1811']</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>15</v>
       </c>
@@ -6223,7 +6222,7 @@
         <v>zviue004:sdi4 -&gt; zviug003:sdi in [label='2307-1812']</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
         <v>16</v>
       </c>
@@ -6258,7 +6257,7 @@
         <v>zviue004:sdi6 -&gt; zviug004:sdi in [label='2307-1813']</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>17</v>
       </c>
@@ -6293,7 +6292,7 @@
         <v>zviue004:sdi8 -&gt; zviug005:sdi in [label='2307-1814']</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
         <v>18</v>
       </c>
@@ -6328,7 +6327,7 @@
         <v>zviue004:sdi3 -&gt; zviue001:sdi in [label='2307-1815']</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>19</v>
       </c>
@@ -6349,7 +6348,7 @@
         <v>: -&gt; : [label='2307-1816']</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
         <v>20</v>
       </c>
@@ -6370,7 +6369,7 @@
         <v>: -&gt; : [label='2307-1817']</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>21</v>
       </c>
@@ -6391,7 +6390,7 @@
         <v>: -&gt; : [label='2307-1818']</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
         <v>22</v>
       </c>
@@ -6418,7 +6417,7 @@
         <v>not used: -&gt; : [label='2307-1819']</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>23</v>
       </c>
@@ -6447,7 +6446,7 @@
         <v>unused: -&gt; : [label='2307-1820']</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
         <v>24</v>
       </c>
@@ -6476,7 +6475,7 @@
         <v>unused: -&gt; : [label='2307-1821']</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>30</v>
       </c>
@@ -6505,7 +6504,7 @@
         <v>unused: -&gt; : [label='2307-1822']</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
         <v>52</v>
       </c>
@@ -6540,7 +6539,7 @@
         <v>zviua008:hdmi -&gt; zvkua003:in4 [label='2307-1828']</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>47</v>
       </c>
@@ -6573,7 +6572,7 @@
         <v>cdmua001:usbc -&gt; zviue005:usbc [label='2307-1824']</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="23" t="s">
         <v>49</v>
       </c>
@@ -6602,7 +6601,7 @@
         <v>unused: -&gt; : [label='2307-1825']</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
         <v>50</v>
       </c>
@@ -6631,7 +6630,7 @@
         <v>unused: -&gt; : [label='2307-1826']</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
         <v>64</v>
       </c>
@@ -6664,7 +6663,7 @@
         <v>zviua004:usb -&gt; cumug001:usb_3 [label='2307-2100']</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
         <v>65</v>
       </c>
@@ -6699,7 +6698,7 @@
         <v>cumug001:ndi -&gt; cumue001:obs [label='2307-2101']</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="s">
         <v>66</v>
       </c>
@@ -6732,7 +6731,7 @@
         <v>camera left: -&gt; cumue001:obs [label='2307-2102']</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>67</v>
       </c>
@@ -6765,7 +6764,7 @@
         <v>camera centre: -&gt; cumue001:obs [label='2307-2103']</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="15" t="s">
         <v>68</v>
       </c>
@@ -6798,7 +6797,7 @@
         <v>camera right: -&gt; cumue001:obs [label='2307-2104']</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
         <v>69</v>
       </c>
@@ -6831,7 +6830,7 @@
         <v>cdmua001:ndi -&gt; cumue001:obs [label='2307-2105']</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="15" t="s">
         <v>81</v>
       </c>
@@ -6864,7 +6863,7 @@
         <v>zvkua001:out_5_hdmi -&gt; zviuc001:hdmi in [label='2307-2300']</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
         <v>85</v>
       </c>
@@ -6901,7 +6900,7 @@
         <v>zviuc001:hdmi out -&gt; zvkua003:in1 [label='2307-2301']</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="15" t="s">
         <v>88</v>
       </c>
@@ -6936,7 +6935,7 @@
         <v>zvcua001:sdi -&gt; zvkua003:in5 [label='2307-2304']</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
         <v>87</v>
       </c>
@@ -6971,7 +6970,7 @@
         <v>zvcua002:sdi -&gt; zvkua003:in6 [label='2307-2303']</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="15" t="s">
         <v>86</v>
       </c>
@@ -7006,7 +7005,7 @@
         <v>zvcua003:sdi -&gt; zvkua003:in7 [label='2307-2302']</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
         <v>95</v>
       </c>
@@ -7043,7 +7042,7 @@
         <v>23072306:barrel -&gt; zvkua003:in8 [label='2307-2305']</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="15" t="s">
         <v>96</v>
       </c>
@@ -7078,7 +7077,7 @@
         <v>z150:sdi -&gt; 23072305:barrel [label='2307-2306']</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
         <v>97</v>
       </c>
@@ -7105,7 +7104,7 @@
         <v>: -&gt; : [label='2307-2307']</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="15" t="s">
         <v>101</v>
       </c>
@@ -7140,7 +7139,7 @@
         <v>zvkua004:sw -&gt; zvcua001:sw [label='2307-2308']</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
         <v>102</v>
       </c>
@@ -7183,7 +7182,7 @@
         <v>zvkua004:sw -&gt; zvcua002:sw [label='2307-2309']</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="15" t="s">
         <v>103</v>
       </c>
@@ -7218,7 +7217,7 @@
         <v>zvkua004:sw -&gt; zvcua003:sw [label='2307-2310']</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
         <v>106</v>
       </c>
@@ -7237,7 +7236,7 @@
         <v>: -&gt; : [label='2307-2311']</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="15" t="s">
         <v>109</v>
       </c>
@@ -7256,7 +7255,7 @@
         <v>: -&gt; : [label='2307-2312']</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
         <v>110</v>
       </c>
@@ -7275,7 +7274,7 @@
         <v>: -&gt; : [label='2307-2313']</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="15" t="s">
         <v>111</v>
       </c>
@@ -7308,7 +7307,7 @@
         <v>zvkua001:out_4_HDbT -&gt; zvvu0001:HDbT [label='2307-2314']</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
         <v>120</v>
       </c>
@@ -7343,7 +7342,7 @@
         <v>zvkua001:out_7_HDbT -&gt; zviua001:HDbT [label='2307-2315']</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="15" t="s">
         <v>121</v>
       </c>
@@ -7376,7 +7375,7 @@
         <v>zviua001:hdmi -&gt; zvvulobby tv :hdmi 1 [label='2307-2316']</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
         <v>122</v>
       </c>
@@ -7403,7 +7402,7 @@
         <v>: -&gt; : [label='2307-2317']</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="15" t="s">
         <v>126</v>
       </c>
@@ -7438,7 +7437,7 @@
         <v>zvkua001:out_8_HDbT -&gt; zviua002:HDbT [label='2307-2318']</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="11" t="s">
         <v>411</v>
       </c>
@@ -7469,7 +7468,7 @@
         <v>zviua002:hdmi -&gt; 23082900:input [label='2308-3001']</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="15" t="s">
         <v>129</v>
       </c>
@@ -7496,7 +7495,7 @@
         <v>: -&gt; : [label='2307-2320']</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
         <v>134</v>
       </c>
@@ -7529,7 +7528,7 @@
         <v>cdmua001:PP_Front_SW -&gt; hdmi_dongle: [label='2307-3000']</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="15" t="s">
         <v>136</v>
       </c>
@@ -7562,7 +7561,7 @@
         <v>zvrua001:OutB -&gt; zvrua002:SDI In [label='2307-3001']</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
         <v>138</v>
       </c>
@@ -7595,7 +7594,7 @@
         <v>zvrua001:OutA -&gt; zviua004:SDI In [label='2307-3002']</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="15" t="s">
         <v>141</v>
       </c>
@@ -7630,7 +7629,7 @@
         <v>zviua004:hdmi out -&gt; zvkua001:in7 [label='2307-3003']</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="11" t="s">
         <v>142</v>
       </c>
@@ -7723,7 +7722,7 @@
         <v>zvkua003:out6 -&gt; zviud002:sdi in [label='2307-3006']</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="15" t="s">
         <v>147</v>
       </c>
@@ -7756,7 +7755,7 @@
         <v>zviud001:hdmi -&gt; zviua004:hdmi in [label='2307-3007']</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">
         <v>160</v>
       </c>
@@ -7791,7 +7790,7 @@
         <v>zviua005:hdmi -&gt; zvkua001:in6 [label='2308-0800']</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="15" t="s">
         <v>203</v>
       </c>
@@ -7823,7 +7822,7 @@
         <v>unused:  -&gt; : [label='2308-0004']</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="11" t="s">
         <v>204</v>
       </c>
@@ -7856,7 +7855,7 @@
         <v>frontguest: -&gt; 23080003:InputC [label='2308-0005']</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="15" t="s">
         <v>205</v>
       </c>
@@ -7891,7 +7890,7 @@
         <v>cdwua002:HdmiOut -&gt; 23080002:In2 [label='2308-0006']</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="11" t="s">
         <v>206</v>
       </c>
@@ -7924,7 +7923,7 @@
         <v>rearguest:hdmi_out -&gt; 23080002:In1 [label='2308-0007']</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="15" t="s">
         <v>207</v>
       </c>
@@ -7957,7 +7956,7 @@
         <v>cdwua002:vga -&gt; vmnu0029:vga [label='2308-0009']</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="11" t="s">
         <v>208</v>
       </c>
@@ -7990,7 +7989,7 @@
         <v>cdwua002:usb -&gt; 23080008:usb [label='2308-0010']</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="11" t="s">
         <v>183</v>
       </c>
@@ -8023,7 +8022,7 @@
         <v>zviug003:hdmi_out -&gt; zvkua001:in1 [label='2308-0915']</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="15" t="s">
         <v>184</v>
       </c>
@@ -8056,7 +8055,7 @@
         <v>zviug004:hdmi_out -&gt; zvkua001:in2 [label='2308-0916']</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="11" t="s">
         <v>185</v>
       </c>
@@ -8089,7 +8088,7 @@
         <v>zviug005:hdmi_out -&gt; zvkua001:in3 [label='2308-0917']</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="15" t="s">
         <v>186</v>
       </c>
@@ -8119,7 +8118,7 @@
       <c r="K74" s="17"/>
       <c r="L74" s="18"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="11" t="s">
         <v>193</v>
       </c>
@@ -8160,7 +8159,7 @@
         <v>zvkua001:out_1_HDbT -&gt; zvvua001:InputD [label='PROJ0001']</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="15" t="s">
         <v>194</v>
       </c>
@@ -8201,7 +8200,7 @@
         <v>zvkua001:out_2_HDbT -&gt; zvvua002:InputD [label='PROJ0002']</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="11" t="s">
         <v>195</v>
       </c>
@@ -8242,7 +8241,7 @@
         <v>zvkua001:out_3_HDbT -&gt; zvvua003:InputD [label='PROJ0003']</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="15" t="s">
         <v>201</v>
       </c>
@@ -8285,7 +8284,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="11" t="s">
         <v>214</v>
       </c>
@@ -8326,7 +8325,7 @@
         <v>cumue001:usba_2 -&gt; 23081110:usb_in [label='2308-1111']</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="15" t="s">
         <v>229</v>
       </c>
@@ -8359,7 +8358,7 @@
         <v>23081110:usb_1 -&gt; 23081104:usb [label='2308-1112']</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="11" t="s">
         <v>230</v>
       </c>
@@ -8392,7 +8391,7 @@
         <v>23081110:usb_2 -&gt; 23081105:usb [label='2308-1113']</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="15" t="s">
         <v>231</v>
       </c>
@@ -8429,7 +8428,7 @@
         <v>cumue001:usbc -&gt; 23081106:hdmi [label='2308-1114']</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="11" t="s">
         <v>232</v>
       </c>
@@ -8464,7 +8463,7 @@
         <v>cumue001:hdmi -&gt; 23081107:hdmi [label='2308-1115']</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="15" t="s">
         <v>233</v>
       </c>
@@ -8497,7 +8496,7 @@
         <v>23081110:usb  -&gt; 23081103:usb [label='2308-1116']</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="11" t="s">
         <v>234</v>
       </c>
@@ -8538,7 +8537,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="15" t="s">
         <v>235</v>
       </c>
@@ -8579,7 +8578,7 @@
         <v>23081100:port3 -&gt; zaiue002:ether [label='2308-1118']</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="11" t="s">
         <v>236</v>
       </c>
@@ -8620,7 +8619,7 @@
         <v>23081100:port4 -&gt; daw_guest:ether [label='2308-1119']</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="15" t="s">
         <v>237</v>
       </c>
@@ -8656,7 +8655,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="11" t="s">
         <v>238</v>
       </c>
@@ -8740,7 +8739,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="11" t="s">
         <v>244</v>
       </c>
@@ -8783,7 +8782,7 @@
         <v>23081124:ch1 -&gt; zvkua003:ch1_audio [label='2308-1124L']</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="15" t="s">
         <v>248</v>
       </c>
@@ -8818,7 +8817,7 @@
         <v>23081124:ch2 -&gt; zvkua003:ch2_audio [label='2308-1124R']</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="11" t="s">
         <v>704</v>
       </c>
@@ -8836,7 +8835,7 @@
         <v>: -&gt; : [label='x93']</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="15" t="s">
         <v>705</v>
       </c>
@@ -8854,7 +8853,7 @@
         <v>: -&gt; : [label='x94']</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="11" t="s">
         <v>706</v>
       </c>
@@ -8887,7 +8886,7 @@
         <v>zakua001:aux4 -&gt; 23080008:Mic_In [label='x95']</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="15"/>
       <c r="B96" s="16" t="s">
         <v>182</v>
@@ -8918,7 +8917,7 @@
         <v>23080906:out -&gt; zakua001:ch_12 [label='']</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="11" t="s">
         <v>702</v>
       </c>
@@ -8949,7 +8948,7 @@
         <v>rearguest:left -&gt; zakua001:ch_13 [label='x97']</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="15" t="s">
         <v>703</v>
       </c>
@@ -8980,7 +8979,7 @@
         <v>rearguest:right -&gt; zakua001:ch_14 [label='x98']</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="11"/>
       <c r="B99" s="12" t="s">
         <v>167</v>
@@ -9009,7 +9008,7 @@
         <v>cdwua002:left -&gt; zakua001:ch_15 [label='']</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="15"/>
       <c r="B100" s="16" t="s">
         <v>167</v>
@@ -9038,7 +9037,7 @@
         <v>cdwua002:right -&gt; zakua001:ch_16 [label='']</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="11"/>
       <c r="B101" s="12" t="s">
         <v>72</v>
@@ -9077,7 +9076,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="15"/>
       <c r="B102" s="16" t="s">
         <v>72</v>
@@ -9116,7 +9115,7 @@
         <v>cumug001:usb_2 -&gt; zviug001:usb_in [label='']</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="11"/>
       <c r="B103" s="12" t="s">
         <v>72</v>
@@ -9157,7 +9156,7 @@
         <v>cumug001:usb_1 -&gt; 23081202:usb [label='']</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="15"/>
       <c r="B104" s="16" t="s">
         <v>260</v>
@@ -9198,7 +9197,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="11" t="s">
         <v>336</v>
       </c>
@@ -9241,7 +9240,7 @@
         <v>23081204:sdi_out -&gt; zviue003:sdi_in [label='2307-1201']</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="15" t="s">
         <v>337</v>
       </c>
@@ -9276,7 +9275,7 @@
         <v>23081205:sdi_out -&gt; zviua008:sdi_in [label='2307-1202']</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="11" t="s">
         <v>51</v>
       </c>
@@ -9311,7 +9310,7 @@
         <v>zviue003:hdmi_out -&gt; zvkua003:in2 [label='2307-1827']</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="15"/>
       <c r="B108" s="16" t="s">
         <v>282</v>
@@ -9342,7 +9341,7 @@
         <v>cdwu0009:vga -&gt; mon:vga [label='']</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="11" t="s">
         <v>284</v>
       </c>
@@ -9377,7 +9376,7 @@
         <v>prwall3:label3 -&gt; 23081100:port1 [label='2308-2001']</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="15" t="s">
         <v>295</v>
       </c>
@@ -9410,7 +9409,7 @@
         <v>23081102:Right -&gt; 23082003:Right [label='2308-2002']</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="11" t="s">
         <v>306</v>
       </c>
@@ -9443,7 +9442,7 @@
         <v>patchpanel:a -&gt; prwall3:b1 [label='a']</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="15" t="s">
         <v>307</v>
       </c>
@@ -9476,7 +9475,7 @@
         <v>modem:c -&gt; router:d [label='b']</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="11" t="s">
         <v>308</v>
       </c>
@@ -9509,7 +9508,7 @@
         <v>router:e -&gt; nscua001:f [label='c']</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="15" t="s">
         <v>313</v>
       </c>
@@ -9542,7 +9541,7 @@
         <v>nscua001:h -&gt; patchpanel:i [label='g']</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="11"/>
       <c r="B115" s="12" t="s">
         <v>305</v>
@@ -9569,7 +9568,7 @@
         <v>nscua001:a  -&gt; nscua002:f [label='']</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="15"/>
       <c r="B116" s="16" t="s">
         <v>305</v>
@@ -9596,7 +9595,7 @@
         <v>nscua001:b  -&gt; nscua005:g [label='']</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="11"/>
       <c r="B117" s="12" t="s">
         <v>324</v>
@@ -9621,7 +9620,7 @@
         <v>nscua005:c  -&gt; nscua003:h  [label='']</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="15"/>
       <c r="B118" s="16" t="s">
         <v>326</v>
@@ -9650,7 +9649,7 @@
         <v>nscua003:d  -&gt; nscua004:i [label='']</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="11"/>
       <c r="B119" s="12" t="s">
         <v>327</v>
@@ -9675,7 +9674,7 @@
         <v>nscua004:e  -&gt; 23081124:ether [label='']</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="15" t="s">
         <v>370</v>
       </c>
@@ -9708,7 +9707,7 @@
         <v>cumug001:usb -&gt; zviuc002:usbc [label='future1']</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="15" t="s">
         <v>373</v>
       </c>
@@ -9741,7 +9740,7 @@
         <v>cdwu0009:hdmi_out -&gt; zvkua001:in5 [label='2308-2500']</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="11" t="s">
         <v>376</v>
       </c>
@@ -9776,7 +9775,7 @@
         <v>zviue001:hdmi_out -&gt; zvkua001:in4 [label='2308-2501']</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="15" t="s">
         <v>377</v>
       </c>
@@ -9805,7 +9804,7 @@
         <v>not used: -&gt; : [label='2308-2502']</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="11" t="s">
         <v>380</v>
       </c>
@@ -9834,7 +9833,7 @@
         <v>not used: -&gt; : [label='2308-2503']</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="15" t="s">
         <v>387</v>
       </c>
@@ -9861,7 +9860,7 @@
         <v>not used: -&gt; : [label='2308-2504']</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="11" t="s">
         <v>388</v>
       </c>
@@ -9896,7 +9895,7 @@
         <v>ncsua004:portxx -&gt; cdmua001:ether [label='2308-2600']</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="15" t="s">
         <v>389</v>
       </c>
@@ -9921,7 +9920,7 @@
         <v>not used: -&gt; : [label='2308-2700']</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="11" t="s">
         <v>390</v>
       </c>
@@ -9946,7 +9945,7 @@
         <v>not used: -&gt; : [label='2308-2701']</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="15" t="s">
         <v>391</v>
       </c>
@@ -9971,7 +9970,7 @@
         <v>unused: -&gt; : [label='2308-2702']</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="11" t="s">
         <v>399</v>
       </c>
@@ -10008,7 +10007,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="15" t="s">
         <v>22</v>
       </c>
@@ -10051,7 +10050,7 @@
         <v>23082900:output2 -&gt; zvvu0003:hdmi1 [label='2307-1819']</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="11" t="s">
         <v>410</v>
       </c>
@@ -10092,7 +10091,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="15" t="s">
         <v>407</v>
       </c>
@@ -10133,7 +10132,7 @@
         <v>zvkua001:out6 -&gt; unknown:unk [label='future135']</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="11"/>
       <c r="B134" s="12"/>
       <c r="C134" s="13"/>
@@ -10152,7 +10151,7 @@
         <v>: -&gt; :unk [label='']</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="15" t="s">
         <v>415</v>
       </c>
@@ -10187,7 +10186,7 @@
         <v>zamua001:ch1 -&gt; zaiub001:s2_in01 [label='2309-1001']</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="11" t="s">
         <v>540</v>
       </c>
@@ -10222,7 +10221,7 @@
         <v>zamua001:ch2 -&gt; zaiub001:s2_in02 [label='2309-1002']</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" s="15" t="s">
         <v>541</v>
       </c>
@@ -10257,7 +10256,7 @@
         <v>zamua001:ch3 -&gt; zaiub001:s2_in03 [label='2309-1003']</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="11" t="s">
         <v>542</v>
       </c>
@@ -10292,7 +10291,7 @@
         <v>zamua001:ch4 -&gt; zaiub001:s2_in04 [label='2309-1004']</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="15" t="s">
         <v>543</v>
       </c>
@@ -10327,7 +10326,7 @@
         <v>zamub001:ch1 -&gt; zaiub001:s2_in05 [label='2309-1005']</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="11" t="s">
         <v>544</v>
       </c>
@@ -10362,7 +10361,7 @@
         <v>zamub001:ch2 -&gt; zaiub001:s2_in06 [label='2309-1006']</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="15" t="s">
         <v>545</v>
       </c>
@@ -10397,7 +10396,7 @@
         <v>zamub001:ch3 -&gt; zaiub001:s2_in07 [label='2309-1007']</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="11" t="s">
         <v>546</v>
       </c>
@@ -10432,7 +10431,7 @@
         <v>zamub001:ch4 -&gt; zaiub001:s2_in08 [label='2309-1008']</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="15" t="s">
         <v>547</v>
       </c>
@@ -10467,7 +10466,7 @@
         <v>zamub002:ch1 -&gt; zaiub001:s2_in09 [label='2309-1009']</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="11" t="s">
         <v>548</v>
       </c>
@@ -10502,7 +10501,7 @@
         <v>zamub002:ch2 -&gt; zaiub001:s2_in10 [label='2309-1010']</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="15" t="s">
         <v>549</v>
       </c>
@@ -10537,7 +10536,7 @@
         <v>zamub002:ch3 -&gt; zaiub001:s2_in11 [label='2309-1011']</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="11" t="s">
         <v>550</v>
       </c>
@@ -10572,7 +10571,7 @@
         <v>zamub002:ch4 -&gt; zaiub001:s2_in12 [label='2309-1012']</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="15" t="s">
         <v>551</v>
       </c>
@@ -10607,7 +10606,7 @@
         <v>zamub003:ch4 -&gt; zaiub001:s2___ [label='2309-1013']</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" s="11" t="s">
         <v>552</v>
       </c>
@@ -10642,7 +10641,7 @@
         <v>zamub002:ch3 -&gt; zaiub002:s2_in01 [label='2309-1014']</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" s="9" t="s">
         <v>553</v>
       </c>
@@ -10677,7 +10676,7 @@
         <v>zamub002:ch4 -&gt; zaiub002:s2_in02 [label='2309-1015']</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>554</v>
       </c>
@@ -10710,7 +10709,7 @@
         <v>zamub003:ch1 -&gt; zaiub002:s2_in03 [label='2309-1016']</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>555</v>
       </c>
@@ -10743,7 +10742,7 @@
         <v>zamub003:ch2 -&gt; zaiub002:s2_in04 [label='2309-1017']</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>556</v>
       </c>
@@ -10776,7 +10775,7 @@
         <v>zamub003:ch3 -&gt; zaiub002:s2_in05 [label='2309-1018']</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>557</v>
       </c>
@@ -10805,7 +10804,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>558</v>
       </c>
@@ -10831,7 +10830,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>559</v>
       </c>
@@ -10857,7 +10856,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" s="8" t="s">
         <v>560</v>
       </c>
@@ -10883,7 +10882,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>561</v>
       </c>
@@ -10909,7 +10908,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>562</v>
       </c>
@@ -10935,7 +10934,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>563</v>
       </c>
@@ -10961,7 +10960,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>564</v>
       </c>
@@ -10987,7 +10986,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>565</v>
       </c>
@@ -11013,7 +11012,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>566</v>
       </c>
@@ -11039,7 +11038,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>567</v>
       </c>
@@ -11065,7 +11064,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>568</v>
       </c>
@@ -11091,7 +11090,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>569</v>
       </c>
@@ -11117,7 +11116,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>570</v>
       </c>
@@ -11143,7 +11142,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>571</v>
       </c>
@@ -11169,7 +11168,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>572</v>
       </c>
@@ -11195,7 +11194,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>573</v>
       </c>
@@ -11221,7 +11220,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>574</v>
       </c>
@@ -11247,7 +11246,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>575</v>
       </c>
@@ -11273,7 +11272,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>576</v>
       </c>
@@ -11299,7 +11298,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>577</v>
       </c>
@@ -11325,7 +11324,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>578</v>
       </c>
@@ -11351,7 +11350,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>579</v>
       </c>
@@ -11377,7 +11376,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>580</v>
       </c>
@@ -11397,7 +11396,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>581</v>
       </c>
@@ -11417,7 +11416,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>582</v>
       </c>
@@ -11437,7 +11436,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>583</v>
       </c>
@@ -11457,7 +11456,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>584</v>
       </c>
@@ -11477,7 +11476,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>585</v>
       </c>
@@ -11497,7 +11496,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>586</v>
       </c>
@@ -11517,7 +11516,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>587</v>
       </c>
@@ -11537,7 +11536,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>588</v>
       </c>
@@ -11557,7 +11556,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>589</v>
       </c>
@@ -11577,7 +11576,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>590</v>
       </c>
@@ -11597,7 +11596,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>591</v>
       </c>
@@ -11617,7 +11616,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>592</v>
       </c>
@@ -11637,7 +11636,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>593</v>
       </c>
@@ -11657,7 +11656,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>594</v>
       </c>
@@ -11677,7 +11676,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>595</v>
       </c>
@@ -11697,7 +11696,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>596</v>
       </c>
@@ -11717,7 +11716,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>597</v>
       </c>
@@ -11737,7 +11736,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>598</v>
       </c>
@@ -11757,7 +11756,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>599</v>
       </c>
@@ -11777,7 +11776,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>600</v>
       </c>
@@ -11797,7 +11796,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>601</v>
       </c>
@@ -11817,7 +11816,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>602</v>
       </c>
@@ -11837,7 +11836,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>603</v>
       </c>
@@ -11857,7 +11856,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>604</v>
       </c>
@@ -11877,7 +11876,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>605</v>
       </c>
@@ -11897,7 +11896,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>606</v>
       </c>
@@ -11917,7 +11916,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>607</v>
       </c>
@@ -11937,7 +11936,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>608</v>
       </c>
@@ -11957,7 +11956,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>609</v>
       </c>
@@ -11977,7 +11976,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>610</v>
       </c>
@@ -11997,7 +11996,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>611</v>
       </c>
@@ -12017,7 +12016,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>612</v>
       </c>
@@ -12046,7 +12045,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>613</v>
       </c>
@@ -12075,7 +12074,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>614</v>
       </c>
@@ -12104,7 +12103,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>615</v>
       </c>
@@ -12133,7 +12132,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>622</v>
       </c>
@@ -12165,7 +12164,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>623</v>
       </c>
@@ -12192,7 +12191,7 @@
       </c>
       <c r="K213" s="3"/>
     </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>627</v>
       </c>
@@ -12221,7 +12220,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>635</v>
       </c>
@@ -12251,7 +12250,7 @@
       </c>
       <c r="K215" s="3"/>
     </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>636</v>
       </c>
@@ -12281,7 +12280,7 @@
       </c>
       <c r="K216" s="3"/>
     </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B217" s="3" t="s">
         <v>639</v>
       </c>
@@ -12311,7 +12310,7 @@
       </c>
       <c r="K217" s="3"/>
     </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B218" s="33" t="s">
         <v>641</v>
       </c>
@@ -12338,11 +12337,11 @@
       </c>
       <c r="K218" s="3"/>
     </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="F219" s="3"/>
       <c r="K219" s="3"/>
     </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>841</v>
       </c>
@@ -12365,7 +12364,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>653</v>
       </c>
@@ -12395,7 +12394,7 @@
       </c>
       <c r="K221" s="3"/>
     </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>659</v>
       </c>
@@ -12425,7 +12424,7 @@
       </c>
       <c r="K222" s="3"/>
     </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>662</v>
       </c>
@@ -12452,7 +12451,7 @@
       </c>
       <c r="K223" s="3"/>
     </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>666</v>
       </c>
@@ -12479,7 +12478,7 @@
       </c>
       <c r="K224" s="3"/>
     </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>667</v>
       </c>
@@ -12506,7 +12505,7 @@
       </c>
       <c r="K225" s="3"/>
     </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>674</v>
       </c>
@@ -12536,7 +12535,7 @@
       </c>
       <c r="K226" s="3"/>
     </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>675</v>
       </c>
@@ -12566,7 +12565,7 @@
       </c>
       <c r="K227" s="3"/>
     </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>681</v>
       </c>
@@ -12593,7 +12592,7 @@
       </c>
       <c r="K228" s="3"/>
     </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>682</v>
       </c>
@@ -12620,7 +12619,7 @@
       </c>
       <c r="K229" s="3"/>
     </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>683</v>
       </c>
@@ -12647,7 +12646,7 @@
       </c>
       <c r="K230" s="3"/>
     </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>688</v>
       </c>
@@ -12674,7 +12673,7 @@
       </c>
       <c r="K231" s="3"/>
     </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>690</v>
       </c>
@@ -12701,7 +12700,7 @@
       </c>
       <c r="K232" s="3"/>
     </row>
-    <row r="233" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>698</v>
       </c>
@@ -12728,7 +12727,7 @@
       </c>
       <c r="K233" s="3"/>
     </row>
-    <row r="234" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>699</v>
       </c>
@@ -12755,7 +12754,7 @@
       </c>
       <c r="K234" s="3"/>
     </row>
-    <row r="235" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>700</v>
       </c>
@@ -12779,7 +12778,7 @@
       </c>
       <c r="K235" s="3"/>
     </row>
-    <row r="236" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>709</v>
       </c>
@@ -12798,7 +12797,7 @@
       <c r="F236" s="3"/>
       <c r="K236" s="3"/>
     </row>
-    <row r="237" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>714</v>
       </c>
@@ -12817,7 +12816,7 @@
       <c r="F237" s="3"/>
       <c r="K237" s="3"/>
     </row>
-    <row r="238" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>717</v>
       </c>
@@ -12836,7 +12835,7 @@
       <c r="F238" s="3"/>
       <c r="K238" s="3"/>
     </row>
-    <row r="239" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>721</v>
       </c>
@@ -12855,7 +12854,7 @@
       <c r="F239" s="3"/>
       <c r="K239" s="3"/>
     </row>
-    <row r="240" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>722</v>
       </c>
@@ -12874,7 +12873,7 @@
       <c r="F240" s="3"/>
       <c r="K240" s="3"/>
     </row>
-    <row r="241" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>725</v>
       </c>
@@ -12895,7 +12894,7 @@
       </c>
       <c r="K241" s="3"/>
     </row>
-    <row r="242" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>804</v>
       </c>
@@ -12922,7 +12921,7 @@
       </c>
       <c r="K242" s="3"/>
     </row>
-    <row r="243" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>739</v>
       </c>
@@ -12937,7 +12936,7 @@
       </c>
       <c r="K243" s="3"/>
     </row>
-    <row r="244" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>740</v>
       </c>
@@ -12958,7 +12957,7 @@
       </c>
       <c r="K244" s="3"/>
     </row>
-    <row r="245" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>741</v>
       </c>
@@ -12979,7 +12978,7 @@
       </c>
       <c r="K245" s="3"/>
     </row>
-    <row r="246" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>742</v>
       </c>
@@ -13000,7 +12999,7 @@
       </c>
       <c r="K246" s="3"/>
     </row>
-    <row r="247" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>805</v>
       </c>
@@ -13024,7 +13023,7 @@
       </c>
       <c r="K247" s="3"/>
     </row>
-    <row r="248" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>823</v>
       </c>
@@ -13048,7 +13047,7 @@
       </c>
       <c r="K248" s="3"/>
     </row>
-    <row r="249" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A249" s="3" t="s">
         <v>825</v>
       </c>
@@ -13078,7 +13077,7 @@
       </c>
       <c r="K249" s="3"/>
     </row>
-    <row r="250" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>819</v>
       </c>
@@ -13105,7 +13104,7 @@
       </c>
       <c r="K250" s="3"/>
     </row>
-    <row r="251" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>806</v>
       </c>
@@ -13129,7 +13128,7 @@
       </c>
       <c r="K251" s="3"/>
     </row>
-    <row r="252" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>807</v>
       </c>
@@ -13159,7 +13158,7 @@
       </c>
       <c r="K252" s="3"/>
     </row>
-    <row r="253" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>809</v>
       </c>
@@ -13186,7 +13185,7 @@
       </c>
       <c r="K253" s="3"/>
     </row>
-    <row r="254" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>745</v>
       </c>
@@ -13207,7 +13206,7 @@
       </c>
       <c r="K254" s="3"/>
     </row>
-    <row r="255" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>746</v>
       </c>
@@ -13226,7 +13225,7 @@
       <c r="F255" s="3"/>
       <c r="K255" s="3"/>
     </row>
-    <row r="256" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>747</v>
       </c>
@@ -13247,7 +13246,7 @@
       </c>
       <c r="K256" s="3"/>
     </row>
-    <row r="257" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>833</v>
       </c>
@@ -13268,7 +13267,7 @@
       </c>
       <c r="K257" s="3"/>
     </row>
-    <row r="258" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>772</v>
       </c>
@@ -13287,7 +13286,7 @@
       <c r="F258" s="3"/>
       <c r="K258" s="3"/>
     </row>
-    <row r="259" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>778</v>
       </c>
@@ -13314,7 +13313,7 @@
       </c>
       <c r="K259" s="3"/>
     </row>
-    <row r="260" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>771</v>
       </c>
@@ -13333,7 +13332,7 @@
       <c r="F260" s="3"/>
       <c r="K260" s="3"/>
     </row>
-    <row r="261" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>770</v>
       </c>
@@ -13352,7 +13351,7 @@
       <c r="F261" s="3"/>
       <c r="K261" s="3"/>
     </row>
-    <row r="262" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>769</v>
       </c>
@@ -13371,7 +13370,7 @@
       <c r="F262" s="3"/>
       <c r="K262" s="3"/>
     </row>
-    <row r="263" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>775</v>
       </c>
@@ -13398,7 +13397,7 @@
       </c>
       <c r="K263" s="3"/>
     </row>
-    <row r="264" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>776</v>
       </c>
@@ -13425,7 +13424,7 @@
       </c>
       <c r="K264" s="3"/>
     </row>
-    <row r="265" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>777</v>
       </c>
@@ -13452,7 +13451,7 @@
       </c>
       <c r="K265" s="3"/>
     </row>
-    <row r="266" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>768</v>
       </c>
@@ -13471,7 +13470,7 @@
       <c r="F266" s="3"/>
       <c r="K266" s="3"/>
     </row>
-    <row r="267" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>767</v>
       </c>
@@ -13490,7 +13489,7 @@
       <c r="F267" s="3"/>
       <c r="K267" s="3"/>
     </row>
-    <row r="268" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>780</v>
       </c>
@@ -13520,7 +13519,7 @@
       </c>
       <c r="K268" s="3"/>
     </row>
-    <row r="269" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>781</v>
       </c>
@@ -13544,7 +13543,7 @@
       </c>
       <c r="K269" s="3"/>
     </row>
-    <row r="270" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>784</v>
       </c>
@@ -13565,7 +13564,7 @@
       </c>
       <c r="K270" s="3"/>
     </row>
-    <row r="271" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>798</v>
       </c>
@@ -13586,7 +13585,7 @@
       </c>
       <c r="K271" s="3"/>
     </row>
-    <row r="272" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>799</v>
       </c>
@@ -13607,7 +13606,7 @@
       </c>
       <c r="K272" s="3"/>
     </row>
-    <row r="273" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>800</v>
       </c>
@@ -13628,7 +13627,7 @@
       </c>
       <c r="K273" s="3"/>
     </row>
-    <row r="274" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>801</v>
       </c>
@@ -13649,7 +13648,7 @@
       </c>
       <c r="K274" s="3"/>
     </row>
-    <row r="275" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>802</v>
       </c>
@@ -13670,7 +13669,7 @@
       </c>
       <c r="K275" s="3"/>
     </row>
-    <row r="276" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>803</v>
       </c>
@@ -13691,7 +13690,7 @@
       </c>
       <c r="K276" s="3"/>
     </row>
-    <row r="277" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>814</v>
       </c>
@@ -13715,7 +13714,7 @@
       </c>
       <c r="K277" s="3"/>
     </row>
-    <row r="278" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>815</v>
       </c>
@@ -13736,389 +13735,311 @@
       </c>
       <c r="K278" s="3"/>
     </row>
-    <row r="279" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A279" s="38" t="s">
+    <row r="279" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A279" t="s">
         <v>834</v>
       </c>
-      <c r="B279" s="39" t="s">
+      <c r="B279" s="3" t="s">
         <v>617</v>
       </c>
-      <c r="C279" s="38"/>
-      <c r="D279" s="39"/>
-      <c r="E279" s="38"/>
-      <c r="F279" s="40" t="s">
+      <c r="F279" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="G279" s="41" t="s">
+      <c r="G279" t="s">
         <v>835</v>
       </c>
-      <c r="H279" s="38" t="s">
+      <c r="H279" t="s">
         <v>132</v>
       </c>
-      <c r="I279" s="38" t="s">
+      <c r="I279" t="s">
         <v>828</v>
       </c>
-      <c r="J279" s="38"/>
-      <c r="K279" s="40"/>
-      <c r="L279" s="38"/>
-    </row>
-    <row r="280" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A280" s="38" t="s">
+      <c r="K279" s="3"/>
+    </row>
+    <row r="280" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A280" t="s">
         <v>836</v>
       </c>
-      <c r="B280" s="39" t="s">
+      <c r="B280" s="3" t="s">
         <v>617</v>
       </c>
-      <c r="C280" s="38"/>
-      <c r="D280" s="39"/>
-      <c r="E280" s="38"/>
-      <c r="F280" s="40" t="s">
+      <c r="F280" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="G280" s="41" t="s">
+      <c r="G280" t="s">
         <v>837</v>
       </c>
-      <c r="H280" s="38" t="s">
+      <c r="H280" t="s">
         <v>132</v>
       </c>
-      <c r="I280" s="38"/>
-      <c r="J280" s="38"/>
-      <c r="K280" s="40"/>
-      <c r="L280" s="38"/>
-    </row>
-    <row r="281" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A281" s="38" t="s">
+      <c r="K280" s="3"/>
+    </row>
+    <row r="281" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A281" t="s">
         <v>838</v>
       </c>
-      <c r="B281" s="39" t="s">
+      <c r="B281" s="3" t="s">
         <v>617</v>
       </c>
-      <c r="C281" s="38"/>
-      <c r="D281" s="39"/>
-      <c r="E281" s="38"/>
-      <c r="F281" s="40" t="s">
+      <c r="F281" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="G281" s="41" t="s">
+      <c r="G281" t="s">
         <v>839</v>
       </c>
-      <c r="H281" s="38" t="s">
+      <c r="H281" t="s">
         <v>132</v>
       </c>
-      <c r="I281" s="38"/>
-      <c r="J281" s="38"/>
-      <c r="K281" s="40"/>
-      <c r="L281" s="38"/>
-    </row>
-    <row r="282" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A282" s="38" t="s">
+      <c r="K281" s="3"/>
+    </row>
+    <row r="282" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A282" t="s">
         <v>840</v>
       </c>
-      <c r="B282" s="39" t="s">
+      <c r="B282" s="3" t="s">
         <v>617</v>
       </c>
-      <c r="C282" s="38"/>
-      <c r="D282" s="39"/>
-      <c r="E282" s="38"/>
-      <c r="F282" s="40" t="s">
+      <c r="F282" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="G282" s="41" t="s">
+      <c r="G282" t="s">
         <v>839</v>
       </c>
-      <c r="H282" s="38" t="s">
+      <c r="H282" t="s">
         <v>132</v>
       </c>
-      <c r="I282" s="38"/>
-      <c r="J282" s="38"/>
-      <c r="K282" s="40"/>
-      <c r="L282" s="38"/>
-    </row>
-    <row r="283" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A283" s="38" t="s">
+      <c r="K282" s="3"/>
+    </row>
+    <row r="283" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A283" t="s">
         <v>842</v>
       </c>
-      <c r="B283" s="39" t="s">
+      <c r="B283" s="3" t="s">
         <v>617</v>
       </c>
-      <c r="C283" s="38"/>
-      <c r="D283" s="39"/>
-      <c r="E283" s="38"/>
-      <c r="F283" s="40" t="s">
+      <c r="F283" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G283" s="41" t="s">
+      <c r="G283" t="s">
         <v>843</v>
       </c>
-      <c r="H283" s="38" t="s">
+      <c r="H283" t="s">
         <v>132</v>
       </c>
-      <c r="I283" s="38"/>
-      <c r="J283" s="38"/>
-      <c r="K283" s="40"/>
-      <c r="L283" s="38"/>
-    </row>
-    <row r="284" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A284" s="38" t="s">
+      <c r="K283" s="3"/>
+    </row>
+    <row r="284" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A284" t="s">
         <v>846</v>
       </c>
-      <c r="B284" s="39" t="s">
+      <c r="B284" s="3" t="s">
         <v>617</v>
       </c>
-      <c r="C284" s="38"/>
-      <c r="D284" s="39"/>
-      <c r="E284" s="38"/>
-      <c r="F284" s="40" t="s">
+      <c r="F284" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G284" s="41" t="s">
+      <c r="G284" t="s">
         <v>844</v>
       </c>
-      <c r="H284" s="38" t="s">
+      <c r="H284" t="s">
         <v>132</v>
       </c>
-      <c r="I284" s="38"/>
-      <c r="J284" s="38"/>
-      <c r="K284" s="40"/>
-      <c r="L284" s="38"/>
-    </row>
-    <row r="285" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A285" s="38" t="s">
+      <c r="K284" s="3"/>
+    </row>
+    <row r="285" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A285" t="s">
         <v>847</v>
       </c>
-      <c r="B285" s="39" t="s">
+      <c r="B285" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C285" s="38" t="s">
+      <c r="C285" t="s">
         <v>861</v>
       </c>
-      <c r="D285" s="38" t="s">
+      <c r="D285" t="s">
         <v>862</v>
       </c>
-      <c r="E285" s="38" t="s">
+      <c r="E285" t="s">
         <v>718</v>
       </c>
-      <c r="F285" s="40" t="s">
+      <c r="F285" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G285" s="41" t="s">
+      <c r="G285" t="s">
         <v>845</v>
       </c>
-      <c r="H285" s="38" t="s">
+      <c r="H285" t="s">
         <v>132</v>
       </c>
-      <c r="I285" s="38"/>
-      <c r="J285" s="38" t="s">
+      <c r="J285" t="s">
         <v>864</v>
       </c>
-      <c r="K285" s="40"/>
-      <c r="L285" s="38"/>
-    </row>
-    <row r="286" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A286" s="38" t="s">
+      <c r="K285" s="3"/>
+    </row>
+    <row r="286" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A286" t="s">
         <v>862</v>
       </c>
-      <c r="B286" s="38" t="s">
+      <c r="B286" t="s">
         <v>847</v>
       </c>
-      <c r="C286" s="38" t="s">
+      <c r="C286" t="s">
         <v>255</v>
       </c>
-      <c r="D286" s="39" t="s">
+      <c r="D286" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E286" s="38" t="s">
+      <c r="E286" t="s">
         <v>358</v>
       </c>
-      <c r="F286" s="37" t="s">
+      <c r="F286" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="G286" s="41"/>
-      <c r="H286" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="I286" s="38"/>
-      <c r="J286" s="38" t="s">
+      <c r="H286" t="s">
+        <v>132</v>
+      </c>
+      <c r="J286" t="s">
         <v>863</v>
       </c>
-      <c r="K286" s="40"/>
-      <c r="L286" s="38"/>
-    </row>
-    <row r="287" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A287" s="38" t="s">
+      <c r="K286" s="3"/>
+    </row>
+    <row r="287" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A287" t="s">
         <v>848</v>
       </c>
-      <c r="B287" s="39" t="s">
+      <c r="B287" s="3" t="s">
         <v>617</v>
       </c>
-      <c r="C287" s="38"/>
-      <c r="D287" s="39"/>
-      <c r="E287" s="38"/>
-      <c r="F287" s="40" t="s">
+      <c r="F287" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G287" s="41" t="s">
+      <c r="G287" t="s">
         <v>849</v>
       </c>
-      <c r="H287" s="38" t="s">
+      <c r="H287" t="s">
         <v>132</v>
       </c>
-      <c r="I287" s="38"/>
-      <c r="J287" s="38" t="s">
+      <c r="J287" t="s">
         <v>850</v>
       </c>
-      <c r="K287" s="40"/>
-      <c r="L287" s="38"/>
-    </row>
-    <row r="288" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A288" s="38" t="s">
+      <c r="K287" s="3"/>
+    </row>
+    <row r="288" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A288" t="s">
         <v>851</v>
       </c>
-      <c r="B288" s="39" t="s">
+      <c r="B288" s="3" t="s">
         <v>617</v>
       </c>
-      <c r="C288" s="38"/>
-      <c r="D288" s="39"/>
-      <c r="E288" s="38"/>
-      <c r="F288" s="40" t="s">
+      <c r="F288" s="3" t="s">
         <v>736</v>
       </c>
-      <c r="G288" s="41" t="s">
+      <c r="G288" t="s">
         <v>852</v>
       </c>
-      <c r="H288" s="38" t="s">
+      <c r="H288" t="s">
         <v>132</v>
       </c>
-      <c r="I288" s="38"/>
-      <c r="J288" s="38" t="s">
+      <c r="J288" t="s">
         <v>853</v>
       </c>
-      <c r="K288" s="40"/>
-      <c r="L288" s="38"/>
-    </row>
-    <row r="289" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A289" s="38" t="s">
+      <c r="K288" s="3"/>
+    </row>
+    <row r="289" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A289" t="s">
         <v>854</v>
       </c>
-      <c r="B289" s="39" t="s">
+      <c r="B289" s="3" t="s">
         <v>617</v>
       </c>
-      <c r="C289" s="38"/>
-      <c r="D289" s="39"/>
-      <c r="E289" s="38"/>
-      <c r="F289" s="40" t="s">
+      <c r="F289" s="3" t="s">
         <v>733</v>
       </c>
-      <c r="G289" s="41" t="s">
+      <c r="G289" t="s">
         <v>630</v>
       </c>
-      <c r="H289" s="38" t="s">
+      <c r="H289" t="s">
         <v>132</v>
       </c>
-      <c r="I289" s="38"/>
-      <c r="J289" s="38"/>
-      <c r="K289" s="40"/>
-      <c r="L289" s="38"/>
-    </row>
-    <row r="290" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A290" s="38" t="s">
+      <c r="K289" s="3"/>
+    </row>
+    <row r="290" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A290" t="s">
         <v>855</v>
       </c>
-      <c r="B290" s="39" t="s">
+      <c r="B290" s="3" t="s">
         <v>617</v>
       </c>
-      <c r="C290" s="38"/>
-      <c r="D290" s="39"/>
-      <c r="E290" s="38"/>
-      <c r="F290" s="40" t="s">
+      <c r="F290" s="3" t="s">
         <v>856</v>
       </c>
-      <c r="G290" s="41" t="s">
+      <c r="G290" t="s">
         <v>401</v>
       </c>
-      <c r="H290" s="38" t="s">
+      <c r="H290" t="s">
         <v>132</v>
       </c>
-      <c r="I290" s="38"/>
-      <c r="J290" s="38"/>
-      <c r="K290" s="40"/>
-      <c r="L290" s="38"/>
-    </row>
-    <row r="291" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A291" s="38" t="s">
+      <c r="K290" s="3"/>
+    </row>
+    <row r="291" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A291" t="s">
         <v>857</v>
       </c>
-      <c r="B291" s="39" t="s">
+      <c r="B291" s="3" t="s">
         <v>617</v>
       </c>
-      <c r="C291" s="38"/>
-      <c r="D291" s="39"/>
-      <c r="E291" s="38"/>
-      <c r="F291" s="40" t="s">
+      <c r="F291" s="3" t="s">
         <v>856</v>
       </c>
-      <c r="G291" s="41" t="s">
+      <c r="G291" t="s">
         <v>401</v>
       </c>
-      <c r="H291" s="38" t="s">
+      <c r="H291" t="s">
         <v>132</v>
       </c>
-      <c r="I291" s="38"/>
-      <c r="J291" s="38"/>
-      <c r="K291" s="40"/>
-      <c r="L291" s="38"/>
-    </row>
-    <row r="292" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A292" s="38" t="s">
+      <c r="K291" s="3"/>
+    </row>
+    <row r="292" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A292" t="s">
         <v>858</v>
       </c>
-      <c r="B292" s="39" t="s">
+      <c r="B292" s="3" t="s">
         <v>617</v>
       </c>
-      <c r="C292" s="38"/>
-      <c r="D292" s="39"/>
-      <c r="E292" s="38"/>
-      <c r="F292" s="40" t="s">
+      <c r="F292" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G292" s="41" t="s">
+      <c r="G292" t="s">
         <v>812</v>
       </c>
-      <c r="H292" s="38" t="s">
+      <c r="H292" t="s">
         <v>132</v>
       </c>
-      <c r="I292" s="38"/>
-      <c r="J292" s="38" t="s">
+      <c r="J292" t="s">
         <v>202</v>
       </c>
-      <c r="K292" s="40"/>
-      <c r="L292" s="38"/>
-    </row>
-    <row r="293" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A293" s="38" t="s">
+      <c r="K292" s="3"/>
+    </row>
+    <row r="293" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A293" t="s">
         <v>860</v>
       </c>
-      <c r="B293" s="39" t="s">
+      <c r="B293" s="3" t="s">
         <v>617</v>
       </c>
-      <c r="C293" s="38"/>
-      <c r="D293" s="39"/>
-      <c r="E293" s="38"/>
-      <c r="F293" s="40" t="s">
+      <c r="F293" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G293" s="41" t="s">
+      <c r="G293" t="s">
         <v>812</v>
       </c>
-      <c r="H293" s="38" t="s">
+      <c r="H293" t="s">
         <v>132</v>
       </c>
-      <c r="I293" s="38"/>
-      <c r="J293" s="38" t="s">
+      <c r="J293" t="s">
         <v>859</v>
       </c>
-      <c r="K293" s="40"/>
-      <c r="L293" s="38"/>
+      <c r="K293" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -14160,7 +14081,7 @@
       <c r="A4" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="B4" s="42">
+      <c r="B4">
         <v>6</v>
       </c>
     </row>
@@ -14168,7 +14089,7 @@
       <c r="A5" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="B5" s="42">
+      <c r="B5">
         <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -14182,13 +14103,13 @@
       <c r="A6" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="B6" s="42">
+      <c r="B6">
         <v>1</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="42">
+      <c r="F6">
         <v>27</v>
       </c>
     </row>
@@ -14196,13 +14117,13 @@
       <c r="A7" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="B7" s="42">
+      <c r="B7">
         <v>6</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F7" s="42">
+      <c r="F7">
         <v>41</v>
       </c>
     </row>
@@ -14210,13 +14131,13 @@
       <c r="A8" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B8" s="42">
+      <c r="B8">
         <v>2</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F8" s="42">
+      <c r="F8">
         <v>9</v>
       </c>
     </row>
@@ -14224,13 +14145,13 @@
       <c r="A9" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="B9" s="42">
+      <c r="B9">
         <v>3</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F9" s="42">
+      <c r="F9">
         <v>57</v>
       </c>
     </row>
@@ -14238,13 +14159,13 @@
       <c r="A10" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B10" s="42">
+      <c r="B10">
         <v>10</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="F10" s="42">
+      <c r="F10">
         <v>134</v>
       </c>
     </row>
@@ -14252,7 +14173,7 @@
       <c r="A11" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="B11" s="42">
+      <c r="B11">
         <v>15</v>
       </c>
     </row>
@@ -14260,7 +14181,7 @@
       <c r="A12" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="42">
+      <c r="B12">
         <v>25</v>
       </c>
     </row>
@@ -14268,7 +14189,7 @@
       <c r="A13" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="B13" s="42">
+      <c r="B13">
         <v>1</v>
       </c>
     </row>
@@ -14276,7 +14197,7 @@
       <c r="A14" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B14" s="42">
+      <c r="B14">
         <v>2</v>
       </c>
     </row>
@@ -14284,7 +14205,7 @@
       <c r="A15" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B15" s="42">
+      <c r="B15">
         <v>2</v>
       </c>
     </row>
@@ -14292,7 +14213,7 @@
       <c r="A16" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B16" s="42">
+      <c r="B16">
         <v>1</v>
       </c>
     </row>
@@ -14300,7 +14221,7 @@
       <c r="A17" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B17" s="42">
+      <c r="B17">
         <v>3</v>
       </c>
     </row>
@@ -14308,7 +14229,7 @@
       <c r="A18" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="42">
+      <c r="B18">
         <v>16</v>
       </c>
     </row>
@@ -14316,7 +14237,7 @@
       <c r="A19" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="B19" s="42">
+      <c r="B19">
         <v>8</v>
       </c>
     </row>
@@ -14324,7 +14245,7 @@
       <c r="A20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="42">
+      <c r="B20">
         <v>1</v>
       </c>
     </row>
@@ -14332,7 +14253,7 @@
       <c r="A21" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="42">
+      <c r="B21">
         <v>1</v>
       </c>
     </row>
@@ -14340,7 +14261,7 @@
       <c r="A22" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="B22" s="42">
+      <c r="B22">
         <v>1</v>
       </c>
     </row>
@@ -14348,7 +14269,7 @@
       <c r="A23" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B23" s="42">
+      <c r="B23">
         <v>6</v>
       </c>
     </row>
@@ -14356,7 +14277,7 @@
       <c r="A24" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="42">
+      <c r="B24">
         <v>1</v>
       </c>
     </row>
@@ -14364,7 +14285,7 @@
       <c r="A25" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B25" s="42">
+      <c r="B25">
         <v>1</v>
       </c>
     </row>
@@ -14372,7 +14293,7 @@
       <c r="A26" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B26" s="42">
+      <c r="B26">
         <v>3</v>
       </c>
     </row>
@@ -14380,7 +14301,7 @@
       <c r="A27" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="B27" s="42">
+      <c r="B27">
         <v>2</v>
       </c>
     </row>
@@ -14388,7 +14309,7 @@
       <c r="A28" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B28" s="42">
+      <c r="B28">
         <v>9</v>
       </c>
     </row>
@@ -14396,7 +14317,7 @@
       <c r="A29" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B29" s="42">
+      <c r="B29">
         <v>134</v>
       </c>
     </row>

</xml_diff>

<commit_message>
asset and cable updates
</commit_message>
<xml_diff>
--- a/data/uac_cables.xlsx
+++ b/data/uac_cables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/donert/Documents/UACTech/SystemDocumentation/github/uactechdoc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856EE09D-8CBB-AC45-BA37-37528FD91E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF217CF-B0D7-B744-BD72-1E1705AE57B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{288904EE-D384-EA4C-9B98-052B972FB267}"/>
+    <workbookView xWindow="4080" yWindow="1600" windowWidth="30240" windowHeight="18880" xr2:uid="{288904EE-D384-EA4C-9B98-052B972FB267}"/>
   </bookViews>
   <sheets>
     <sheet name="Cables" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,8 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="63" r:id="rId3"/>
-    <pivotCache cacheId="64" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId3"/>
+    <pivotCache cacheId="19" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2327" uniqueCount="939">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2534" uniqueCount="1020">
   <si>
     <t>Tag</t>
   </si>
@@ -2858,12 +2858,258 @@
   </si>
   <si>
     <t>out_a</t>
+  </si>
+  <si>
+    <t>2311-2703</t>
+  </si>
+  <si>
+    <t>studio</t>
+  </si>
+  <si>
+    <t>usbc1</t>
+  </si>
+  <si>
+    <t>2311-2702</t>
+  </si>
+  <si>
+    <t>0.4m</t>
+  </si>
+  <si>
+    <t>external SSD</t>
+  </si>
+  <si>
+    <t>2311-2802</t>
+  </si>
+  <si>
+    <t>2311-2801</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>0.8m</t>
+  </si>
+  <si>
+    <t>2311-2803</t>
+  </si>
+  <si>
+    <t>2310-2406</t>
+  </si>
+  <si>
+    <t>thru</t>
+  </si>
+  <si>
+    <t>2401-0900</t>
+  </si>
+  <si>
+    <t>Network to video recorder</t>
+  </si>
+  <si>
+    <t>2401-0901</t>
+  </si>
+  <si>
+    <t>CUMU-G002</t>
+  </si>
+  <si>
+    <t>Testing with fault</t>
+  </si>
+  <si>
+    <t>2401-1501</t>
+  </si>
+  <si>
+    <t>18.3m</t>
+  </si>
+  <si>
+    <t>fellowship hall video to projector</t>
+  </si>
+  <si>
+    <t>avshop #363084 2024-01-12 (paid for by Tony. Balance of the 100' roll is in invneotry)</t>
+  </si>
+  <si>
+    <t>2401-3005</t>
+  </si>
+  <si>
+    <t>2401-3006</t>
+  </si>
+  <si>
+    <t>2401-3007</t>
+  </si>
+  <si>
+    <t>2401-3008</t>
+  </si>
+  <si>
+    <t>4.65m</t>
+  </si>
+  <si>
+    <t>syncwire</t>
+  </si>
+  <si>
+    <t>amazonbasics</t>
+  </si>
+  <si>
+    <t>2401-3009</t>
+  </si>
+  <si>
+    <t>FH computer</t>
+  </si>
+  <si>
+    <t>2.4m</t>
+  </si>
+  <si>
+    <t>CDWU-A001</t>
+  </si>
+  <si>
+    <t>proj</t>
+  </si>
+  <si>
+    <t>2401-3010</t>
+  </si>
+  <si>
+    <t>guest</t>
+  </si>
+  <si>
+    <t>2401-3004</t>
+  </si>
+  <si>
+    <t>fh_guest</t>
+  </si>
+  <si>
+    <t>inx</t>
+  </si>
+  <si>
+    <t>iny</t>
+  </si>
+  <si>
+    <t>2401-3002</t>
+  </si>
+  <si>
+    <t>1704-0100</t>
+  </si>
+  <si>
+    <t>2401-3001</t>
+  </si>
+  <si>
+    <t>a320-1</t>
+  </si>
+  <si>
+    <t>2401-2800</t>
+  </si>
+  <si>
+    <t>2401-3003</t>
+  </si>
+  <si>
+    <t>audio feed</t>
+  </si>
+  <si>
+    <t>ch_in</t>
+  </si>
+  <si>
+    <t>2401-3100</t>
+  </si>
+  <si>
+    <t>2401-3101</t>
+  </si>
+  <si>
+    <t>2401-3102</t>
+  </si>
+  <si>
+    <t>2401-3103</t>
+  </si>
+  <si>
+    <t>a324_1</t>
+  </si>
+  <si>
+    <t>fh_mic</t>
+  </si>
+  <si>
+    <t>xlr</t>
+  </si>
+  <si>
+    <t>port</t>
+  </si>
+  <si>
+    <t>2401-3105</t>
+  </si>
+  <si>
+    <t>rca</t>
+  </si>
+  <si>
+    <t>audio_rca</t>
+  </si>
+  <si>
+    <t>Also has svideo not used</t>
+  </si>
+  <si>
+    <t>2401-3113</t>
+  </si>
+  <si>
+    <t>2401-3106</t>
+  </si>
+  <si>
+    <t>11.9m</t>
+  </si>
+  <si>
+    <t>Canare L-4E6S</t>
+  </si>
+  <si>
+    <t>2401-6034</t>
+  </si>
+  <si>
+    <t>2401-3107</t>
+  </si>
+  <si>
+    <t>2401-3108</t>
+  </si>
+  <si>
+    <t>2.2m</t>
+  </si>
+  <si>
+    <t>2401-3109</t>
+  </si>
+  <si>
+    <t>1_8_audio</t>
+  </si>
+  <si>
+    <t>in_9_10</t>
+  </si>
+  <si>
+    <t>audio_18_trs</t>
+  </si>
+  <si>
+    <t>Guest audio</t>
+  </si>
+  <si>
+    <t>2401-3110</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>2401-3111</t>
+  </si>
+  <si>
+    <t>43m</t>
+  </si>
+  <si>
+    <t>2401-3112</t>
+  </si>
+  <si>
+    <t>2.5m</t>
+  </si>
+  <si>
+    <t>2401-3114</t>
+  </si>
+  <si>
+    <t>tape_CD_In</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;Yes&quot;;&quot;Yes&quot;;&quot;No&quot;"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -3093,7 +3339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3145,6 +3391,18 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3321,7 +3579,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="45221.662918634262" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="293" xr:uid="{966EC718-ADB8-7746-9366-54097C9D57FA}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:L307" sheet="Cables"/>
+    <worksheetSource ref="A1:L333" sheet="Cables"/>
   </cacheSource>
   <cacheFields count="12">
     <cacheField name="Tag" numFmtId="0">
@@ -9595,7 +9853,70 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{10F736CA-5D69-4D44-A803-D4241D124F38}" name="PivotTable1" cacheId="64" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{331FD294-EE6F-3D4E-A534-813A4D9D566E}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="E5:F10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="12">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="7"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Tag" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{10F736CA-5D69-4D44-A803-D4241D124F38}" name="PivotTable1" cacheId="19" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B42" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField dataField="1" showAll="0"/>
@@ -9795,78 +10116,9 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{331FD294-EE6F-3D4E-A534-813A4D9D566E}" name="PivotTable2" cacheId="63" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="E5:F10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="12">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="7"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Tag" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD7E3698-8860-904B-8BDB-00EF1039C49C}" name="Table1" displayName="Table1" ref="A1:L307" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="5">
-  <autoFilter ref="A1:L307" xr:uid="{BD7E3698-8860-904B-8BDB-00EF1039C49C}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="2308-0912"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD7E3698-8860-904B-8BDB-00EF1039C49C}" name="Table1" displayName="Table1" ref="A1:L333" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="5">
+  <autoFilter ref="A1:L333" xr:uid="{BD7E3698-8860-904B-8BDB-00EF1039C49C}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{4D442337-BE86-B24A-84A4-338FB80A6A49}" name="Tag"/>
     <tableColumn id="2" xr3:uid="{74A36D7B-C989-3B4B-B1E5-AB1FA4C2DD45}" name="SrcTag" dataDxfId="4"/>
@@ -10182,13 +10434,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B91ADC-4569-1C4E-B002-1ED2E647C959}">
-  <dimension ref="A1:L307"/>
+  <dimension ref="A1:V333"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B302" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B316" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A308" sqref="A308:XFD308"/>
+      <selection pane="bottomRight" activeCell="E330" sqref="E330"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10244,7 +10496,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>25</v>
       </c>
@@ -10287,7 +10539,7 @@
         <v>cdmua001:Key -&gt; zviue004:sw1 [label='2307-1800']</v>
       </c>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>4</v>
       </c>
@@ -10322,7 +10574,7 @@
         <v>cdmua001:Fill -&gt; zviue004:sw2 [label='2307-1801']</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>5</v>
       </c>
@@ -10357,7 +10609,7 @@
         <v>cdmua001:ProjA -&gt; zviue004:sw4 [label='2307-1802']</v>
       </c>
     </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>6</v>
       </c>
@@ -10392,7 +10644,7 @@
         <v>cdmua001:ProjB -&gt; zviue004:sw6 [label='2307-1803']</v>
       </c>
     </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>7</v>
       </c>
@@ -10427,7 +10679,7 @@
         <v>cdmua001:ProjC -&gt; zviue004:sw8 [label='2307-1804']</v>
       </c>
     </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>8</v>
       </c>
@@ -10462,7 +10714,7 @@
         <v>cdmua001:RearDeckLink -&gt; zviue004:sw3 [label='2307-1805']</v>
       </c>
     </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>9</v>
       </c>
@@ -10495,7 +10747,7 @@
         <v>zvkua003:PGM -&gt; zviua005:sdi [label='2307-1806']</v>
       </c>
     </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
         <v>10</v>
       </c>
@@ -10530,7 +10782,7 @@
         <v>cdmua001:in1 -&gt; zviue004:sw5 [label='2307-1807']</v>
       </c>
     </row>
-    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>11</v>
       </c>
@@ -10565,7 +10817,7 @@
         <v>zvkua003:aux -&gt; zviud001:sdi in [label='2307-1808']</v>
       </c>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
         <v>12</v>
       </c>
@@ -10608,7 +10860,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>13</v>
       </c>
@@ -10653,7 +10905,7 @@
         <v>zviue004:sdi1 -&gt; 23081204:sdi in [label='2307-1810']</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>14</v>
       </c>
@@ -10690,7 +10942,7 @@
         <v>zviue004:sdi2 -&gt; 23081205:sdi in [label='2307-1811']</v>
       </c>
     </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>15</v>
       </c>
@@ -10725,7 +10977,7 @@
         <v>zviue004:sdi4 -&gt; zviug003:sdi in [label='2307-1812']</v>
       </c>
     </row>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
         <v>16</v>
       </c>
@@ -10760,7 +11012,7 @@
         <v>zviue004:sdi6 -&gt; zviug004:sdi in [label='2307-1813']</v>
       </c>
     </row>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>17</v>
       </c>
@@ -10795,7 +11047,7 @@
         <v>zviue004:sdi8 -&gt; zviug005:sdi in [label='2307-1814']</v>
       </c>
     </row>
-    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
         <v>18</v>
       </c>
@@ -10830,7 +11082,7 @@
         <v>zviue004:sdi3 -&gt; zviue001:sdi in [label='2307-1815']</v>
       </c>
     </row>
-    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>19</v>
       </c>
@@ -10851,7 +11103,7 @@
         <v>: -&gt; : [label='2307-1816']</v>
       </c>
     </row>
-    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
         <v>20</v>
       </c>
@@ -10872,7 +11124,7 @@
         <v>: -&gt; : [label='2307-1817']</v>
       </c>
     </row>
-    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>21</v>
       </c>
@@ -10893,7 +11145,7 @@
         <v>: -&gt; : [label='2307-1818']</v>
       </c>
     </row>
-    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
         <v>22</v>
       </c>
@@ -10920,7 +11172,7 @@
         <v>not used: -&gt; : [label='2307-1819']</v>
       </c>
     </row>
-    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>23</v>
       </c>
@@ -10949,7 +11201,7 @@
         <v>unused: -&gt; : [label='2307-1820']</v>
       </c>
     </row>
-    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
         <v>24</v>
       </c>
@@ -10978,7 +11230,7 @@
         <v>unused: -&gt; : [label='2307-1821']</v>
       </c>
     </row>
-    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>30</v>
       </c>
@@ -11007,7 +11259,7 @@
         <v>unused: -&gt; : [label='2307-1822']</v>
       </c>
     </row>
-    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
         <v>52</v>
       </c>
@@ -11042,7 +11294,7 @@
         <v>zviua008:hdmi -&gt; zvkua003:in4 [label='2307-1828']</v>
       </c>
     </row>
-    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>47</v>
       </c>
@@ -11075,7 +11327,7 @@
         <v>cdmua001:usbc -&gt; zviue005:usbc [label='2307-1824']</v>
       </c>
     </row>
-    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="23" t="s">
         <v>49</v>
       </c>
@@ -11104,7 +11356,7 @@
         <v>unused: -&gt; : [label='2307-1825']</v>
       </c>
     </row>
-    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
         <v>50</v>
       </c>
@@ -11133,7 +11385,7 @@
         <v>unused: -&gt; : [label='2307-1826']</v>
       </c>
     </row>
-    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
         <v>64</v>
       </c>
@@ -11166,7 +11418,7 @@
         <v>zviua004:usb -&gt; cumug001:usb_3 [label='2307-2100']</v>
       </c>
     </row>
-    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
         <v>65</v>
       </c>
@@ -11201,7 +11453,7 @@
         <v>cumug001:ndi -&gt; cumue001:obs [label='2307-2101']</v>
       </c>
     </row>
-    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="s">
         <v>66</v>
       </c>
@@ -11234,7 +11486,7 @@
         <v>camera left: -&gt; cumue001:obs [label='2307-2102']</v>
       </c>
     </row>
-    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>67</v>
       </c>
@@ -11267,7 +11519,7 @@
         <v>camera centre: -&gt; cumue001:obs [label='2307-2103']</v>
       </c>
     </row>
-    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="15" t="s">
         <v>68</v>
       </c>
@@ -11300,7 +11552,7 @@
         <v>camera right: -&gt; cumue001:obs [label='2307-2104']</v>
       </c>
     </row>
-    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
         <v>69</v>
       </c>
@@ -11333,7 +11585,7 @@
         <v>cdmua001:ndi -&gt; cumue001:obs [label='2307-2105']</v>
       </c>
     </row>
-    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="15" t="s">
         <v>81</v>
       </c>
@@ -11366,7 +11618,7 @@
         <v>zvkua001:out_5_hdmi -&gt; zviuc001:hdmi in [label='2307-2300']</v>
       </c>
     </row>
-    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
         <v>85</v>
       </c>
@@ -11403,7 +11655,7 @@
         <v>zviuc001:hdmi out -&gt; zvkua003:in1 [label='2307-2301']</v>
       </c>
     </row>
-    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="15" t="s">
         <v>88</v>
       </c>
@@ -11438,7 +11690,7 @@
         <v>zvcua001:sdi -&gt; zvkua003:in5 [label='2307-2304']</v>
       </c>
     </row>
-    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
         <v>87</v>
       </c>
@@ -11473,7 +11725,7 @@
         <v>zvcua002:sdi -&gt; zvkua003:in6 [label='2307-2303']</v>
       </c>
     </row>
-    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="15" t="s">
         <v>86</v>
       </c>
@@ -11508,7 +11760,7 @@
         <v>zvcua003:sdi -&gt; zvkua003:in7 [label='2307-2302']</v>
       </c>
     </row>
-    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
         <v>95</v>
       </c>
@@ -11545,7 +11797,7 @@
         <v>23072306:barrel -&gt; zvkua003:in8 [label='2307-2305']</v>
       </c>
     </row>
-    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="15" t="s">
         <v>96</v>
       </c>
@@ -11580,7 +11832,7 @@
         <v>z150:sdi -&gt; 23072305:barrel [label='2307-2306']</v>
       </c>
     </row>
-    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
         <v>97</v>
       </c>
@@ -11607,7 +11859,7 @@
         <v>: -&gt; : [label='2307-2307']</v>
       </c>
     </row>
-    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="15" t="s">
         <v>101</v>
       </c>
@@ -11642,7 +11894,7 @@
         <v>zvkua004:sw -&gt; zvcua001:sw [label='2307-2308']</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
         <v>102</v>
       </c>
@@ -11685,7 +11937,7 @@
         <v>zvkua004:sw -&gt; zvcua002:sw [label='2307-2309']</v>
       </c>
     </row>
-    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="15" t="s">
         <v>103</v>
       </c>
@@ -11720,7 +11972,7 @@
         <v>zvkua004:sw -&gt; zvcua003:sw [label='2307-2310']</v>
       </c>
     </row>
-    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
         <v>106</v>
       </c>
@@ -11739,7 +11991,7 @@
         <v>: -&gt; : [label='2307-2311']</v>
       </c>
     </row>
-    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="15" t="s">
         <v>109</v>
       </c>
@@ -11758,7 +12010,7 @@
         <v>: -&gt; : [label='2307-2312']</v>
       </c>
     </row>
-    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
         <v>110</v>
       </c>
@@ -11777,7 +12029,7 @@
         <v>: -&gt; : [label='2307-2313']</v>
       </c>
     </row>
-    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="15" t="s">
         <v>111</v>
       </c>
@@ -11810,7 +12062,7 @@
         <v>zvkua001:out_4_HDbT -&gt; zvvu0001:HDbT [label='2307-2314']</v>
       </c>
     </row>
-    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
         <v>120</v>
       </c>
@@ -11845,7 +12097,7 @@
         <v>zvkua001:out_7_HDbT -&gt; zviua001:HDbT [label='2307-2315']</v>
       </c>
     </row>
-    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="15" t="s">
         <v>121</v>
       </c>
@@ -11878,7 +12130,7 @@
         <v>zviua001:hdmi -&gt; zvvulobby tv :hdmi 1 [label='2307-2316']</v>
       </c>
     </row>
-    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
         <v>122</v>
       </c>
@@ -11905,7 +12157,7 @@
         <v>: -&gt; : [label='2307-2317']</v>
       </c>
     </row>
-    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="15" t="s">
         <v>126</v>
       </c>
@@ -11940,7 +12192,7 @@
         <v>zvkua001:out_8_HDbT -&gt; zviua002:HDbT [label='2307-2318']</v>
       </c>
     </row>
-    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="11" t="s">
         <v>407</v>
       </c>
@@ -11971,7 +12223,7 @@
         <v>zviua002:hdmi -&gt; 23082900:input [label='2308-3001']</v>
       </c>
     </row>
-    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="15" t="s">
         <v>129</v>
       </c>
@@ -11998,7 +12250,7 @@
         <v>: -&gt; : [label='2307-2320']</v>
       </c>
     </row>
-    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
         <v>134</v>
       </c>
@@ -12031,7 +12283,7 @@
         <v>cdmua001:PP_Front_SW -&gt; hdmi_dongle: [label='2307-3000']</v>
       </c>
     </row>
-    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="15" t="s">
         <v>136</v>
       </c>
@@ -12064,7 +12316,7 @@
         <v>zvrua001:OutB -&gt; zvrua002:SDI In [label='2307-3001']</v>
       </c>
     </row>
-    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
         <v>138</v>
       </c>
@@ -12097,7 +12349,7 @@
         <v>zvrua001:OutA -&gt; zviua004:SDI In [label='2307-3002']</v>
       </c>
     </row>
-    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="15" t="s">
         <v>141</v>
       </c>
@@ -12132,7 +12384,7 @@
         <v>zviua004:hdmi out -&gt; zvkua001:in7 [label='2307-3003']</v>
       </c>
     </row>
-    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="11" t="s">
         <v>142</v>
       </c>
@@ -12151,7 +12403,7 @@
         <v>: -&gt; : [label='2307-3004']</v>
       </c>
     </row>
-    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="15" t="s">
         <v>143</v>
       </c>
@@ -12188,7 +12440,7 @@
         <v>zvkua003:out5 -&gt; zvrua001:sdi in [label='2307-3005']</v>
       </c>
     </row>
-    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" s="11" t="s">
         <v>144</v>
       </c>
@@ -12225,7 +12477,7 @@
         <v>zvkua003:out6 -&gt; zviud002:sdi in [label='2307-3006']</v>
       </c>
     </row>
-    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" s="15" t="s">
         <v>147</v>
       </c>
@@ -12258,7 +12510,7 @@
         <v>zviud001:hdmi -&gt; zviua004:hdmi in [label='2307-3007']</v>
       </c>
     </row>
-    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">
         <v>160</v>
       </c>
@@ -12293,7 +12545,7 @@
         <v>zviua005:hdmi -&gt; zvkua001:in6 [label='2308-0800']</v>
       </c>
     </row>
-    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" s="15" t="s">
         <v>202</v>
       </c>
@@ -12325,7 +12577,7 @@
         <v>unused:  -&gt; : [label='2308-0004']</v>
       </c>
     </row>
-    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="11" t="s">
         <v>203</v>
       </c>
@@ -12358,7 +12610,7 @@
         <v>frontguest: -&gt; 23080003:InputC [label='2308-0005']</v>
       </c>
     </row>
-    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" s="15" t="s">
         <v>204</v>
       </c>
@@ -12393,7 +12645,7 @@
         <v>cdwua002:HdmiOut -&gt; 23080002:In2 [label='2308-0006']</v>
       </c>
     </row>
-    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" s="11" t="s">
         <v>205</v>
       </c>
@@ -12426,7 +12678,7 @@
         <v>rearguest:hdmi_out -&gt; 23080002:In1 [label='2308-0007']</v>
       </c>
     </row>
-    <row r="69" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" s="15" t="s">
         <v>206</v>
       </c>
@@ -12459,7 +12711,7 @@
         <v>cdwua002:vga -&gt; vmnu0029:vga [label='2308-0009']</v>
       </c>
     </row>
-    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" s="11" t="s">
         <v>207</v>
       </c>
@@ -12492,7 +12744,7 @@
         <v>cdwua002:usb -&gt; 23080008:usb [label='2308-0010']</v>
       </c>
     </row>
-    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" s="11" t="s">
         <v>183</v>
       </c>
@@ -12525,7 +12777,7 @@
         <v>zviug003:hdmi_out -&gt; zvkua001:in1 [label='2308-0915']</v>
       </c>
     </row>
-    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72" s="15" t="s">
         <v>184</v>
       </c>
@@ -12558,7 +12810,7 @@
         <v>zviug004:hdmi_out -&gt; zvkua001:in2 [label='2308-0916']</v>
       </c>
     </row>
-    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" s="11" t="s">
         <v>185</v>
       </c>
@@ -12591,7 +12843,7 @@
         <v>zviug005:hdmi_out -&gt; zvkua001:in3 [label='2308-0917']</v>
       </c>
     </row>
-    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" s="15" t="s">
         <v>186</v>
       </c>
@@ -12621,7 +12873,7 @@
       <c r="K74" s="17"/>
       <c r="L74" s="18"/>
     </row>
-    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" s="11" t="s">
         <v>193</v>
       </c>
@@ -12662,7 +12914,7 @@
         <v>zvkua001:out_1_HDbT -&gt; zvvua001:InputD [label='PROJ0001']</v>
       </c>
     </row>
-    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" s="15" t="s">
         <v>194</v>
       </c>
@@ -12703,7 +12955,7 @@
         <v>zvkua001:out_2_HDbT -&gt; zvvua002:InputD [label='PROJ0002']</v>
       </c>
     </row>
-    <row r="77" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" s="11" t="s">
         <v>195</v>
       </c>
@@ -12744,7 +12996,7 @@
         <v>zvkua001:out_3_HDbT -&gt; zvvua003:InputD [label='PROJ0003']</v>
       </c>
     </row>
-    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78" s="15" t="s">
         <v>200</v>
       </c>
@@ -12787,7 +13039,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" s="11" t="s">
         <v>213</v>
       </c>
@@ -12828,7 +13080,7 @@
         <v>cumue001:usba_2 -&gt; 23081110:usb_in [label='2308-1111']</v>
       </c>
     </row>
-    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80" s="15" t="s">
         <v>228</v>
       </c>
@@ -12861,7 +13113,7 @@
         <v>23081110:usb_1 -&gt; 23081104:usb [label='2308-1112']</v>
       </c>
     </row>
-    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" s="11" t="s">
         <v>229</v>
       </c>
@@ -12894,7 +13146,7 @@
         <v>23081110:usb_2 -&gt; 23081105:usb [label='2308-1113']</v>
       </c>
     </row>
-    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82" s="15" t="s">
         <v>230</v>
       </c>
@@ -12931,7 +13183,7 @@
         <v>cumue001:usbc -&gt; 23081106:hdmi [label='2308-1114']</v>
       </c>
     </row>
-    <row r="83" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" s="11" t="s">
         <v>231</v>
       </c>
@@ -12966,7 +13218,7 @@
         <v>cumue001:hdmi -&gt; 23081107:hdmi [label='2308-1115']</v>
       </c>
     </row>
-    <row r="84" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84" s="15" t="s">
         <v>232</v>
       </c>
@@ -12999,7 +13251,7 @@
         <v>23081110:usb  -&gt; 23081103:usb [label='2308-1116']</v>
       </c>
     </row>
-    <row r="85" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A85" s="11" t="s">
         <v>233</v>
       </c>
@@ -13040,7 +13292,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86" s="15" t="s">
         <v>234</v>
       </c>
@@ -13081,7 +13333,7 @@
         <v>23081100:port3 -&gt; zaiue002:ether [label='2308-1118']</v>
       </c>
     </row>
-    <row r="87" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87" s="11" t="s">
         <v>235</v>
       </c>
@@ -13122,7 +13374,7 @@
         <v>23081100:port4 -&gt; daw_guest:ether [label='2308-1119']</v>
       </c>
     </row>
-    <row r="88" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88" s="15" t="s">
         <v>236</v>
       </c>
@@ -13158,7 +13410,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="89" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89" s="11" t="s">
         <v>237</v>
       </c>
@@ -13199,7 +13451,7 @@
         <v>zaiue002:Ch2 -&gt; 23081102:right [label='2308-1121']</v>
       </c>
     </row>
-    <row r="90" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A90" s="15" t="s">
         <v>238</v>
       </c>
@@ -13242,7 +13494,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="91" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A91" s="11" t="s">
         <v>243</v>
       </c>
@@ -13285,7 +13537,7 @@
         <v>23081124:ch1 -&gt; zvkua003:ch1_audio [label='2308-1124L']</v>
       </c>
     </row>
-    <row r="92" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A92" s="15" t="s">
         <v>247</v>
       </c>
@@ -13320,7 +13572,7 @@
         <v>23081124:ch2 -&gt; zvkua003:ch2_audio [label='2308-1124R']</v>
       </c>
     </row>
-    <row r="93" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A93" s="11" t="s">
         <v>688</v>
       </c>
@@ -13338,7 +13590,7 @@
         <v>: -&gt; : [label='x93']</v>
       </c>
     </row>
-    <row r="94" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A94" s="15" t="s">
         <v>689</v>
       </c>
@@ -13356,7 +13608,7 @@
         <v>: -&gt; : [label='x94']</v>
       </c>
     </row>
-    <row r="95" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A95" s="11" t="s">
         <v>658</v>
       </c>
@@ -13389,7 +13641,7 @@
         <v>zakua001:aux_4 -&gt; 23080008:Mic_In [label='2309-2505']</v>
       </c>
     </row>
-    <row r="96" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A96" s="11"/>
       <c r="B96" s="12" t="s">
         <v>72</v>
@@ -13428,7 +13680,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="97" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A97" s="15"/>
       <c r="B97" s="16" t="s">
         <v>72</v>
@@ -13467,7 +13719,7 @@
         <v>cumug001:usb_2 -&gt; zviug001:usb_in [label='']</v>
       </c>
     </row>
-    <row r="98" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A98" s="11"/>
       <c r="B98" s="12" t="s">
         <v>72</v>
@@ -13508,7 +13760,7 @@
         <v>cumug001:usb_1 -&gt; 23081202:usb [label='']</v>
       </c>
     </row>
-    <row r="99" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A99" s="15"/>
       <c r="B99" s="16" t="s">
         <v>256</v>
@@ -13549,7 +13801,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="100" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A100" s="11" t="s">
         <v>332</v>
       </c>
@@ -13592,7 +13844,7 @@
         <v>23081204:sdi_out -&gt; zviue003:sdi_in [label='2307-1201']</v>
       </c>
     </row>
-    <row r="101" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A101" s="15" t="s">
         <v>333</v>
       </c>
@@ -13627,7 +13879,7 @@
         <v>23081205:sdi_out -&gt; zviua008:sdi_in [label='2307-1202']</v>
       </c>
     </row>
-    <row r="102" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A102" s="11" t="s">
         <v>51</v>
       </c>
@@ -13662,7 +13914,7 @@
         <v>zviue003:hdmi_out -&gt; zvkua003:in2 [label='2307-1827']</v>
       </c>
     </row>
-    <row r="103" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A103" s="15"/>
       <c r="B103" s="16" t="s">
         <v>278</v>
@@ -13693,7 +13945,7 @@
         <v>cdwu0009:vga -&gt; mon:vga [label='']</v>
       </c>
     </row>
-    <row r="104" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A104" s="11" t="s">
         <v>280</v>
       </c>
@@ -13728,7 +13980,7 @@
         <v>prwall3:label3 -&gt; 23081100:port1 [label='2308-2001']</v>
       </c>
     </row>
-    <row r="105" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A105" s="15" t="s">
         <v>291</v>
       </c>
@@ -13761,7 +14013,7 @@
         <v>23081102:Right -&gt; 23082003:Right [label='2308-2002']</v>
       </c>
     </row>
-    <row r="106" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A106" s="11" t="s">
         <v>302</v>
       </c>
@@ -13794,7 +14046,7 @@
         <v>patchpanel:a -&gt; prwall3:b1 [label='a']</v>
       </c>
     </row>
-    <row r="107" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A107" s="15" t="s">
         <v>303</v>
       </c>
@@ -13827,7 +14079,7 @@
         <v>modem:c -&gt; router:d [label='b']</v>
       </c>
     </row>
-    <row r="108" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A108" s="11" t="s">
         <v>304</v>
       </c>
@@ -13860,7 +14112,7 @@
         <v>router:e -&gt; nscua001:f [label='c']</v>
       </c>
     </row>
-    <row r="109" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A109" s="15" t="s">
         <v>309</v>
       </c>
@@ -13893,7 +14145,7 @@
         <v>nscua001:h -&gt; patchpanel:i [label='g']</v>
       </c>
     </row>
-    <row r="110" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A110" s="11"/>
       <c r="B110" s="12" t="s">
         <v>301</v>
@@ -13920,7 +14172,7 @@
         <v>nscua001:a  -&gt; nscua002:f [label='']</v>
       </c>
     </row>
-    <row r="111" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A111" s="15"/>
       <c r="B111" s="16" t="s">
         <v>301</v>
@@ -13947,7 +14199,7 @@
         <v>nscua001:b  -&gt; nscua005:g [label='']</v>
       </c>
     </row>
-    <row r="112" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A112" s="11"/>
       <c r="B112" s="12" t="s">
         <v>320</v>
@@ -13972,7 +14224,7 @@
         <v>nscua005:c  -&gt; nscua003:h  [label='']</v>
       </c>
     </row>
-    <row r="113" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A113" s="15"/>
       <c r="B113" s="16" t="s">
         <v>322</v>
@@ -14001,7 +14253,7 @@
         <v>nscua003:d  -&gt; nscua004:i [label='']</v>
       </c>
     </row>
-    <row r="114" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A114" s="11"/>
       <c r="B114" s="12" t="s">
         <v>323</v>
@@ -14026,7 +14278,7 @@
         <v>nscua004:e  -&gt; 23081124:ether [label='']</v>
       </c>
     </row>
-    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A115" s="15" t="s">
         <v>366</v>
       </c>
@@ -14059,7 +14311,7 @@
         <v>cumug001:usb -&gt; zviuc002:usbc [label='future1']</v>
       </c>
     </row>
-    <row r="116" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A116" s="15" t="s">
         <v>369</v>
       </c>
@@ -14092,7 +14344,7 @@
         <v>cdwu0009:hdmi_out -&gt; zvkua001:in5 [label='2308-2500']</v>
       </c>
     </row>
-    <row r="117" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A117" s="11" t="s">
         <v>372</v>
       </c>
@@ -14127,7 +14379,7 @@
         <v>zviue001:hdmi_out -&gt; zvkua001:in4 [label='2308-2501']</v>
       </c>
     </row>
-    <row r="118" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A118" s="15" t="s">
         <v>373</v>
       </c>
@@ -14156,7 +14408,7 @@
         <v>not used: -&gt; : [label='2308-2502']</v>
       </c>
     </row>
-    <row r="119" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A119" s="11" t="s">
         <v>376</v>
       </c>
@@ -14185,7 +14437,7 @@
         <v>not used: -&gt; : [label='2308-2503']</v>
       </c>
     </row>
-    <row r="120" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A120" s="15" t="s">
         <v>383</v>
       </c>
@@ -14212,7 +14464,7 @@
         <v>not used: -&gt; : [label='2308-2504']</v>
       </c>
     </row>
-    <row r="121" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A121" s="11" t="s">
         <v>384</v>
       </c>
@@ -14247,7 +14499,7 @@
         <v>ncsua004:portxx -&gt; cdmua001:ether [label='2308-2600']</v>
       </c>
     </row>
-    <row r="122" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A122" s="15" t="s">
         <v>385</v>
       </c>
@@ -14272,7 +14524,7 @@
         <v>not used: -&gt; : [label='2308-2700']</v>
       </c>
     </row>
-    <row r="123" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A123" s="11" t="s">
         <v>386</v>
       </c>
@@ -14297,7 +14549,7 @@
         <v>not used: -&gt; : [label='2308-2701']</v>
       </c>
     </row>
-    <row r="124" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A124" s="15" t="s">
         <v>387</v>
       </c>
@@ -14322,7 +14574,7 @@
         <v>unused: -&gt; : [label='2308-2702']</v>
       </c>
     </row>
-    <row r="125" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A125" s="11" t="s">
         <v>395</v>
       </c>
@@ -14359,7 +14611,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="126" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A126" s="15" t="s">
         <v>22</v>
       </c>
@@ -14402,7 +14654,7 @@
         <v>23082900:output2 -&gt; zvvu0003:hdmi1 [label='2307-1819']</v>
       </c>
     </row>
-    <row r="127" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A127" s="11" t="s">
         <v>406</v>
       </c>
@@ -14443,7 +14695,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="128" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A128" s="15" t="s">
         <v>403</v>
       </c>
@@ -14484,7 +14736,7 @@
         <v>zvkua001:out6 -&gt; unknown:unk [label='future135']</v>
       </c>
     </row>
-    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A129" s="11"/>
       <c r="B129" s="12"/>
       <c r="C129" s="13"/>
@@ -14503,7 +14755,7 @@
         <v>: -&gt; :unk [label='']</v>
       </c>
     </row>
-    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A130" s="15" t="s">
         <v>411</v>
       </c>
@@ -14538,7 +14790,7 @@
         <v>zamua001:ch1 -&gt; zaiub001:s2_in01 [label='2309-1001']</v>
       </c>
     </row>
-    <row r="131" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A131" s="11" t="s">
         <v>536</v>
       </c>
@@ -14573,7 +14825,7 @@
         <v>zamua001:ch2 -&gt; zaiub001:s2_in02 [label='2309-1002']</v>
       </c>
     </row>
-    <row r="132" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A132" s="15" t="s">
         <v>537</v>
       </c>
@@ -14608,7 +14860,7 @@
         <v>zamua001:ch3 -&gt; zaiub001:s2_in03 [label='2309-1003']</v>
       </c>
     </row>
-    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A133" s="11" t="s">
         <v>538</v>
       </c>
@@ -14643,7 +14895,7 @@
         <v>zamua001:ch4 -&gt; zaiub001:s2_in04 [label='2309-1004']</v>
       </c>
     </row>
-    <row r="134" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A134" s="15" t="s">
         <v>539</v>
       </c>
@@ -14678,7 +14930,7 @@
         <v>zamub001:ch1 -&gt; zaiub001:s2_in05 [label='2309-1005']</v>
       </c>
     </row>
-    <row r="135" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A135" s="11" t="s">
         <v>540</v>
       </c>
@@ -14713,7 +14965,7 @@
         <v>zamub001:ch2 -&gt; zaiub001:s2_in06 [label='2309-1006']</v>
       </c>
     </row>
-    <row r="136" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A136" s="15" t="s">
         <v>541</v>
       </c>
@@ -14748,7 +15000,7 @@
         <v>zamub001:ch3 -&gt; zaiub001:s2_in07 [label='2309-1007']</v>
       </c>
     </row>
-    <row r="137" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A137" s="11" t="s">
         <v>542</v>
       </c>
@@ -14783,7 +15035,7 @@
         <v>zamub001:ch4 -&gt; zaiub001:s2_in08 [label='2309-1008']</v>
       </c>
     </row>
-    <row r="138" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A138" s="15" t="s">
         <v>543</v>
       </c>
@@ -14818,7 +15070,7 @@
         <v>zamub002:ch1 -&gt; zaiub001:s2_in09 [label='2309-1009']</v>
       </c>
     </row>
-    <row r="139" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A139" s="11" t="s">
         <v>544</v>
       </c>
@@ -14853,7 +15105,7 @@
         <v>zamub002:ch2 -&gt; zaiub001:s2_in10 [label='2309-1010']</v>
       </c>
     </row>
-    <row r="140" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A140" s="15" t="s">
         <v>545</v>
       </c>
@@ -14888,7 +15140,7 @@
         <v>zamub002:ch3 -&gt; zaiub001:s2_in11 [label='2309-1011']</v>
       </c>
     </row>
-    <row r="141" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A141" s="11" t="s">
         <v>546</v>
       </c>
@@ -14923,7 +15175,7 @@
         <v>zamub002:ch4 -&gt; zaiub001:s2_in12 [label='2309-1012']</v>
       </c>
     </row>
-    <row r="142" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A142" s="15" t="s">
         <v>547</v>
       </c>
@@ -14958,7 +15210,7 @@
         <v>zamub003:ch4 -&gt; zaiub001:s2___ [label='2309-1013']</v>
       </c>
     </row>
-    <row r="143" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A143" s="11" t="s">
         <v>548</v>
       </c>
@@ -14993,7 +15245,7 @@
         <v>zamub002:ch3 -&gt; zaiub002:s2_in01 [label='2309-1014']</v>
       </c>
     </row>
-    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A144" s="9" t="s">
         <v>549</v>
       </c>
@@ -15028,7 +15280,7 @@
         <v>zamub002:ch4 -&gt; zaiub002:s2_in02 [label='2309-1015']</v>
       </c>
     </row>
-    <row r="145" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>550</v>
       </c>
@@ -15061,7 +15313,7 @@
         <v>zamub003:ch1 -&gt; zaiub002:s2_in03 [label='2309-1016']</v>
       </c>
     </row>
-    <row r="146" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>551</v>
       </c>
@@ -15094,7 +15346,7 @@
         <v>zamub003:ch2 -&gt; zaiub002:s2_in04 [label='2309-1017']</v>
       </c>
     </row>
-    <row r="147" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>552</v>
       </c>
@@ -15127,7 +15379,7 @@
         <v>zamub003:ch3 -&gt; zaiub002:s2_in05 [label='2309-1018']</v>
       </c>
     </row>
-    <row r="148" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>553</v>
       </c>
@@ -15156,7 +15408,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="149" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>554</v>
       </c>
@@ -15182,7 +15434,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="150" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>555</v>
       </c>
@@ -15208,7 +15460,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="151" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A151" s="8" t="s">
         <v>556</v>
       </c>
@@ -15234,7 +15486,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="152" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>557</v>
       </c>
@@ -15260,7 +15512,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="153" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>558</v>
       </c>
@@ -15286,7 +15538,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="154" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>559</v>
       </c>
@@ -15312,7 +15564,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="155" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>560</v>
       </c>
@@ -15338,7 +15590,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="156" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>561</v>
       </c>
@@ -15364,7 +15616,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="157" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>562</v>
       </c>
@@ -15390,7 +15642,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="158" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>563</v>
       </c>
@@ -15416,7 +15668,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="159" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>564</v>
       </c>
@@ -15442,7 +15694,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="160" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>565</v>
       </c>
@@ -15468,7 +15720,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="161" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>566</v>
       </c>
@@ -15494,7 +15746,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="162" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>567</v>
       </c>
@@ -15520,7 +15772,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="163" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>568</v>
       </c>
@@ -15546,7 +15798,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="164" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>569</v>
       </c>
@@ -15572,7 +15824,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="165" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>570</v>
       </c>
@@ -15598,7 +15850,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="166" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>571</v>
       </c>
@@ -15624,7 +15876,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="167" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>572</v>
       </c>
@@ -15650,7 +15902,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="168" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>573</v>
       </c>
@@ -15676,7 +15928,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="169" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>574</v>
       </c>
@@ -15702,7 +15954,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="170" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>575</v>
       </c>
@@ -15728,7 +15980,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="171" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>576</v>
       </c>
@@ -15748,7 +16000,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="172" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>577</v>
       </c>
@@ -15768,7 +16020,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="173" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>578</v>
       </c>
@@ -15788,7 +16040,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="174" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>579</v>
       </c>
@@ -15808,7 +16060,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="175" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>580</v>
       </c>
@@ -15828,7 +16080,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="176" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>581</v>
       </c>
@@ -15848,7 +16100,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="177" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>582</v>
       </c>
@@ -15868,7 +16120,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="178" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>583</v>
       </c>
@@ -15888,7 +16140,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="179" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>584</v>
       </c>
@@ -15908,7 +16160,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="180" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>585</v>
       </c>
@@ -15928,7 +16180,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="181" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>586</v>
       </c>
@@ -15948,7 +16200,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="182" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>587</v>
       </c>
@@ -15968,7 +16220,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="183" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>588</v>
       </c>
@@ -15988,7 +16240,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="184" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>589</v>
       </c>
@@ -16008,7 +16260,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="185" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>590</v>
       </c>
@@ -16028,7 +16280,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="186" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>591</v>
       </c>
@@ -16048,7 +16300,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="187" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>592</v>
       </c>
@@ -16068,7 +16320,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="188" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>593</v>
       </c>
@@ -16088,7 +16340,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>594</v>
       </c>
@@ -16108,7 +16360,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>595</v>
       </c>
@@ -16128,7 +16380,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>596</v>
       </c>
@@ -16148,7 +16400,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="192" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>597</v>
       </c>
@@ -16168,7 +16420,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="193" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>598</v>
       </c>
@@ -16188,7 +16440,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="194" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>599</v>
       </c>
@@ -16208,7 +16460,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="195" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>600</v>
       </c>
@@ -16228,7 +16480,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="196" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>601</v>
       </c>
@@ -16248,7 +16500,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="197" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>602</v>
       </c>
@@ -16268,7 +16520,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="198" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>603</v>
       </c>
@@ -16288,7 +16540,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="199" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>604</v>
       </c>
@@ -16308,7 +16560,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="200" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>605</v>
       </c>
@@ -16328,7 +16580,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="201" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>606</v>
       </c>
@@ -16348,7 +16600,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="202" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>607</v>
       </c>
@@ -16368,7 +16620,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="203" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>608</v>
       </c>
@@ -16397,7 +16649,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="204" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>609</v>
       </c>
@@ -16426,7 +16678,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="205" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>610</v>
       </c>
@@ -16455,7 +16707,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="206" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>611</v>
       </c>
@@ -16484,7 +16736,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="207" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>618</v>
       </c>
@@ -16516,7 +16768,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="208" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>619</v>
       </c>
@@ -16543,7 +16795,7 @@
       </c>
       <c r="K208" s="3"/>
     </row>
-    <row r="209" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>623</v>
       </c>
@@ -16572,7 +16824,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="210" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>631</v>
       </c>
@@ -16602,7 +16854,7 @@
       </c>
       <c r="K210" s="3"/>
     </row>
-    <row r="211" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>632</v>
       </c>
@@ -16632,7 +16884,7 @@
       </c>
       <c r="K211" s="3"/>
     </row>
-    <row r="212" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B212" s="3" t="s">
         <v>635</v>
       </c>
@@ -16662,7 +16914,7 @@
       </c>
       <c r="K212" s="3"/>
     </row>
-    <row r="213" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B213" s="33" t="s">
         <v>637</v>
       </c>
@@ -16689,11 +16941,11 @@
       </c>
       <c r="K213" s="3"/>
     </row>
-    <row r="214" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.2">
       <c r="F214" s="3"/>
       <c r="K214" s="3"/>
     </row>
-    <row r="215" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>809</v>
       </c>
@@ -16716,7 +16968,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="216" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>649</v>
       </c>
@@ -16746,7 +16998,7 @@
       </c>
       <c r="K216" s="3"/>
     </row>
-    <row r="217" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>655</v>
       </c>
@@ -16776,7 +17028,7 @@
       </c>
       <c r="K217" s="3"/>
     </row>
-    <row r="218" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>658</v>
       </c>
@@ -16806,7 +17058,7 @@
       </c>
       <c r="K218" s="3"/>
     </row>
-    <row r="219" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>662</v>
       </c>
@@ -16836,7 +17088,7 @@
       </c>
       <c r="K219" s="3"/>
     </row>
-    <row r="220" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>663</v>
       </c>
@@ -16866,7 +17118,7 @@
       </c>
       <c r="K220" s="3"/>
     </row>
-    <row r="221" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A221" s="44" t="s">
         <v>670</v>
       </c>
@@ -16896,7 +17148,7 @@
       </c>
       <c r="K221" s="3"/>
     </row>
-    <row r="222" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>671</v>
       </c>
@@ -16926,7 +17178,7 @@
       </c>
       <c r="K222" s="3"/>
     </row>
-    <row r="223" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>676</v>
       </c>
@@ -16953,7 +17205,7 @@
       </c>
       <c r="K223" s="3"/>
     </row>
-    <row r="224" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>677</v>
       </c>
@@ -16980,7 +17232,7 @@
       </c>
       <c r="K224" s="3"/>
     </row>
-    <row r="225" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>678</v>
       </c>
@@ -17007,7 +17259,7 @@
       </c>
       <c r="K225" s="3"/>
     </row>
-    <row r="226" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>888</v>
       </c>
@@ -17034,7 +17286,7 @@
       </c>
       <c r="K226" s="3"/>
     </row>
-    <row r="227" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>889</v>
       </c>
@@ -17061,7 +17313,7 @@
       </c>
       <c r="K227" s="3"/>
     </row>
-    <row r="228" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>694</v>
       </c>
@@ -17082,7 +17334,7 @@
       </c>
       <c r="K228" s="3"/>
     </row>
-    <row r="229" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>773</v>
       </c>
@@ -17109,7 +17361,7 @@
       </c>
       <c r="K229" s="3"/>
     </row>
-    <row r="230" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>708</v>
       </c>
@@ -17124,7 +17376,7 @@
       </c>
       <c r="K230" s="3"/>
     </row>
-    <row r="231" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>709</v>
       </c>
@@ -17145,7 +17397,7 @@
       </c>
       <c r="K231" s="3"/>
     </row>
-    <row r="232" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>710</v>
       </c>
@@ -17166,7 +17418,7 @@
       </c>
       <c r="K232" s="3"/>
     </row>
-    <row r="233" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>711</v>
       </c>
@@ -17187,7 +17439,7 @@
       </c>
       <c r="K233" s="3"/>
     </row>
-    <row r="234" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>774</v>
       </c>
@@ -17211,7 +17463,7 @@
       </c>
       <c r="K234" s="3"/>
     </row>
-    <row r="235" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>791</v>
       </c>
@@ -17235,7 +17487,7 @@
       </c>
       <c r="K235" s="3"/>
     </row>
-    <row r="236" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A236" s="3" t="s">
         <v>793</v>
       </c>
@@ -17265,7 +17517,7 @@
       </c>
       <c r="K236" s="3"/>
     </row>
-    <row r="237" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>788</v>
       </c>
@@ -17292,7 +17544,7 @@
       </c>
       <c r="K237" s="3"/>
     </row>
-    <row r="238" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>775</v>
       </c>
@@ -17316,7 +17568,7 @@
       </c>
       <c r="K238" s="3"/>
     </row>
-    <row r="239" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>776</v>
       </c>
@@ -17346,7 +17598,7 @@
       </c>
       <c r="K239" s="3"/>
     </row>
-    <row r="240" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>778</v>
       </c>
@@ -17373,7 +17625,7 @@
       </c>
       <c r="K240" s="3"/>
     </row>
-    <row r="241" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>714</v>
       </c>
@@ -17394,7 +17646,7 @@
       </c>
       <c r="K241" s="3"/>
     </row>
-    <row r="242" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>715</v>
       </c>
@@ -17413,7 +17665,7 @@
       <c r="F242" s="3"/>
       <c r="K242" s="3"/>
     </row>
-    <row r="243" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>716</v>
       </c>
@@ -17434,7 +17686,7 @@
       </c>
       <c r="K243" s="3"/>
     </row>
-    <row r="244" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>801</v>
       </c>
@@ -17455,7 +17707,7 @@
       </c>
       <c r="K244" s="3"/>
     </row>
-    <row r="245" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>741</v>
       </c>
@@ -17474,7 +17726,7 @@
       <c r="F245" s="3"/>
       <c r="K245" s="3"/>
     </row>
-    <row r="246" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>747</v>
       </c>
@@ -17501,7 +17753,7 @@
       </c>
       <c r="K246" s="3"/>
     </row>
-    <row r="247" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>740</v>
       </c>
@@ -17520,7 +17772,7 @@
       <c r="F247" s="3"/>
       <c r="K247" s="3"/>
     </row>
-    <row r="248" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>739</v>
       </c>
@@ -17539,7 +17791,7 @@
       <c r="F248" s="3"/>
       <c r="K248" s="3"/>
     </row>
-    <row r="249" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>738</v>
       </c>
@@ -17558,7 +17810,7 @@
       <c r="F249" s="3"/>
       <c r="K249" s="3"/>
     </row>
-    <row r="250" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>744</v>
       </c>
@@ -17585,7 +17837,7 @@
       </c>
       <c r="K250" s="3"/>
     </row>
-    <row r="251" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>745</v>
       </c>
@@ -17612,7 +17864,7 @@
       </c>
       <c r="K251" s="3"/>
     </row>
-    <row r="252" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>746</v>
       </c>
@@ -17639,7 +17891,7 @@
       </c>
       <c r="K252" s="3"/>
     </row>
-    <row r="253" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>737</v>
       </c>
@@ -17658,7 +17910,7 @@
       <c r="F253" s="3"/>
       <c r="K253" s="3"/>
     </row>
-    <row r="254" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>736</v>
       </c>
@@ -17677,7 +17929,7 @@
       <c r="F254" s="3"/>
       <c r="K254" s="3"/>
     </row>
-    <row r="255" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>749</v>
       </c>
@@ -17707,7 +17959,7 @@
       </c>
       <c r="K255" s="3"/>
     </row>
-    <row r="256" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>750</v>
       </c>
@@ -17731,7 +17983,7 @@
       </c>
       <c r="K256" s="3"/>
     </row>
-    <row r="257" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>753</v>
       </c>
@@ -17752,7 +18004,7 @@
       </c>
       <c r="K257" s="3"/>
     </row>
-    <row r="258" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>767</v>
       </c>
@@ -17773,7 +18025,7 @@
       </c>
       <c r="K258" s="3"/>
     </row>
-    <row r="259" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>768</v>
       </c>
@@ -17794,7 +18046,7 @@
       </c>
       <c r="K259" s="3"/>
     </row>
-    <row r="260" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>769</v>
       </c>
@@ -17815,7 +18067,7 @@
       </c>
       <c r="K260" s="3"/>
     </row>
-    <row r="261" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>770</v>
       </c>
@@ -17836,7 +18088,7 @@
       </c>
       <c r="K261" s="3"/>
     </row>
-    <row r="262" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>771</v>
       </c>
@@ -17857,7 +18109,7 @@
       </c>
       <c r="K262" s="3"/>
     </row>
-    <row r="263" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>772</v>
       </c>
@@ -17878,7 +18130,7 @@
       </c>
       <c r="K263" s="3"/>
     </row>
-    <row r="264" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>783</v>
       </c>
@@ -17902,7 +18154,7 @@
       </c>
       <c r="K264" s="3"/>
     </row>
-    <row r="265" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>784</v>
       </c>
@@ -17923,7 +18175,7 @@
       </c>
       <c r="K265" s="3"/>
     </row>
-    <row r="266" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>802</v>
       </c>
@@ -17944,7 +18196,7 @@
       </c>
       <c r="K266" s="3"/>
     </row>
-    <row r="267" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>804</v>
       </c>
@@ -17962,7 +18214,7 @@
       </c>
       <c r="K267" s="3"/>
     </row>
-    <row r="268" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>806</v>
       </c>
@@ -17980,7 +18232,7 @@
       </c>
       <c r="K268" s="3"/>
     </row>
-    <row r="269" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>808</v>
       </c>
@@ -17998,7 +18250,7 @@
       </c>
       <c r="K269" s="3"/>
     </row>
-    <row r="270" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>810</v>
       </c>
@@ -18016,7 +18268,7 @@
       </c>
       <c r="K270" s="3"/>
     </row>
-    <row r="271" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>814</v>
       </c>
@@ -18034,7 +18286,7 @@
       </c>
       <c r="K271" s="3"/>
     </row>
-    <row r="272" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>815</v>
       </c>
@@ -18064,7 +18316,7 @@
       </c>
       <c r="K272" s="3"/>
     </row>
-    <row r="273" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>830</v>
       </c>
@@ -18091,7 +18343,7 @@
       </c>
       <c r="K273" s="3"/>
     </row>
-    <row r="274" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>816</v>
       </c>
@@ -18112,7 +18364,7 @@
       </c>
       <c r="K274" s="3"/>
     </row>
-    <row r="275" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>819</v>
       </c>
@@ -18133,7 +18385,7 @@
       </c>
       <c r="K275" s="3"/>
     </row>
-    <row r="276" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>822</v>
       </c>
@@ -18151,7 +18403,7 @@
       </c>
       <c r="K276" s="3"/>
     </row>
-    <row r="277" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>823</v>
       </c>
@@ -18169,7 +18421,7 @@
       </c>
       <c r="K277" s="3"/>
     </row>
-    <row r="278" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>825</v>
       </c>
@@ -18187,7 +18439,7 @@
       </c>
       <c r="K278" s="3"/>
     </row>
-    <row r="279" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>826</v>
       </c>
@@ -18208,7 +18460,7 @@
       </c>
       <c r="K279" s="3"/>
     </row>
-    <row r="280" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>828</v>
       </c>
@@ -18230,7 +18482,7 @@
       </c>
       <c r="K280" s="3"/>
     </row>
-    <row r="281" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>838</v>
       </c>
@@ -18251,7 +18503,7 @@
       </c>
       <c r="K281" s="3"/>
     </row>
-    <row r="282" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>840</v>
       </c>
@@ -18278,7 +18530,7 @@
       </c>
       <c r="K282" s="3"/>
     </row>
-    <row r="283" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A283" s="3" t="s">
         <v>845</v>
       </c>
@@ -18305,7 +18557,7 @@
       </c>
       <c r="K283" s="3"/>
     </row>
-    <row r="284" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>846</v>
       </c>
@@ -18329,7 +18581,7 @@
       </c>
       <c r="K284" s="3"/>
     </row>
-    <row r="285" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>853</v>
       </c>
@@ -18348,7 +18600,7 @@
       </c>
       <c r="K285" s="3"/>
     </row>
-    <row r="286" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A286" s="39" t="s">
         <v>855</v>
       </c>
@@ -18381,7 +18633,7 @@
       </c>
       <c r="K286" s="3"/>
     </row>
-    <row r="287" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A287" s="40" t="s">
         <v>856</v>
       </c>
@@ -18414,7 +18666,7 @@
       </c>
       <c r="K287" s="3"/>
     </row>
-    <row r="288" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A288" s="42" t="s">
         <v>857</v>
       </c>
@@ -18447,7 +18699,7 @@
       </c>
       <c r="K288" s="3"/>
     </row>
-    <row r="289" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A289" s="44" t="s">
         <v>858</v>
       </c>
@@ -18480,7 +18732,7 @@
       </c>
       <c r="K289" s="3"/>
     </row>
-    <row r="290" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>869</v>
       </c>
@@ -18507,7 +18759,7 @@
       </c>
       <c r="K290" s="3"/>
     </row>
-    <row r="291" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>870</v>
       </c>
@@ -18537,7 +18789,7 @@
       </c>
       <c r="K291" s="3"/>
     </row>
-    <row r="292" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>872</v>
       </c>
@@ -18564,7 +18816,7 @@
       </c>
       <c r="K292" s="3"/>
     </row>
-    <row r="293" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A293" s="44" t="s">
         <v>874</v>
       </c>
@@ -18597,7 +18849,7 @@
       </c>
       <c r="K293" s="3"/>
     </row>
-    <row r="294" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A294" s="40" t="s">
         <v>927</v>
       </c>
@@ -18627,7 +18879,7 @@
       </c>
       <c r="K294" s="3"/>
     </row>
-    <row r="295" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A295" s="39" t="s">
         <v>926</v>
       </c>
@@ -18657,7 +18909,7 @@
       </c>
       <c r="K295" s="3"/>
     </row>
-    <row r="296" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A296" s="42" t="s">
         <v>929</v>
       </c>
@@ -18687,7 +18939,7 @@
       </c>
       <c r="K296" s="3"/>
     </row>
-    <row r="297" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>878</v>
       </c>
@@ -18717,7 +18969,7 @@
       </c>
       <c r="K297" s="3"/>
     </row>
-    <row r="298" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>879</v>
       </c>
@@ -18747,7 +18999,7 @@
       </c>
       <c r="K298" s="3"/>
     </row>
-    <row r="299" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>882</v>
       </c>
@@ -18777,7 +19029,7 @@
       </c>
       <c r="K299" s="3"/>
     </row>
-    <row r="300" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>901</v>
       </c>
@@ -18812,7 +19064,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="301" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>904</v>
       </c>
@@ -18847,7 +19099,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="302" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>909</v>
       </c>
@@ -18877,7 +19129,7 @@
       </c>
       <c r="K302" s="3"/>
     </row>
-    <row r="303" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>911</v>
       </c>
@@ -18907,7 +19159,7 @@
       </c>
       <c r="K303" s="3"/>
     </row>
-    <row r="304" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>913</v>
       </c>
@@ -18934,7 +19186,7 @@
       </c>
       <c r="K304" s="3"/>
     </row>
-    <row r="305" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>915</v>
       </c>
@@ -18964,7 +19216,7 @@
       </c>
       <c r="K305" s="3"/>
     </row>
-    <row r="306" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>918</v>
       </c>
@@ -18994,7 +19246,7 @@
       </c>
       <c r="K306" s="3"/>
     </row>
-    <row r="307" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>919</v>
       </c>
@@ -19020,6 +19272,728 @@
         <v>132</v>
       </c>
       <c r="K307" s="3"/>
+    </row>
+    <row r="308" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A308" t="s">
+        <v>939</v>
+      </c>
+      <c r="B308" s="3" t="s">
+        <v>940</v>
+      </c>
+      <c r="C308" t="s">
+        <v>941</v>
+      </c>
+      <c r="D308" s="3" t="s">
+        <v>942</v>
+      </c>
+      <c r="E308" t="s">
+        <v>32</v>
+      </c>
+      <c r="F308" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G308" t="s">
+        <v>943</v>
+      </c>
+      <c r="H308" t="s">
+        <v>132</v>
+      </c>
+      <c r="I308" t="s">
+        <v>944</v>
+      </c>
+      <c r="K308" s="3"/>
+    </row>
+    <row r="309" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A309" t="s">
+        <v>945</v>
+      </c>
+      <c r="F309" s="3" t="s">
+        <v>661</v>
+      </c>
+      <c r="G309" t="s">
+        <v>948</v>
+      </c>
+      <c r="H309" t="s">
+        <v>132</v>
+      </c>
+      <c r="J309" t="s">
+        <v>642</v>
+      </c>
+      <c r="K309" s="3"/>
+    </row>
+    <row r="310" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A310" t="s">
+        <v>946</v>
+      </c>
+      <c r="B310" t="s">
+        <v>950</v>
+      </c>
+      <c r="C310" t="s">
+        <v>951</v>
+      </c>
+      <c r="D310" s="3" t="s">
+        <v>949</v>
+      </c>
+      <c r="E310" t="s">
+        <v>691</v>
+      </c>
+      <c r="F310" s="3" t="s">
+        <v>661</v>
+      </c>
+      <c r="G310" t="s">
+        <v>948</v>
+      </c>
+      <c r="H310" t="s">
+        <v>132</v>
+      </c>
+      <c r="J310" t="s">
+        <v>947</v>
+      </c>
+      <c r="K310" s="3"/>
+    </row>
+    <row r="311" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A311" t="s">
+        <v>952</v>
+      </c>
+      <c r="B311" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C311" t="s">
+        <v>220</v>
+      </c>
+      <c r="D311" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="E311" t="s">
+        <v>405</v>
+      </c>
+      <c r="F311" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="G311" t="s">
+        <v>34</v>
+      </c>
+      <c r="H311" t="s">
+        <v>132</v>
+      </c>
+      <c r="I311" t="s">
+        <v>953</v>
+      </c>
+      <c r="K311" s="3"/>
+    </row>
+    <row r="312" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A312" t="s">
+        <v>954</v>
+      </c>
+      <c r="B312" s="3" t="s">
+        <v>955</v>
+      </c>
+      <c r="C312" t="s">
+        <v>220</v>
+      </c>
+      <c r="D312" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="E312" t="s">
+        <v>405</v>
+      </c>
+      <c r="F312" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="G312" t="s">
+        <v>379</v>
+      </c>
+      <c r="H312" t="s">
+        <v>132</v>
+      </c>
+      <c r="J312" t="s">
+        <v>956</v>
+      </c>
+      <c r="K312" s="3"/>
+    </row>
+    <row r="313" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A313" t="s">
+        <v>957</v>
+      </c>
+      <c r="B313" s="3" t="s">
+        <v>981</v>
+      </c>
+      <c r="D313" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="F313" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G313" t="s">
+        <v>958</v>
+      </c>
+      <c r="H313" t="s">
+        <v>132</v>
+      </c>
+      <c r="I313" t="s">
+        <v>959</v>
+      </c>
+      <c r="K313" s="3" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="314" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A314" t="s">
+        <v>961</v>
+      </c>
+      <c r="B314" s="3" t="s">
+        <v>975</v>
+      </c>
+      <c r="C314" t="s">
+        <v>192</v>
+      </c>
+      <c r="D314" s="3" t="s">
+        <v>981</v>
+      </c>
+      <c r="E314" t="s">
+        <v>241</v>
+      </c>
+      <c r="F314" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="G314" s="50" t="s">
+        <v>849</v>
+      </c>
+      <c r="H314" t="s">
+        <v>132</v>
+      </c>
+      <c r="J314" t="s">
+        <v>966</v>
+      </c>
+      <c r="K314" s="49" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="315" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A315" t="s">
+        <v>962</v>
+      </c>
+      <c r="F315" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="G315" s="50" t="s">
+        <v>849</v>
+      </c>
+      <c r="H315" t="s">
+        <v>132</v>
+      </c>
+      <c r="J315" t="s">
+        <v>966</v>
+      </c>
+      <c r="K315" s="49" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="316" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A316" t="s">
+        <v>963</v>
+      </c>
+      <c r="B316" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="C316" t="s">
+        <v>39</v>
+      </c>
+      <c r="D316" s="3" t="s">
+        <v>980</v>
+      </c>
+      <c r="E316" t="s">
+        <v>400</v>
+      </c>
+      <c r="F316" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="G316" s="50" t="s">
+        <v>242</v>
+      </c>
+      <c r="H316" t="s">
+        <v>132</v>
+      </c>
+      <c r="J316" t="s">
+        <v>966</v>
+      </c>
+      <c r="K316" s="49" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="317" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A317" t="s">
+        <v>964</v>
+      </c>
+      <c r="B317" s="3" t="s">
+        <v>976</v>
+      </c>
+      <c r="C317" t="s">
+        <v>39</v>
+      </c>
+      <c r="D317" s="3" t="s">
+        <v>975</v>
+      </c>
+      <c r="E317" t="s">
+        <v>977</v>
+      </c>
+      <c r="F317" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="G317" s="50" t="s">
+        <v>965</v>
+      </c>
+      <c r="H317" t="s">
+        <v>132</v>
+      </c>
+      <c r="J317" t="s">
+        <v>967</v>
+      </c>
+      <c r="K317" s="49"/>
+    </row>
+    <row r="318" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A318" t="s">
+        <v>968</v>
+      </c>
+      <c r="B318" s="3" t="s">
+        <v>971</v>
+      </c>
+      <c r="C318" t="s">
+        <v>972</v>
+      </c>
+      <c r="D318" s="3" t="s">
+        <v>975</v>
+      </c>
+      <c r="E318" t="s">
+        <v>978</v>
+      </c>
+      <c r="F318" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="G318" s="50" t="s">
+        <v>970</v>
+      </c>
+      <c r="H318" t="s">
+        <v>132</v>
+      </c>
+      <c r="I318" t="s">
+        <v>969</v>
+      </c>
+      <c r="J318" t="s">
+        <v>967</v>
+      </c>
+      <c r="K318" s="49"/>
+    </row>
+    <row r="319" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A319" t="s">
+        <v>973</v>
+      </c>
+      <c r="B319" s="3" t="s">
+        <v>974</v>
+      </c>
+      <c r="C319" t="s">
+        <v>39</v>
+      </c>
+      <c r="D319" s="12" t="s">
+        <v>975</v>
+      </c>
+      <c r="E319" t="s">
+        <v>974</v>
+      </c>
+      <c r="F319" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="G319" s="50" t="s">
+        <v>836</v>
+      </c>
+      <c r="H319" t="s">
+        <v>132</v>
+      </c>
+      <c r="K319" s="49"/>
+    </row>
+    <row r="320" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A320" t="s">
+        <v>982</v>
+      </c>
+      <c r="B320" s="3" t="s">
+        <v>983</v>
+      </c>
+      <c r="C320" t="s">
+        <v>180</v>
+      </c>
+      <c r="D320" s="3" t="s">
+        <v>984</v>
+      </c>
+      <c r="E320" t="s">
+        <v>986</v>
+      </c>
+      <c r="F320" s="49" t="s">
+        <v>180</v>
+      </c>
+      <c r="G320" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="H320" t="s">
+        <v>84</v>
+      </c>
+      <c r="I320" t="s">
+        <v>985</v>
+      </c>
+      <c r="K320" s="49"/>
+    </row>
+    <row r="321" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A321" t="s">
+        <v>989</v>
+      </c>
+      <c r="B321" s="3" t="s">
+        <v>984</v>
+      </c>
+      <c r="C321" t="s">
+        <v>442</v>
+      </c>
+      <c r="D321" t="s">
+        <v>987</v>
+      </c>
+      <c r="E321" t="s">
+        <v>691</v>
+      </c>
+      <c r="F321" s="49" t="s">
+        <v>851</v>
+      </c>
+      <c r="G321" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="H321" t="s">
+        <v>84</v>
+      </c>
+      <c r="K321" s="49"/>
+    </row>
+    <row r="322" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A322" t="s">
+        <v>990</v>
+      </c>
+      <c r="B322" s="3" t="s">
+        <v>984</v>
+      </c>
+      <c r="C322" t="s">
+        <v>444</v>
+      </c>
+      <c r="D322" t="s">
+        <v>988</v>
+      </c>
+      <c r="E322" t="s">
+        <v>691</v>
+      </c>
+      <c r="F322" s="49" t="s">
+        <v>851</v>
+      </c>
+      <c r="G322" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="H322" t="s">
+        <v>84</v>
+      </c>
+      <c r="K322" s="49"/>
+    </row>
+    <row r="323" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A323" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B323" s="3" t="s">
+        <v>981</v>
+      </c>
+      <c r="C323" t="s">
+        <v>264</v>
+      </c>
+      <c r="D323" s="3" t="s">
+        <v>983</v>
+      </c>
+      <c r="E323" t="s">
+        <v>266</v>
+      </c>
+      <c r="F323" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="G323" s="50" t="s">
+        <v>943</v>
+      </c>
+      <c r="H323" t="s">
+        <v>132</v>
+      </c>
+      <c r="K323" s="49"/>
+    </row>
+    <row r="324" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A324" t="s">
+        <v>991</v>
+      </c>
+      <c r="B324" s="3" t="s">
+        <v>992</v>
+      </c>
+      <c r="C324" t="s">
+        <v>993</v>
+      </c>
+      <c r="D324" s="3" t="s">
+        <v>984</v>
+      </c>
+      <c r="E324" t="s">
+        <v>660</v>
+      </c>
+      <c r="F324" s="49" t="s">
+        <v>669</v>
+      </c>
+      <c r="G324" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="H324" t="s">
+        <v>84</v>
+      </c>
+      <c r="I324" t="s">
+        <v>643</v>
+      </c>
+      <c r="K324" s="49"/>
+    </row>
+    <row r="325" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A325" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B325" t="s">
+        <v>318</v>
+      </c>
+      <c r="C325" t="s">
+        <v>994</v>
+      </c>
+      <c r="D325" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E325" t="s">
+        <v>220</v>
+      </c>
+      <c r="F325" s="49" t="s">
+        <v>288</v>
+      </c>
+      <c r="G325" s="50" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H325" t="s">
+        <v>132</v>
+      </c>
+      <c r="K325" s="49"/>
+    </row>
+    <row r="326" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A326" t="s">
+        <v>995</v>
+      </c>
+      <c r="B326" s="3" t="s">
+        <v>983</v>
+      </c>
+      <c r="C326" t="s">
+        <v>996</v>
+      </c>
+      <c r="D326" s="3" t="s">
+        <v>984</v>
+      </c>
+      <c r="E326" t="s">
+        <v>1019</v>
+      </c>
+      <c r="F326" s="49" t="s">
+        <v>997</v>
+      </c>
+      <c r="G326" s="50" t="s">
+        <v>397</v>
+      </c>
+      <c r="H326" t="s">
+        <v>132</v>
+      </c>
+      <c r="J326" t="s">
+        <v>998</v>
+      </c>
+      <c r="K326" s="49"/>
+    </row>
+    <row r="327" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A327" s="55" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B327" s="56" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C327" s="55"/>
+      <c r="D327" s="56" t="s">
+        <v>984</v>
+      </c>
+      <c r="E327" s="55"/>
+      <c r="F327" s="57" t="s">
+        <v>669</v>
+      </c>
+      <c r="G327" s="58" t="s">
+        <v>1001</v>
+      </c>
+      <c r="H327" s="55" t="s">
+        <v>132</v>
+      </c>
+      <c r="I327" s="55"/>
+      <c r="J327" s="48" t="s">
+        <v>1002</v>
+      </c>
+      <c r="K327" s="54"/>
+      <c r="L327" s="48"/>
+      <c r="M327" s="51"/>
+      <c r="N327" s="52"/>
+      <c r="Q327" s="48"/>
+      <c r="R327" s="48"/>
+      <c r="S327" s="48"/>
+      <c r="T327" s="53"/>
+      <c r="U327" s="48"/>
+      <c r="V327" s="47"/>
+    </row>
+    <row r="328" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A328" s="55" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B328" s="56"/>
+      <c r="C328" s="55"/>
+      <c r="D328" s="56"/>
+      <c r="E328" s="55"/>
+      <c r="F328" s="57" t="s">
+        <v>39</v>
+      </c>
+      <c r="G328" s="58" t="s">
+        <v>388</v>
+      </c>
+      <c r="H328" s="55" t="s">
+        <v>132</v>
+      </c>
+      <c r="I328" s="55"/>
+      <c r="J328" s="55" t="s">
+        <v>967</v>
+      </c>
+      <c r="K328" s="57"/>
+      <c r="L328" s="55"/>
+    </row>
+    <row r="329" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A329" s="55" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B329" s="56"/>
+      <c r="C329" s="55"/>
+      <c r="D329" s="56"/>
+      <c r="E329" s="55"/>
+      <c r="F329" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="G329" s="58" t="s">
+        <v>1006</v>
+      </c>
+      <c r="H329" s="55" t="s">
+        <v>132</v>
+      </c>
+      <c r="I329" s="55"/>
+      <c r="J329" s="55"/>
+      <c r="K329" s="57"/>
+      <c r="L329" s="55"/>
+    </row>
+    <row r="330" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A330" s="55" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B330" s="56" t="s">
+        <v>976</v>
+      </c>
+      <c r="C330" s="55" t="s">
+        <v>1008</v>
+      </c>
+      <c r="D330" s="56" t="s">
+        <v>984</v>
+      </c>
+      <c r="E330" t="s">
+        <v>1019</v>
+      </c>
+      <c r="F330" s="49" t="s">
+        <v>1010</v>
+      </c>
+      <c r="G330" s="58" t="s">
+        <v>368</v>
+      </c>
+      <c r="H330" s="55" t="s">
+        <v>132</v>
+      </c>
+      <c r="I330" s="55" t="s">
+        <v>1011</v>
+      </c>
+      <c r="J330" s="55"/>
+      <c r="K330" s="57"/>
+      <c r="L330" s="55"/>
+    </row>
+    <row r="331" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A331" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B331" s="3" t="s">
+        <v>971</v>
+      </c>
+      <c r="C331" t="s">
+        <v>1013</v>
+      </c>
+      <c r="D331" s="3" t="s">
+        <v>984</v>
+      </c>
+      <c r="E331" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F331" s="57" t="s">
+        <v>1010</v>
+      </c>
+      <c r="G331" s="50" t="s">
+        <v>397</v>
+      </c>
+      <c r="H331" t="s">
+        <v>132</v>
+      </c>
+      <c r="K331" s="49"/>
+    </row>
+    <row r="332" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A332" t="s">
+        <v>999</v>
+      </c>
+      <c r="B332" s="3" t="s">
+        <v>981</v>
+      </c>
+      <c r="C332" t="s">
+        <v>264</v>
+      </c>
+      <c r="D332" s="3" t="s">
+        <v>957</v>
+      </c>
+      <c r="F332" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="G332" s="50" t="s">
+        <v>1017</v>
+      </c>
+      <c r="H332" t="s">
+        <v>132</v>
+      </c>
+      <c r="K332" s="49"/>
+    </row>
+    <row r="333" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A333" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B333" s="3" t="s">
+        <v>957</v>
+      </c>
+      <c r="D333" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="F333" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="G333" s="50" t="s">
+        <v>943</v>
+      </c>
+      <c r="H333" t="s">
+        <v>132</v>
+      </c>
+      <c r="K333" s="49"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
updated FH details - improved readability
</commit_message>
<xml_diff>
--- a/data/uac_cables.xlsx
+++ b/data/uac_cables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/donert/Documents/UACTech/SystemDocumentation/github/uactechdoc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F90F0C-A819-8D46-801C-19D7F6FC3D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD8584C-3E2F-B949-B41C-3AE415B95062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-64360" yWindow="-30380" windowWidth="61940" windowHeight="34380" xr2:uid="{288904EE-D384-EA4C-9B98-052B972FB267}"/>
+    <workbookView xWindow="20" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{288904EE-D384-EA4C-9B98-052B972FB267}"/>
   </bookViews>
   <sheets>
     <sheet name="Cables" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <calcPr calcId="191029"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId3"/>
-    <pivotCache cacheId="8" r:id="rId4"/>
+    <pivotCache cacheId="9" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2542" uniqueCount="1030">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2543" uniqueCount="1032">
   <si>
     <t>Tag</t>
   </si>
@@ -3043,9 +3043,6 @@
     <t>tape_CD_In</t>
   </si>
   <si>
-    <t>2401-3012</t>
-  </si>
-  <si>
     <t>a334_1</t>
   </si>
   <si>
@@ -3079,9 +3076,6 @@
     <t>2402-2300</t>
   </si>
   <si>
-    <t>hdmi_in_2</t>
-  </si>
-  <si>
     <t>Guest Audio+video</t>
   </si>
   <si>
@@ -3131,6 +3125,18 @@
   </si>
   <si>
     <t>A334_2</t>
+  </si>
+  <si>
+    <t>ZVPU-0001</t>
+  </si>
+  <si>
+    <t>hdmi_in1</t>
+  </si>
+  <si>
+    <t>hdmi_in3</t>
+  </si>
+  <si>
+    <t>hdmi_in2</t>
   </si>
 </sst>
 </file>
@@ -3602,7 +3608,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="45221.662918634262" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="293" xr:uid="{966EC718-ADB8-7746-9366-54097C9D57FA}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:L334" sheet="Cables"/>
+    <worksheetSource ref="A1:L335" sheet="Cables"/>
   </cacheSource>
   <cacheFields count="12">
     <cacheField name="Tag" numFmtId="0">
@@ -9876,7 +9882,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{10F736CA-5D69-4D44-A803-D4241D124F38}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{10F736CA-5D69-4D44-A803-D4241D124F38}" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B42" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField dataField="1" showAll="0"/>
@@ -10140,8 +10146,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD7E3698-8860-904B-8BDB-00EF1039C49C}" name="Table1" displayName="Table1" ref="A1:L334" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="5">
-  <autoFilter ref="A1:L334" xr:uid="{BD7E3698-8860-904B-8BDB-00EF1039C49C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD7E3698-8860-904B-8BDB-00EF1039C49C}" name="Table1" displayName="Table1" ref="A1:L335" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="5">
+  <autoFilter ref="A1:L335" xr:uid="{BD7E3698-8860-904B-8BDB-00EF1039C49C}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="2309-3004"/>
+        <filter val="2401-3004"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{4D442337-BE86-B24A-84A4-338FB80A6A49}" name="Tag"/>
     <tableColumn id="2" xr3:uid="{74A36D7B-C989-3B4B-B1E5-AB1FA4C2DD45}" name="SrcTag" dataDxfId="4"/>
@@ -10457,13 +10470,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B91ADC-4569-1C4E-B002-1ED2E647C959}">
-  <dimension ref="A1:V334"/>
+  <dimension ref="A1:V335"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B314" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B230" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E327" sqref="E327"/>
+      <selection pane="bottomRight" activeCell="C333" sqref="C333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10519,7 +10532,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>25</v>
       </c>
@@ -10562,7 +10575,7 @@
         <v>cdmua001:Key -&gt; zviue004:sw1 [label='2307-1800']</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>4</v>
       </c>
@@ -10597,7 +10610,7 @@
         <v>cdmua001:Fill -&gt; zviue004:sw2 [label='2307-1801']</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>5</v>
       </c>
@@ -10632,7 +10645,7 @@
         <v>cdmua001:ProjA -&gt; zviue004:sw4 [label='2307-1802']</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>6</v>
       </c>
@@ -10667,7 +10680,7 @@
         <v>cdmua001:ProjB -&gt; zviue004:sw6 [label='2307-1803']</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>7</v>
       </c>
@@ -10702,7 +10715,7 @@
         <v>cdmua001:ProjC -&gt; zviue004:sw8 [label='2307-1804']</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>8</v>
       </c>
@@ -10737,7 +10750,7 @@
         <v>cdmua001:RearDeckLink -&gt; zviue004:sw3 [label='2307-1805']</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>9</v>
       </c>
@@ -10770,7 +10783,7 @@
         <v>zvkua003:PGM -&gt; zviua005:sdi [label='2307-1806']</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
         <v>10</v>
       </c>
@@ -10805,7 +10818,7 @@
         <v>cdmua001:in1 -&gt; zviue004:sw5 [label='2307-1807']</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>11</v>
       </c>
@@ -10840,7 +10853,7 @@
         <v>zvkua003:aux -&gt; zviud001:sdi in [label='2307-1808']</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
         <v>12</v>
       </c>
@@ -10883,7 +10896,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>13</v>
       </c>
@@ -10928,7 +10941,7 @@
         <v>zviue004:sdi1 -&gt; 23081204:sdi in [label='2307-1810']</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>14</v>
       </c>
@@ -10965,7 +10978,7 @@
         <v>zviue004:sdi2 -&gt; 23081205:sdi in [label='2307-1811']</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>15</v>
       </c>
@@ -11000,7 +11013,7 @@
         <v>zviue004:sdi4 -&gt; zviug003:sdi in [label='2307-1812']</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
         <v>16</v>
       </c>
@@ -11035,7 +11048,7 @@
         <v>zviue004:sdi6 -&gt; zviug004:sdi in [label='2307-1813']</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>17</v>
       </c>
@@ -11070,7 +11083,7 @@
         <v>zviue004:sdi8 -&gt; zviug005:sdi in [label='2307-1814']</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
         <v>18</v>
       </c>
@@ -11105,7 +11118,7 @@
         <v>zviue004:sdi3 -&gt; zviue001:sdi in [label='2307-1815']</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>19</v>
       </c>
@@ -11126,7 +11139,7 @@
         <v>: -&gt; : [label='2307-1816']</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
         <v>20</v>
       </c>
@@ -11147,7 +11160,7 @@
         <v>: -&gt; : [label='2307-1817']</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>21</v>
       </c>
@@ -11168,7 +11181,7 @@
         <v>: -&gt; : [label='2307-1818']</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
         <v>22</v>
       </c>
@@ -11195,7 +11208,7 @@
         <v>not used: -&gt; : [label='2307-1819']</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>23</v>
       </c>
@@ -11224,7 +11237,7 @@
         <v>unused: -&gt; : [label='2307-1820']</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
         <v>24</v>
       </c>
@@ -11253,7 +11266,7 @@
         <v>unused: -&gt; : [label='2307-1821']</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>30</v>
       </c>
@@ -11282,7 +11295,7 @@
         <v>unused: -&gt; : [label='2307-1822']</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
         <v>52</v>
       </c>
@@ -11317,7 +11330,7 @@
         <v>zviua008:hdmi -&gt; zvkua003:in4 [label='2307-1828']</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>47</v>
       </c>
@@ -11350,7 +11363,7 @@
         <v>cdmua001:usbc -&gt; zviue005:usbc [label='2307-1824']</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="23" t="s">
         <v>49</v>
       </c>
@@ -11379,7 +11392,7 @@
         <v>unused: -&gt; : [label='2307-1825']</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
         <v>50</v>
       </c>
@@ -11408,7 +11421,7 @@
         <v>unused: -&gt; : [label='2307-1826']</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
         <v>64</v>
       </c>
@@ -11441,7 +11454,7 @@
         <v>zviua004:usb -&gt; cumug001:usb_3 [label='2307-2100']</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
         <v>65</v>
       </c>
@@ -11476,7 +11489,7 @@
         <v>cumug001:ndi -&gt; cumue001:obs [label='2307-2101']</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="s">
         <v>66</v>
       </c>
@@ -11509,7 +11522,7 @@
         <v>camera left: -&gt; cumue001:obs [label='2307-2102']</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>67</v>
       </c>
@@ -11542,7 +11555,7 @@
         <v>camera centre: -&gt; cumue001:obs [label='2307-2103']</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="15" t="s">
         <v>68</v>
       </c>
@@ -11575,7 +11588,7 @@
         <v>camera right: -&gt; cumue001:obs [label='2307-2104']</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
         <v>69</v>
       </c>
@@ -11608,7 +11621,7 @@
         <v>cdmua001:ndi -&gt; cumue001:obs [label='2307-2105']</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="15" t="s">
         <v>81</v>
       </c>
@@ -11641,7 +11654,7 @@
         <v>zvkua001:out_5_hdmi -&gt; zviuc001:hdmi in [label='2307-2300']</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
         <v>85</v>
       </c>
@@ -11678,7 +11691,7 @@
         <v>zviuc001:hdmi out -&gt; zvkua003:in1 [label='2307-2301']</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="15" t="s">
         <v>88</v>
       </c>
@@ -11713,7 +11726,7 @@
         <v>zvcua001:sdi -&gt; zvkua003:in5 [label='2307-2304']</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
         <v>87</v>
       </c>
@@ -11748,7 +11761,7 @@
         <v>zvcua002:sdi -&gt; zvkua003:in6 [label='2307-2303']</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="15" t="s">
         <v>86</v>
       </c>
@@ -11783,7 +11796,7 @@
         <v>zvcua003:sdi -&gt; zvkua003:in7 [label='2307-2302']</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
         <v>95</v>
       </c>
@@ -11820,7 +11833,7 @@
         <v>23072306:barrel -&gt; zvkua003:in8 [label='2307-2305']</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="15" t="s">
         <v>96</v>
       </c>
@@ -11855,7 +11868,7 @@
         <v>z150:sdi -&gt; 23072305:barrel [label='2307-2306']</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
         <v>97</v>
       </c>
@@ -11882,7 +11895,7 @@
         <v>: -&gt; : [label='2307-2307']</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="15" t="s">
         <v>101</v>
       </c>
@@ -11917,7 +11930,7 @@
         <v>zvkua004:sw -&gt; zvcua001:sw [label='2307-2308']</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
         <v>102</v>
       </c>
@@ -11960,7 +11973,7 @@
         <v>zvkua004:sw -&gt; zvcua002:sw [label='2307-2309']</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="15" t="s">
         <v>103</v>
       </c>
@@ -11995,7 +12008,7 @@
         <v>zvkua004:sw -&gt; zvcua003:sw [label='2307-2310']</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
         <v>106</v>
       </c>
@@ -12014,7 +12027,7 @@
         <v>: -&gt; : [label='2307-2311']</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="15" t="s">
         <v>109</v>
       </c>
@@ -12033,7 +12046,7 @@
         <v>: -&gt; : [label='2307-2312']</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
         <v>110</v>
       </c>
@@ -12052,7 +12065,7 @@
         <v>: -&gt; : [label='2307-2313']</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="15" t="s">
         <v>111</v>
       </c>
@@ -12085,7 +12098,7 @@
         <v>zvkua001:out_4_HDbT -&gt; zvvu0001:HDbT [label='2307-2314']</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
         <v>120</v>
       </c>
@@ -12120,7 +12133,7 @@
         <v>zvkua001:out_7_HDbT -&gt; zviua001:HDbT [label='2307-2315']</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="15" t="s">
         <v>121</v>
       </c>
@@ -12153,7 +12166,7 @@
         <v>zviua001:hdmi -&gt; zvvulobby tv :hdmi 1 [label='2307-2316']</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
         <v>122</v>
       </c>
@@ -12180,7 +12193,7 @@
         <v>: -&gt; : [label='2307-2317']</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="15" t="s">
         <v>126</v>
       </c>
@@ -12215,7 +12228,7 @@
         <v>zvkua001:out_8_HDbT -&gt; zviua002:HDbT [label='2307-2318']</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="11" t="s">
         <v>406</v>
       </c>
@@ -12246,7 +12259,7 @@
         <v>zviua002:hdmi -&gt; 23082900:input [label='2308-3001']</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="15" t="s">
         <v>129</v>
       </c>
@@ -12273,7 +12286,7 @@
         <v>: -&gt; : [label='2307-2320']</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
         <v>134</v>
       </c>
@@ -12306,7 +12319,7 @@
         <v>cdmua001:PP_Front_SW -&gt; hdmi_dongle: [label='2307-3000']</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="15" t="s">
         <v>136</v>
       </c>
@@ -12339,7 +12352,7 @@
         <v>zvrua001:OutB -&gt; zvrua002:SDI In [label='2307-3001']</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
         <v>138</v>
       </c>
@@ -12372,7 +12385,7 @@
         <v>zvrua001:OutA -&gt; zviua004:SDI In [label='2307-3002']</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="15" t="s">
         <v>141</v>
       </c>
@@ -12407,7 +12420,7 @@
         <v>zviua004:hdmi out -&gt; zvkua001:in7 [label='2307-3003']</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="11" t="s">
         <v>142</v>
       </c>
@@ -12426,7 +12439,7 @@
         <v>: -&gt; : [label='2307-3004']</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="15" t="s">
         <v>143</v>
       </c>
@@ -12463,7 +12476,7 @@
         <v>zvkua003:out5 -&gt; zvrua001:sdi in [label='2307-3005']</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="11" t="s">
         <v>144</v>
       </c>
@@ -12500,7 +12513,7 @@
         <v>zvkua003:out6 -&gt; zviud002:sdi in [label='2307-3006']</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="15" t="s">
         <v>147</v>
       </c>
@@ -12533,7 +12546,7 @@
         <v>zviud001:hdmi -&gt; zviua004:hdmi in [label='2307-3007']</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">
         <v>160</v>
       </c>
@@ -12568,7 +12581,7 @@
         <v>zviua005:hdmi -&gt; zvkua001:in6 [label='2308-0800']</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="15" t="s">
         <v>202</v>
       </c>
@@ -12600,7 +12613,7 @@
         <v>unused:  -&gt; : [label='2308-0004']</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="11" t="s">
         <v>203</v>
       </c>
@@ -12633,7 +12646,7 @@
         <v>frontguest: -&gt; 23080003:InputC [label='2308-0005']</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="15" t="s">
         <v>204</v>
       </c>
@@ -12668,7 +12681,7 @@
         <v>cdwua002:HdmiOut -&gt; 23080002:In2 [label='2308-0006']</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="11" t="s">
         <v>205</v>
       </c>
@@ -12701,7 +12714,7 @@
         <v>rearguest:hdmi_out -&gt; 23080002:In1 [label='2308-0007']</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="15" t="s">
         <v>206</v>
       </c>
@@ -12734,7 +12747,7 @@
         <v>cdwua002:vga -&gt; vmnu0029:vga [label='2308-0009']</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="11" t="s">
         <v>207</v>
       </c>
@@ -12767,7 +12780,7 @@
         <v>cdwua002:usb -&gt; 23080008:usb [label='2308-0010']</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="11" t="s">
         <v>183</v>
       </c>
@@ -12800,7 +12813,7 @@
         <v>zviug003:hdmi_out -&gt; zvkua001:in1 [label='2308-0915']</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="15" t="s">
         <v>184</v>
       </c>
@@ -12833,7 +12846,7 @@
         <v>zviug004:hdmi_out -&gt; zvkua001:in2 [label='2308-0916']</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="11" t="s">
         <v>185</v>
       </c>
@@ -12866,7 +12879,7 @@
         <v>zviug005:hdmi_out -&gt; zvkua001:in3 [label='2308-0917']</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="15" t="s">
         <v>186</v>
       </c>
@@ -12896,7 +12909,7 @@
       <c r="K74" s="17"/>
       <c r="L74" s="18"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="11" t="s">
         <v>193</v>
       </c>
@@ -12937,7 +12950,7 @@
         <v>zvkua001:out_1_HDbT -&gt; zvvua001:InputD [label='PROJ0001']</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="15" t="s">
         <v>194</v>
       </c>
@@ -12978,7 +12991,7 @@
         <v>zvkua001:out_2_HDbT -&gt; zvvua002:InputD [label='PROJ0002']</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="11" t="s">
         <v>195</v>
       </c>
@@ -13019,7 +13032,7 @@
         <v>zvkua001:out_3_HDbT -&gt; zvvua003:InputD [label='PROJ0003']</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="15" t="s">
         <v>200</v>
       </c>
@@ -13062,7 +13075,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="11" t="s">
         <v>213</v>
       </c>
@@ -13103,7 +13116,7 @@
         <v>cumue001:usba_2 -&gt; 23081110:usb_in [label='2308-1111']</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="15" t="s">
         <v>228</v>
       </c>
@@ -13136,7 +13149,7 @@
         <v>23081110:usb_1 -&gt; 23081104:usb [label='2308-1112']</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="11" t="s">
         <v>229</v>
       </c>
@@ -13169,7 +13182,7 @@
         <v>23081110:usb_2 -&gt; 23081105:usb [label='2308-1113']</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="15" t="s">
         <v>230</v>
       </c>
@@ -13206,7 +13219,7 @@
         <v>cumue001:usbc -&gt; 23081106:hdmi [label='2308-1114']</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="11" t="s">
         <v>231</v>
       </c>
@@ -13241,7 +13254,7 @@
         <v>cumue001:hdmi -&gt; 23081107:hdmi [label='2308-1115']</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="15" t="s">
         <v>232</v>
       </c>
@@ -13274,7 +13287,7 @@
         <v>23081110:usb  -&gt; 23081103:usb [label='2308-1116']</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="11" t="s">
         <v>233</v>
       </c>
@@ -13315,7 +13328,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="15" t="s">
         <v>234</v>
       </c>
@@ -13356,7 +13369,7 @@
         <v>23081100:port3 -&gt; zaiue002:ether [label='2308-1118']</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="11" t="s">
         <v>235</v>
       </c>
@@ -13397,7 +13410,7 @@
         <v>23081100:port4 -&gt; daw_guest:ether [label='2308-1119']</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="15" t="s">
         <v>236</v>
       </c>
@@ -13433,7 +13446,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="11" t="s">
         <v>237</v>
       </c>
@@ -13474,7 +13487,7 @@
         <v>zaiue002:Ch2 -&gt; 23081102:right [label='2308-1121']</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="15" t="s">
         <v>238</v>
       </c>
@@ -13517,7 +13530,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="11" t="s">
         <v>243</v>
       </c>
@@ -13560,7 +13573,7 @@
         <v>23081124:ch1 -&gt; zvkua003:ch1_audio [label='2308-1124L']</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="15" t="s">
         <v>247</v>
       </c>
@@ -13595,7 +13608,7 @@
         <v>23081124:ch2 -&gt; zvkua003:ch2_audio [label='2308-1124R']</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="11" t="s">
         <v>687</v>
       </c>
@@ -13613,7 +13626,7 @@
         <v>: -&gt; : [label='x93']</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="15" t="s">
         <v>688</v>
       </c>
@@ -13631,7 +13644,7 @@
         <v>: -&gt; : [label='x94']</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="11" t="s">
         <v>657</v>
       </c>
@@ -13664,7 +13677,7 @@
         <v>zakua001:aux_4 -&gt; 23080008:Mic_In [label='2309-2505']</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="11"/>
       <c r="B96" s="12" t="s">
         <v>72</v>
@@ -13703,7 +13716,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="15"/>
       <c r="B97" s="16" t="s">
         <v>72</v>
@@ -13742,7 +13755,7 @@
         <v>cumug001:usb_2 -&gt; zviug001:usb_in [label='']</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="11"/>
       <c r="B98" s="12" t="s">
         <v>72</v>
@@ -13783,7 +13796,7 @@
         <v>cumug001:usb_1 -&gt; 23081202:usb [label='']</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="15"/>
       <c r="B99" s="16" t="s">
         <v>256</v>
@@ -13824,7 +13837,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="11" t="s">
         <v>331</v>
       </c>
@@ -13867,7 +13880,7 @@
         <v>23081204:sdi_out -&gt; zviue003:sdi_in [label='2307-1201']</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="15" t="s">
         <v>332</v>
       </c>
@@ -13902,7 +13915,7 @@
         <v>23081205:sdi_out -&gt; zviua008:sdi_in [label='2307-1202']</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="11" t="s">
         <v>51</v>
       </c>
@@ -13937,7 +13950,7 @@
         <v>zviue003:hdmi_out -&gt; zvkua003:in2 [label='2307-1827']</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="15"/>
       <c r="B103" s="16" t="s">
         <v>278</v>
@@ -13968,7 +13981,7 @@
         <v>cdwu0009:vga -&gt; mon:vga [label='']</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="11" t="s">
         <v>280</v>
       </c>
@@ -14003,7 +14016,7 @@
         <v>prwall3:label3 -&gt; 23081100:port1 [label='2308-2001']</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="15" t="s">
         <v>291</v>
       </c>
@@ -14036,9 +14049,9 @@
         <v>23081102:Right -&gt; 23082003:Right [label='2308-2002']</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="11" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="B106" s="12" t="s">
         <v>298</v>
@@ -14069,9 +14082,9 @@
         <v>patchpanel:a -&gt; prwall3:b1 [label='a106_1']</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="15" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="B107" s="16" t="s">
         <v>299</v>
@@ -14102,9 +14115,9 @@
         <v>modem:c -&gt; router:d [label='a107_1']</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="11" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="B108" s="12" t="s">
         <v>300</v>
@@ -14135,9 +14148,9 @@
         <v>router:e -&gt; nscua001:f [label='a108_1']</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="15" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="B109" s="16" t="s">
         <v>301</v>
@@ -14168,9 +14181,9 @@
         <v>nscua001:h -&gt; patchpanel:i [label='a109_1']</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="11" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="B110" s="12" t="s">
         <v>301</v>
@@ -14197,9 +14210,9 @@
         <v>nscua001:a  -&gt; nscua002:f [label='a110_1']</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="15" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="B111" s="16" t="s">
         <v>301</v>
@@ -14226,9 +14239,9 @@
         <v>nscua001:b  -&gt; nscua005:g [label='a111_1']</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="11" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="B112" s="12" t="s">
         <v>319</v>
@@ -14253,9 +14266,9 @@
         <v>nscua005:c  -&gt; nscua003:h  [label='a112_1']</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="15" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="B113" s="16" t="s">
         <v>321</v>
@@ -14284,9 +14297,9 @@
         <v>nscua003:d  -&gt; nscua004:i [label='a113_1']</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="11" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="B114" s="12" t="s">
         <v>322</v>
@@ -14311,7 +14324,7 @@
         <v>nscua004:e  -&gt; 23081124:ether [label='a114_1']</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="15" t="s">
         <v>365</v>
       </c>
@@ -14344,7 +14357,7 @@
         <v>cumug001:usb -&gt; zviuc002:usbc [label='future1']</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="15" t="s">
         <v>368</v>
       </c>
@@ -14377,7 +14390,7 @@
         <v>cdwu0009:hdmi_out -&gt; zvkua001:in5 [label='2308-2500']</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="11" t="s">
         <v>371</v>
       </c>
@@ -14412,7 +14425,7 @@
         <v>zviue001:hdmi_out -&gt; zvkua001:in4 [label='2308-2501']</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="15" t="s">
         <v>372</v>
       </c>
@@ -14441,7 +14454,7 @@
         <v>not used: -&gt; : [label='2308-2502']</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="11" t="s">
         <v>375</v>
       </c>
@@ -14470,7 +14483,7 @@
         <v>not used: -&gt; : [label='2308-2503']</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="15" t="s">
         <v>382</v>
       </c>
@@ -14497,7 +14510,7 @@
         <v>not used: -&gt; : [label='2308-2504']</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="11" t="s">
         <v>383</v>
       </c>
@@ -14532,7 +14545,7 @@
         <v>ncsua004:portxx -&gt; cdmua001:ether [label='2308-2600']</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="15" t="s">
         <v>384</v>
       </c>
@@ -14557,7 +14570,7 @@
         <v>not used: -&gt; : [label='2308-2700']</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="11" t="s">
         <v>385</v>
       </c>
@@ -14582,7 +14595,7 @@
         <v>not used: -&gt; : [label='2308-2701']</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="15" t="s">
         <v>386</v>
       </c>
@@ -14607,7 +14620,7 @@
         <v>unused: -&gt; : [label='2308-2702']</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="11" t="s">
         <v>394</v>
       </c>
@@ -14644,7 +14657,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="15" t="s">
         <v>22</v>
       </c>
@@ -14687,7 +14700,7 @@
         <v>23082900:output2 -&gt; zvvu0003:hdmi1 [label='2307-1819']</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="11" t="s">
         <v>405</v>
       </c>
@@ -14728,7 +14741,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="15" t="s">
         <v>402</v>
       </c>
@@ -14769,7 +14782,7 @@
         <v>zvkua001:out6 -&gt; unknown:unk [label='future135']</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="11"/>
       <c r="B129" s="12"/>
       <c r="C129" s="13"/>
@@ -14788,7 +14801,7 @@
         <v>: -&gt; :unk [label='']</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="15" t="s">
         <v>410</v>
       </c>
@@ -14823,7 +14836,7 @@
         <v>zamua001:ch1 -&gt; zaiub001:s2_in01 [label='2309-1001']</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="11" t="s">
         <v>535</v>
       </c>
@@ -14858,7 +14871,7 @@
         <v>zamua001:ch2 -&gt; zaiub001:s2_in02 [label='2309-1002']</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="15" t="s">
         <v>536</v>
       </c>
@@ -14893,7 +14906,7 @@
         <v>zamua001:ch3 -&gt; zaiub001:s2_in03 [label='2309-1003']</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="11" t="s">
         <v>537</v>
       </c>
@@ -14928,7 +14941,7 @@
         <v>zamua001:ch4 -&gt; zaiub001:s2_in04 [label='2309-1004']</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="15" t="s">
         <v>538</v>
       </c>
@@ -14963,7 +14976,7 @@
         <v>zamub001:ch1 -&gt; zaiub001:s2_in05 [label='2309-1005']</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="11" t="s">
         <v>539</v>
       </c>
@@ -14998,7 +15011,7 @@
         <v>zamub001:ch2 -&gt; zaiub001:s2_in06 [label='2309-1006']</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="15" t="s">
         <v>540</v>
       </c>
@@ -15033,7 +15046,7 @@
         <v>zamub001:ch3 -&gt; zaiub001:s2_in07 [label='2309-1007']</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" s="11" t="s">
         <v>541</v>
       </c>
@@ -15068,7 +15081,7 @@
         <v>zamub001:ch4 -&gt; zaiub001:s2_in08 [label='2309-1008']</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="15" t="s">
         <v>542</v>
       </c>
@@ -15103,7 +15116,7 @@
         <v>zamub002:ch1 -&gt; zaiub001:s2_in09 [label='2309-1009']</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="11" t="s">
         <v>543</v>
       </c>
@@ -15138,7 +15151,7 @@
         <v>zamub002:ch2 -&gt; zaiub001:s2_in10 [label='2309-1010']</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="15" t="s">
         <v>544</v>
       </c>
@@ -15173,7 +15186,7 @@
         <v>zamub002:ch3 -&gt; zaiub001:s2_in11 [label='2309-1011']</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="11" t="s">
         <v>545</v>
       </c>
@@ -15208,7 +15221,7 @@
         <v>zamub002:ch4 -&gt; zaiub001:s2_in12 [label='2309-1012']</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="15" t="s">
         <v>546</v>
       </c>
@@ -15243,7 +15256,7 @@
         <v>zamub003:ch4 -&gt; zaiub001:s2___ [label='2309-1013']</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="11" t="s">
         <v>547</v>
       </c>
@@ -15278,7 +15291,7 @@
         <v>zamub002:ch3 -&gt; zaiub002:s2_in01 [label='2309-1014']</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="9" t="s">
         <v>548</v>
       </c>
@@ -15313,7 +15326,7 @@
         <v>zamub002:ch4 -&gt; zaiub002:s2_in02 [label='2309-1015']</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>549</v>
       </c>
@@ -15346,7 +15359,7 @@
         <v>zamub003:ch1 -&gt; zaiub002:s2_in03 [label='2309-1016']</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>550</v>
       </c>
@@ -15379,7 +15392,7 @@
         <v>zamub003:ch2 -&gt; zaiub002:s2_in04 [label='2309-1017']</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>551</v>
       </c>
@@ -15412,7 +15425,7 @@
         <v>zamub003:ch3 -&gt; zaiub002:s2_in05 [label='2309-1018']</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>552</v>
       </c>
@@ -15441,7 +15454,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>553</v>
       </c>
@@ -15467,7 +15480,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>554</v>
       </c>
@@ -15493,7 +15506,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" s="8" t="s">
         <v>555</v>
       </c>
@@ -15519,7 +15532,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>556</v>
       </c>
@@ -15545,7 +15558,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>557</v>
       </c>
@@ -15571,7 +15584,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>558</v>
       </c>
@@ -15597,7 +15610,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>559</v>
       </c>
@@ -15623,7 +15636,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>560</v>
       </c>
@@ -15649,7 +15662,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>561</v>
       </c>
@@ -15675,7 +15688,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>562</v>
       </c>
@@ -15701,7 +15714,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>563</v>
       </c>
@@ -15727,7 +15740,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>564</v>
       </c>
@@ -15753,7 +15766,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>565</v>
       </c>
@@ -15779,7 +15792,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>566</v>
       </c>
@@ -15805,7 +15818,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>567</v>
       </c>
@@ -15831,7 +15844,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>568</v>
       </c>
@@ -15857,7 +15870,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>569</v>
       </c>
@@ -15883,7 +15896,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>570</v>
       </c>
@@ -15909,7 +15922,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>571</v>
       </c>
@@ -15935,7 +15948,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>572</v>
       </c>
@@ -15961,7 +15974,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>573</v>
       </c>
@@ -15987,7 +16000,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>574</v>
       </c>
@@ -16013,7 +16026,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>575</v>
       </c>
@@ -16033,7 +16046,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>576</v>
       </c>
@@ -16053,7 +16066,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>577</v>
       </c>
@@ -16073,7 +16086,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>578</v>
       </c>
@@ -16093,7 +16106,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>579</v>
       </c>
@@ -16113,7 +16126,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>580</v>
       </c>
@@ -16133,7 +16146,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>581</v>
       </c>
@@ -16153,7 +16166,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>582</v>
       </c>
@@ -16173,7 +16186,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>583</v>
       </c>
@@ -16193,7 +16206,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>584</v>
       </c>
@@ -16213,7 +16226,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>585</v>
       </c>
@@ -16233,7 +16246,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>586</v>
       </c>
@@ -16253,7 +16266,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>587</v>
       </c>
@@ -16273,7 +16286,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>588</v>
       </c>
@@ -16293,7 +16306,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>589</v>
       </c>
@@ -16313,7 +16326,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>590</v>
       </c>
@@ -16333,7 +16346,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>591</v>
       </c>
@@ -16353,7 +16366,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>592</v>
       </c>
@@ -16373,7 +16386,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>593</v>
       </c>
@@ -16393,7 +16406,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>594</v>
       </c>
@@ -16413,7 +16426,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>595</v>
       </c>
@@ -16433,7 +16446,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>596</v>
       </c>
@@ -16453,7 +16466,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>597</v>
       </c>
@@ -16473,7 +16486,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>598</v>
       </c>
@@ -16493,7 +16506,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>599</v>
       </c>
@@ -16513,7 +16526,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>600</v>
       </c>
@@ -16533,7 +16546,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>601</v>
       </c>
@@ -16553,7 +16566,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>602</v>
       </c>
@@ -16573,7 +16586,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>603</v>
       </c>
@@ -16593,7 +16606,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>604</v>
       </c>
@@ -16613,7 +16626,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>605</v>
       </c>
@@ -16633,7 +16646,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>606</v>
       </c>
@@ -16653,7 +16666,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>607</v>
       </c>
@@ -16682,7 +16695,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>608</v>
       </c>
@@ -16711,7 +16724,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>609</v>
       </c>
@@ -16740,7 +16753,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>610</v>
       </c>
@@ -16769,7 +16782,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>617</v>
       </c>
@@ -16801,7 +16814,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>618</v>
       </c>
@@ -16828,7 +16841,7 @@
       </c>
       <c r="K208" s="3"/>
     </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>622</v>
       </c>
@@ -16857,7 +16870,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>630</v>
       </c>
@@ -16887,7 +16900,7 @@
       </c>
       <c r="K210" s="3"/>
     </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>631</v>
       </c>
@@ -16917,7 +16930,7 @@
       </c>
       <c r="K211" s="3"/>
     </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B212" s="3" t="s">
         <v>634</v>
       </c>
@@ -16947,7 +16960,7 @@
       </c>
       <c r="K212" s="3"/>
     </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B213" s="33" t="s">
         <v>636</v>
       </c>
@@ -16974,11 +16987,11 @@
       </c>
       <c r="K213" s="3"/>
     </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="F214" s="3"/>
       <c r="K214" s="3"/>
     </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>808</v>
       </c>
@@ -17001,7 +17014,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>648</v>
       </c>
@@ -17031,7 +17044,7 @@
       </c>
       <c r="K216" s="3"/>
     </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>654</v>
       </c>
@@ -17061,7 +17074,7 @@
       </c>
       <c r="K217" s="3"/>
     </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>657</v>
       </c>
@@ -17091,7 +17104,7 @@
       </c>
       <c r="K218" s="3"/>
     </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>661</v>
       </c>
@@ -17121,7 +17134,7 @@
       </c>
       <c r="K219" s="3"/>
     </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>662</v>
       </c>
@@ -17151,7 +17164,7 @@
       </c>
       <c r="K220" s="3"/>
     </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A221" s="44" t="s">
         <v>669</v>
       </c>
@@ -17181,7 +17194,7 @@
       </c>
       <c r="K221" s="3"/>
     </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>670</v>
       </c>
@@ -17211,7 +17224,7 @@
       </c>
       <c r="K222" s="3"/>
     </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>675</v>
       </c>
@@ -17238,7 +17251,7 @@
       </c>
       <c r="K223" s="3"/>
     </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>676</v>
       </c>
@@ -17265,7 +17278,7 @@
       </c>
       <c r="K224" s="3"/>
     </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>677</v>
       </c>
@@ -17292,7 +17305,7 @@
       </c>
       <c r="K225" s="3"/>
     </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>887</v>
       </c>
@@ -17319,7 +17332,7 @@
       </c>
       <c r="K226" s="3"/>
     </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>888</v>
       </c>
@@ -17346,7 +17359,7 @@
       </c>
       <c r="K227" s="3"/>
     </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>693</v>
       </c>
@@ -17367,7 +17380,7 @@
       </c>
       <c r="K228" s="3"/>
     </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>772</v>
       </c>
@@ -17409,7 +17422,7 @@
       </c>
       <c r="K230" s="3"/>
     </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>708</v>
       </c>
@@ -17430,7 +17443,7 @@
       </c>
       <c r="K231" s="3"/>
     </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>709</v>
       </c>
@@ -17451,7 +17464,7 @@
       </c>
       <c r="K232" s="3"/>
     </row>
-    <row r="233" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>710</v>
       </c>
@@ -17472,7 +17485,7 @@
       </c>
       <c r="K233" s="3"/>
     </row>
-    <row r="234" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>773</v>
       </c>
@@ -17496,7 +17509,7 @@
       </c>
       <c r="K234" s="3"/>
     </row>
-    <row r="235" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>790</v>
       </c>
@@ -17520,7 +17533,7 @@
       </c>
       <c r="K235" s="3"/>
     </row>
-    <row r="236" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A236" s="3" t="s">
         <v>792</v>
       </c>
@@ -17550,7 +17563,7 @@
       </c>
       <c r="K236" s="3"/>
     </row>
-    <row r="237" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>787</v>
       </c>
@@ -17577,7 +17590,7 @@
       </c>
       <c r="K237" s="3"/>
     </row>
-    <row r="238" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>774</v>
       </c>
@@ -17601,7 +17614,7 @@
       </c>
       <c r="K238" s="3"/>
     </row>
-    <row r="239" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>775</v>
       </c>
@@ -17631,7 +17644,7 @@
       </c>
       <c r="K239" s="3"/>
     </row>
-    <row r="240" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>777</v>
       </c>
@@ -17658,7 +17671,7 @@
       </c>
       <c r="K240" s="3"/>
     </row>
-    <row r="241" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>713</v>
       </c>
@@ -17679,7 +17692,7 @@
       </c>
       <c r="K241" s="3"/>
     </row>
-    <row r="242" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>714</v>
       </c>
@@ -17698,7 +17711,7 @@
       <c r="F242" s="3"/>
       <c r="K242" s="3"/>
     </row>
-    <row r="243" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>715</v>
       </c>
@@ -17719,7 +17732,7 @@
       </c>
       <c r="K243" s="3"/>
     </row>
-    <row r="244" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>800</v>
       </c>
@@ -17740,7 +17753,7 @@
       </c>
       <c r="K244" s="3"/>
     </row>
-    <row r="245" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>740</v>
       </c>
@@ -17759,7 +17772,7 @@
       <c r="F245" s="3"/>
       <c r="K245" s="3"/>
     </row>
-    <row r="246" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>746</v>
       </c>
@@ -17786,7 +17799,7 @@
       </c>
       <c r="K246" s="3"/>
     </row>
-    <row r="247" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>739</v>
       </c>
@@ -17805,7 +17818,7 @@
       <c r="F247" s="3"/>
       <c r="K247" s="3"/>
     </row>
-    <row r="248" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>738</v>
       </c>
@@ -17824,7 +17837,7 @@
       <c r="F248" s="3"/>
       <c r="K248" s="3"/>
     </row>
-    <row r="249" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>737</v>
       </c>
@@ -17843,7 +17856,7 @@
       <c r="F249" s="3"/>
       <c r="K249" s="3"/>
     </row>
-    <row r="250" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>743</v>
       </c>
@@ -17870,7 +17883,7 @@
       </c>
       <c r="K250" s="3"/>
     </row>
-    <row r="251" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>744</v>
       </c>
@@ -17897,7 +17910,7 @@
       </c>
       <c r="K251" s="3"/>
     </row>
-    <row r="252" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>745</v>
       </c>
@@ -17924,7 +17937,7 @@
       </c>
       <c r="K252" s="3"/>
     </row>
-    <row r="253" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>736</v>
       </c>
@@ -17943,7 +17956,7 @@
       <c r="F253" s="3"/>
       <c r="K253" s="3"/>
     </row>
-    <row r="254" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>735</v>
       </c>
@@ -17962,7 +17975,7 @@
       <c r="F254" s="3"/>
       <c r="K254" s="3"/>
     </row>
-    <row r="255" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>748</v>
       </c>
@@ -17992,7 +18005,7 @@
       </c>
       <c r="K255" s="3"/>
     </row>
-    <row r="256" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>749</v>
       </c>
@@ -18016,7 +18029,7 @@
       </c>
       <c r="K256" s="3"/>
     </row>
-    <row r="257" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>752</v>
       </c>
@@ -18037,7 +18050,7 @@
       </c>
       <c r="K257" s="3"/>
     </row>
-    <row r="258" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>766</v>
       </c>
@@ -18058,7 +18071,7 @@
       </c>
       <c r="K258" s="3"/>
     </row>
-    <row r="259" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>767</v>
       </c>
@@ -18079,7 +18092,7 @@
       </c>
       <c r="K259" s="3"/>
     </row>
-    <row r="260" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>768</v>
       </c>
@@ -18100,7 +18113,7 @@
       </c>
       <c r="K260" s="3"/>
     </row>
-    <row r="261" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>769</v>
       </c>
@@ -18121,7 +18134,7 @@
       </c>
       <c r="K261" s="3"/>
     </row>
-    <row r="262" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>770</v>
       </c>
@@ -18142,7 +18155,7 @@
       </c>
       <c r="K262" s="3"/>
     </row>
-    <row r="263" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>771</v>
       </c>
@@ -18163,7 +18176,7 @@
       </c>
       <c r="K263" s="3"/>
     </row>
-    <row r="264" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>782</v>
       </c>
@@ -18187,7 +18200,7 @@
       </c>
       <c r="K264" s="3"/>
     </row>
-    <row r="265" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>783</v>
       </c>
@@ -18208,7 +18221,7 @@
       </c>
       <c r="K265" s="3"/>
     </row>
-    <row r="266" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>801</v>
       </c>
@@ -18229,7 +18242,7 @@
       </c>
       <c r="K266" s="3"/>
     </row>
-    <row r="267" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>803</v>
       </c>
@@ -18247,7 +18260,7 @@
       </c>
       <c r="K267" s="3"/>
     </row>
-    <row r="268" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>805</v>
       </c>
@@ -18265,7 +18278,7 @@
       </c>
       <c r="K268" s="3"/>
     </row>
-    <row r="269" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>807</v>
       </c>
@@ -18283,7 +18296,7 @@
       </c>
       <c r="K269" s="3"/>
     </row>
-    <row r="270" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>809</v>
       </c>
@@ -18301,7 +18314,7 @@
       </c>
       <c r="K270" s="3"/>
     </row>
-    <row r="271" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>813</v>
       </c>
@@ -18319,7 +18332,7 @@
       </c>
       <c r="K271" s="3"/>
     </row>
-    <row r="272" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>814</v>
       </c>
@@ -18349,7 +18362,7 @@
       </c>
       <c r="K272" s="3"/>
     </row>
-    <row r="273" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>829</v>
       </c>
@@ -18376,7 +18389,7 @@
       </c>
       <c r="K273" s="3"/>
     </row>
-    <row r="274" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>815</v>
       </c>
@@ -18397,7 +18410,7 @@
       </c>
       <c r="K274" s="3"/>
     </row>
-    <row r="275" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>818</v>
       </c>
@@ -18418,7 +18431,7 @@
       </c>
       <c r="K275" s="3"/>
     </row>
-    <row r="276" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>821</v>
       </c>
@@ -18436,7 +18449,7 @@
       </c>
       <c r="K276" s="3"/>
     </row>
-    <row r="277" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>822</v>
       </c>
@@ -18454,7 +18467,7 @@
       </c>
       <c r="K277" s="3"/>
     </row>
-    <row r="278" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>824</v>
       </c>
@@ -18472,7 +18485,7 @@
       </c>
       <c r="K278" s="3"/>
     </row>
-    <row r="279" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>825</v>
       </c>
@@ -18493,7 +18506,7 @@
       </c>
       <c r="K279" s="3"/>
     </row>
-    <row r="280" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>827</v>
       </c>
@@ -18515,7 +18528,7 @@
       </c>
       <c r="K280" s="3"/>
     </row>
-    <row r="281" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>837</v>
       </c>
@@ -18536,7 +18549,7 @@
       </c>
       <c r="K281" s="3"/>
     </row>
-    <row r="282" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>839</v>
       </c>
@@ -18563,7 +18576,7 @@
       </c>
       <c r="K282" s="3"/>
     </row>
-    <row r="283" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A283" s="3" t="s">
         <v>844</v>
       </c>
@@ -18590,7 +18603,7 @@
       </c>
       <c r="K283" s="3"/>
     </row>
-    <row r="284" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>845</v>
       </c>
@@ -18614,7 +18627,7 @@
       </c>
       <c r="K284" s="3"/>
     </row>
-    <row r="285" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>852</v>
       </c>
@@ -18633,7 +18646,7 @@
       </c>
       <c r="K285" s="3"/>
     </row>
-    <row r="286" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A286" s="39" t="s">
         <v>854</v>
       </c>
@@ -18666,7 +18679,7 @@
       </c>
       <c r="K286" s="3"/>
     </row>
-    <row r="287" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A287" s="40" t="s">
         <v>855</v>
       </c>
@@ -18699,7 +18712,7 @@
       </c>
       <c r="K287" s="3"/>
     </row>
-    <row r="288" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A288" s="42" t="s">
         <v>856</v>
       </c>
@@ -18732,7 +18745,7 @@
       </c>
       <c r="K288" s="3"/>
     </row>
-    <row r="289" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A289" s="44" t="s">
         <v>857</v>
       </c>
@@ -18765,7 +18778,7 @@
       </c>
       <c r="K289" s="3"/>
     </row>
-    <row r="290" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>868</v>
       </c>
@@ -18792,7 +18805,7 @@
       </c>
       <c r="K290" s="3"/>
     </row>
-    <row r="291" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>869</v>
       </c>
@@ -18822,7 +18835,7 @@
       </c>
       <c r="K291" s="3"/>
     </row>
-    <row r="292" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>871</v>
       </c>
@@ -18849,7 +18862,7 @@
       </c>
       <c r="K292" s="3"/>
     </row>
-    <row r="293" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A293" s="44" t="s">
         <v>873</v>
       </c>
@@ -18882,7 +18895,7 @@
       </c>
       <c r="K293" s="3"/>
     </row>
-    <row r="294" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A294" s="40" t="s">
         <v>926</v>
       </c>
@@ -18912,7 +18925,7 @@
       </c>
       <c r="K294" s="3"/>
     </row>
-    <row r="295" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A295" s="39" t="s">
         <v>925</v>
       </c>
@@ -18942,7 +18955,7 @@
       </c>
       <c r="K295" s="3"/>
     </row>
-    <row r="296" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A296" s="42" t="s">
         <v>928</v>
       </c>
@@ -18972,7 +18985,7 @@
       </c>
       <c r="K296" s="3"/>
     </row>
-    <row r="297" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>877</v>
       </c>
@@ -19002,7 +19015,7 @@
       </c>
       <c r="K297" s="3"/>
     </row>
-    <row r="298" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>878</v>
       </c>
@@ -19032,7 +19045,7 @@
       </c>
       <c r="K298" s="3"/>
     </row>
-    <row r="299" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>881</v>
       </c>
@@ -19062,7 +19075,7 @@
       </c>
       <c r="K299" s="3"/>
     </row>
-    <row r="300" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>900</v>
       </c>
@@ -19097,7 +19110,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="301" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>903</v>
       </c>
@@ -19132,7 +19145,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="302" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>908</v>
       </c>
@@ -19162,7 +19175,7 @@
       </c>
       <c r="K302" s="3"/>
     </row>
-    <row r="303" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>910</v>
       </c>
@@ -19192,7 +19205,7 @@
       </c>
       <c r="K303" s="3"/>
     </row>
-    <row r="304" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>912</v>
       </c>
@@ -19219,7 +19232,7 @@
       </c>
       <c r="K304" s="3"/>
     </row>
-    <row r="305" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>914</v>
       </c>
@@ -19249,7 +19262,7 @@
       </c>
       <c r="K305" s="3"/>
     </row>
-    <row r="306" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>917</v>
       </c>
@@ -19279,7 +19292,7 @@
       </c>
       <c r="K306" s="3"/>
     </row>
-    <row r="307" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>918</v>
       </c>
@@ -19306,7 +19319,7 @@
       </c>
       <c r="K307" s="3"/>
     </row>
-    <row r="308" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>938</v>
       </c>
@@ -19336,7 +19349,7 @@
       </c>
       <c r="K308" s="3"/>
     </row>
-    <row r="309" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>944</v>
       </c>
@@ -19354,7 +19367,7 @@
       </c>
       <c r="K309" s="3"/>
     </row>
-    <row r="310" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>945</v>
       </c>
@@ -19384,7 +19397,7 @@
       </c>
       <c r="K310" s="3"/>
     </row>
-    <row r="311" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>951</v>
       </c>
@@ -19414,7 +19427,7 @@
       </c>
       <c r="K311" s="3"/>
     </row>
-    <row r="312" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>953</v>
       </c>
@@ -19444,12 +19457,12 @@
       </c>
       <c r="K312" s="3"/>
     </row>
-    <row r="313" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>956</v>
       </c>
       <c r="B313" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="C313" t="s">
         <v>264</v>
@@ -19467,13 +19480,13 @@
         <v>132</v>
       </c>
       <c r="I313" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="K313" s="3" t="s">
         <v>958</v>
       </c>
     </row>
-    <row r="314" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>959</v>
       </c>
@@ -19493,7 +19506,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="315" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>960</v>
       </c>
@@ -19525,7 +19538,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="316" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>961</v>
       </c>
@@ -19539,7 +19552,7 @@
         <v>132</v>
       </c>
       <c r="I316" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="J316" t="s">
         <v>964</v>
@@ -19560,7 +19573,7 @@
         <v>971</v>
       </c>
       <c r="E317" t="s">
-        <v>36</v>
+        <v>1029</v>
       </c>
       <c r="F317" s="3" t="s">
         <v>39</v>
@@ -19579,7 +19592,7 @@
       </c>
       <c r="K317" s="3"/>
     </row>
-    <row r="318" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>970</v>
       </c>
@@ -19601,7 +19614,7 @@
       </c>
       <c r="K318" s="3"/>
     </row>
-    <row r="319" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>979</v>
       </c>
@@ -19628,7 +19641,7 @@
       </c>
       <c r="K319" s="3"/>
     </row>
-    <row r="320" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>980</v>
       </c>
@@ -19655,7 +19668,7 @@
       </c>
       <c r="K320" s="3"/>
     </row>
-    <row r="321" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>995</v>
       </c>
@@ -19681,11 +19694,11 @@
         <v>132</v>
       </c>
       <c r="I321" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="K321" s="3"/>
     </row>
-    <row r="322" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>984</v>
       </c>
@@ -19724,7 +19737,7 @@
       <c r="U322" s="4"/>
       <c r="V322" s="5"/>
     </row>
-    <row r="323" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>988</v>
       </c>
@@ -19742,7 +19755,7 @@
       </c>
       <c r="K323" s="3"/>
     </row>
-    <row r="324" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>989</v>
       </c>
@@ -19757,7 +19770,7 @@
       </c>
       <c r="K324" s="3"/>
     </row>
-    <row r="325" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>991</v>
       </c>
@@ -19765,7 +19778,7 @@
         <v>972</v>
       </c>
       <c r="C325" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="D325" s="3" t="s">
         <v>976</v>
@@ -19787,7 +19800,7 @@
       </c>
       <c r="K325" s="3"/>
     </row>
-    <row r="326" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>983</v>
       </c>
@@ -19811,7 +19824,7 @@
       </c>
       <c r="K326" s="3"/>
     </row>
-    <row r="327" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>998</v>
       </c>
@@ -19831,16 +19844,19 @@
     </row>
     <row r="328" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
-        <v>1001</v>
-      </c>
-      <c r="B328" s="3" t="s">
         <v>1000</v>
+      </c>
+      <c r="B328" t="s">
+        <v>1028</v>
+      </c>
+      <c r="C328" t="s">
+        <v>192</v>
       </c>
       <c r="D328" s="3" t="s">
         <v>971</v>
       </c>
       <c r="E328" t="s">
-        <v>38</v>
+        <v>1030</v>
       </c>
       <c r="F328" s="3" t="s">
         <v>39</v>
@@ -19853,9 +19869,9 @@
       </c>
       <c r="K328" s="3"/>
     </row>
-    <row r="329" spans="1:22" s="39" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:22" s="39" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A329" s="39" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="B329" s="35" t="s">
         <v>971</v>
@@ -19864,7 +19880,7 @@
         <v>192</v>
       </c>
       <c r="D329" s="39" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="E329" s="39" t="s">
         <v>241</v>
@@ -19877,18 +19893,18 @@
       </c>
       <c r="K329" s="35"/>
     </row>
-    <row r="330" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="C330" t="s">
         <v>192</v>
       </c>
       <c r="D330" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E330" t="s">
         <v>241</v>
@@ -19901,12 +19917,12 @@
       </c>
       <c r="K330" s="50"/>
     </row>
-    <row r="331" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>994</v>
       </c>
       <c r="B331" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="C331" s="3" t="s">
         <v>992</v>
@@ -19915,10 +19931,10 @@
         <v>976</v>
       </c>
       <c r="E331" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="F331" s="50" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="G331" s="51" t="s">
         <v>34</v>
@@ -19927,28 +19943,28 @@
         <v>132</v>
       </c>
       <c r="I331" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="K331" s="50"/>
     </row>
-    <row r="332" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="C332" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="D332" s="3" t="s">
         <v>968</v>
       </c>
       <c r="E332" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="F332" s="50" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="G332" s="51" t="s">
         <v>84</v>
@@ -19957,13 +19973,13 @@
         <v>84</v>
       </c>
       <c r="I332" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="K332" s="50"/>
     </row>
     <row r="333" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="B333" s="3" t="s">
         <v>972</v>
@@ -19975,7 +19991,7 @@
         <v>971</v>
       </c>
       <c r="E333" t="s">
-        <v>1012</v>
+        <v>1031</v>
       </c>
       <c r="F333" s="50" t="s">
         <v>39</v>
@@ -19987,18 +20003,18 @@
         <v>132</v>
       </c>
       <c r="I333" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="J333" t="s">
         <v>964</v>
       </c>
       <c r="K333" s="50" t="s">
-        <v>1014</v>
-      </c>
-    </row>
-    <row r="334" spans="1:22" x14ac:dyDescent="0.2">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="334" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="B334" s="3" t="s">
         <v>317</v>
@@ -20007,7 +20023,7 @@
         <v>982</v>
       </c>
       <c r="D334" s="3" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="E334" t="s">
         <v>281</v>
@@ -20022,6 +20038,11 @@
         <v>695</v>
       </c>
       <c r="K334" s="50"/>
+    </row>
+    <row r="335" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F335" s="50"/>
+      <c r="G335" s="51"/>
+      <c r="K335" s="50"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>